<commit_message>
updating scenario functions to work with new data structure
</commit_message>
<xml_diff>
--- a/inst/extdata/country_summary_template.xlsx
+++ b/inst/extdata/country_summary_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ellio\Documents\WHO\rapporteuR\inst\extdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ellio\Documents\WHO\rapporteur\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E6FF9C1-C6B8-45D1-92B3-38FA0C901471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA3B38AB-C2E7-4E49-8F46-588DF842CA0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="26136" windowHeight="16896" tabRatio="942" activeTab="10" xr2:uid="{A0469F42-B2BF-41E9-9270-FEA8E2D23640}"/>
+    <workbookView xWindow="32280" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="942" xr2:uid="{A0469F42-B2BF-41E9-9270-FEA8E2D23640}"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="12" r:id="rId1"/>
@@ -29,14 +29,6 @@
     <sheet name="HPOP_Chart" sheetId="6" r:id="rId14"/>
     <sheet name="HPOP_Inter" sheetId="5" r:id="rId15"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId16"/>
-  </externalReferences>
-  <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="6">HEP_summary!$A$1:$C$31</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="11">HPOP_summary!$A$1:$D$28</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">UHC_summary!$A$1:$D$30</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -55,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1239" uniqueCount="471">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1250" uniqueCount="471">
   <si>
     <t>Magnitude +</t>
   </si>
@@ -3500,6 +3492,9 @@
     <xf numFmtId="0" fontId="11" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="12" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="42" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3644,9 +3639,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="12" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="3" builtinId="3"/>
@@ -4333,7 +4325,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A163F0F1-AB48-4117-91E7-A58DC04BF958}" type="CELLRANGE">
+                    <a:fld id="{695CA04D-A59B-4040-9FAA-9E514EDDEDBF}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4394,7 +4386,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A5EA9445-52FF-4555-8B04-DF3E8D84F7F2}" type="CELLRANGE">
+                    <a:fld id="{9703A0F3-8940-46D8-A47B-B21EE8736BA1}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4455,7 +4447,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{10117B8D-C6E7-4864-93CD-773DC0FDC8B2}" type="CELLRANGE">
+                    <a:fld id="{F2DFD7B7-EC14-48E4-BC9B-9411B31CD9F0}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4489,7 +4481,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{20D75D12-FF9B-44D8-B22C-E423AFAA25AB}" type="CELLRANGE">
+                    <a:fld id="{153F5C4A-48A0-46F2-B84F-58F7B29BB803}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4508,7 +4500,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -4550,7 +4541,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2154E94F-065A-4C46-8F55-0F944BA89D51}" type="CELLRANGE">
+                    <a:fld id="{6BF412FE-E13E-4DE7-A059-FB8FE07603D7}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4584,7 +4575,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D1D2E703-C162-4AEB-9C6F-17281CC7966C}" type="CELLRANGE">
+                    <a:fld id="{656BC4CD-494B-497B-AFC8-612AC607BB4E}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4618,7 +4609,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{02BBFAE2-8BDD-4662-B28D-1ED011BFF498}" type="CELLRANGE">
+                    <a:fld id="{B175A792-335C-4032-BC96-25B9F31AE2DB}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4652,7 +4643,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{52E92A29-C288-4533-BB94-A2DB691CEDD3}" type="CELLRANGE">
+                    <a:fld id="{94DF599B-7C8B-4D50-9221-1873FD11807A}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4686,7 +4677,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DC08C465-582D-41DD-B81A-89167ECC39BD}" type="CELLRANGE">
+                    <a:fld id="{B567D36E-9AA4-4C16-A829-FC5A7AB849E7}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4720,7 +4711,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4E870895-0FB8-41B5-B991-915C263EDE09}" type="CELLRANGE">
+                    <a:fld id="{5DEBA03B-A675-4057-A27C-782FA7D7451F}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4754,7 +4745,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D500A0AB-ED4C-40BC-B3FC-2F03F53A2F5F}" type="CELLRANGE">
+                    <a:fld id="{1BE7FB43-7A7F-41DB-BBD2-5EEE3950C192}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4773,7 +4764,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -6516,7 +6506,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{76F15903-526B-46E7-A2BF-95D56BAC3A24}" type="CELLRANGE">
+                    <a:fld id="{66DAD0D0-10FF-49B6-A11F-A8CA0295FBAF}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6577,7 +6567,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{50317BF9-A812-44E6-B919-D87897FAAA6D}" type="CELLRANGE">
+                    <a:fld id="{D71076F6-FA24-4BBC-80BC-19BF96002FF4}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6638,7 +6628,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9E0E7F46-B202-433D-ADB5-08CEBED893B1}" type="CELLRANGE">
+                    <a:fld id="{A14A0C96-7EF3-4010-8950-DF578CFCBB21}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6672,7 +6662,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{22E61868-B728-4CCA-A067-B1E60ED18759}" type="CELLRANGE">
+                    <a:fld id="{FD49D6B9-8F7C-43D9-91D6-1FDD02414C92}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6733,7 +6723,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{422D1941-E4B3-4E27-9D7B-767F586CECC3}" type="CELLRANGE">
+                    <a:fld id="{55DA4FB0-4080-440C-82C7-38EBB8101E1E}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6767,7 +6757,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9C6C78A3-DD5D-4A1D-B604-A057F2EF701D}" type="CELLRANGE">
+                    <a:fld id="{B1E3E3C1-EE8A-41B7-8B1A-4E662CBB1E20}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6801,7 +6791,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{66674A9F-F1B3-4CED-BB9E-48DEFB60A1E1}" type="CELLRANGE">
+                    <a:fld id="{70202BED-F21D-48A7-8DF6-EA90B09CB18C}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6835,7 +6825,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{05100990-BB64-49EA-BFD2-2B351447DF56}" type="CELLRANGE">
+                    <a:fld id="{ECC75A69-40A2-42AF-9BEC-8C5EF6390BE8}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6869,7 +6859,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AD6BB55D-EFBA-469C-A9E2-84C5D92F5C6E}" type="CELLRANGE">
+                    <a:fld id="{8815E306-05A7-4923-AEAB-FF0B3CDDDA94}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6903,7 +6893,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FCC1312A-C070-4CB8-B51C-BE29EE1B9A67}" type="CELLRANGE">
+                    <a:fld id="{210446CD-9B68-4839-88F8-286C62CEE355}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6937,7 +6927,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8114CA48-C457-452F-B175-C49DC8634550}" type="CELLRANGE">
+                    <a:fld id="{B635EA97-B718-4BFE-B012-14BDD02811EF}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6971,7 +6961,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EC5F8702-A553-435E-84BF-875861564212}" type="CELLRANGE">
+                    <a:fld id="{E6858B06-F945-4BEB-BDBB-4963833554BE}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7005,7 +6995,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F984FD68-9EA1-41CB-A308-51D403B85F45}" type="CELLRANGE">
+                    <a:fld id="{F71BD4EE-688B-4834-A335-28C9C79F2C8D}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7589,1011 +7579,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Intro"/>
-      <sheetName val="Indicator List"/>
-      <sheetName val="UHC_summary"/>
-      <sheetName val="UHC_Time Series"/>
-      <sheetName val="UHC_Chart"/>
-      <sheetName val="UHC_Inter"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2">
-        <row r="1">
-          <cell r="B1"/>
-          <cell r="C1"/>
-          <cell r="D1"/>
-          <cell r="E1"/>
-          <cell r="I1"/>
-          <cell r="J1"/>
-          <cell r="L1"/>
-          <cell r="M1"/>
-        </row>
-        <row r="2">
-          <cell r="B2"/>
-          <cell r="C2"/>
-          <cell r="D2"/>
-          <cell r="E2"/>
-          <cell r="I2"/>
-          <cell r="J2"/>
-          <cell r="L2"/>
-          <cell r="M2"/>
-        </row>
-        <row r="3">
-          <cell r="B3"/>
-          <cell r="C3"/>
-          <cell r="D3"/>
-          <cell r="E3"/>
-          <cell r="I3"/>
-          <cell r="J3"/>
-          <cell r="L3"/>
-          <cell r="M3"/>
-        </row>
-        <row r="4">
-          <cell r="B4"/>
-          <cell r="C4"/>
-          <cell r="D4"/>
-          <cell r="E4"/>
-          <cell r="I4"/>
-          <cell r="J4"/>
-          <cell r="L4"/>
-          <cell r="M4"/>
-        </row>
-        <row r="5">
-          <cell r="B5"/>
-          <cell r="C5"/>
-          <cell r="D5"/>
-          <cell r="E5"/>
-          <cell r="I5"/>
-          <cell r="J5"/>
-          <cell r="L5"/>
-          <cell r="M5"/>
-        </row>
-        <row r="6">
-          <cell r="B6"/>
-          <cell r="C6"/>
-          <cell r="D6"/>
-          <cell r="E6"/>
-          <cell r="I6"/>
-          <cell r="J6"/>
-          <cell r="L6"/>
-          <cell r="M6"/>
-        </row>
-        <row r="7">
-          <cell r="B7"/>
-          <cell r="C7"/>
-          <cell r="D7"/>
-          <cell r="E7"/>
-          <cell r="I7"/>
-          <cell r="J7"/>
-          <cell r="L7"/>
-          <cell r="M7"/>
-        </row>
-        <row r="8">
-          <cell r="B8"/>
-          <cell r="C8"/>
-          <cell r="D8"/>
-          <cell r="E8"/>
-          <cell r="I8"/>
-          <cell r="J8"/>
-          <cell r="L8"/>
-          <cell r="M8"/>
-        </row>
-        <row r="9">
-          <cell r="B9"/>
-          <cell r="C9" t="str">
-            <v>Latest Reported/Estimated Data Available</v>
-          </cell>
-          <cell r="D9"/>
-          <cell r="E9"/>
-          <cell r="I9" t="str">
-            <v>2018 Baseline, and 2023 Projection</v>
-          </cell>
-          <cell r="J9"/>
-          <cell r="L9"/>
-          <cell r="M9"/>
-        </row>
-        <row r="10">
-          <cell r="B10"/>
-          <cell r="C10" t="str">
-            <v>Raw Value</v>
-          </cell>
-          <cell r="D10" t="str">
-            <v>Transformed Value</v>
-          </cell>
-          <cell r="E10" t="str">
-            <v>Year</v>
-          </cell>
-          <cell r="I10" t="str">
-            <v>Raw Value</v>
-          </cell>
-          <cell r="J10" t="str">
-            <v/>
-          </cell>
-          <cell r="L10" t="str">
-            <v>Transformed Value</v>
-          </cell>
-          <cell r="M10" t="str">
-            <v/>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="B11" t="str">
-            <v>Tracer Indicator</v>
-          </cell>
-          <cell r="C11"/>
-          <cell r="D11"/>
-          <cell r="E11"/>
-          <cell r="I11" t="str">
-            <v>2018</v>
-          </cell>
-          <cell r="J11" t="str">
-            <v>2023</v>
-          </cell>
-          <cell r="L11" t="str">
-            <v>2018</v>
-          </cell>
-          <cell r="M11" t="str">
-            <v>2023</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="B12"/>
-          <cell r="C12"/>
-          <cell r="D12"/>
-          <cell r="E12"/>
-          <cell r="I12"/>
-          <cell r="J12"/>
-          <cell r="L12"/>
-          <cell r="M12"/>
-        </row>
-        <row r="13">
-          <cell r="B13" t="str">
-            <v>Demand satisfied with modern methods (married women or in-union) 1</v>
-          </cell>
-          <cell r="C13">
-            <v>57.99</v>
-          </cell>
-          <cell r="D13" t="str">
-            <v/>
-          </cell>
-          <cell r="E13">
-            <v>2020</v>
-          </cell>
-          <cell r="I13">
-            <v>56.35</v>
-          </cell>
-          <cell r="J13">
-            <v>60.55</v>
-          </cell>
-          <cell r="L13"/>
-          <cell r="M13"/>
-        </row>
-        <row r="14">
-          <cell r="B14" t="str">
-            <v>Antenatal care coverage (+4 visits) 2</v>
-          </cell>
-          <cell r="C14"/>
-          <cell r="D14" t="str">
-            <v/>
-          </cell>
-          <cell r="E14"/>
-          <cell r="I14">
-            <v>98.58</v>
-          </cell>
-          <cell r="J14">
-            <v>98.46</v>
-          </cell>
-          <cell r="L14"/>
-          <cell r="M14"/>
-        </row>
-        <row r="15">
-          <cell r="B15" t="str">
-            <v>DPT3 Immunization coverage</v>
-          </cell>
-          <cell r="C15">
-            <v>98</v>
-          </cell>
-          <cell r="D15" t="str">
-            <v/>
-          </cell>
-          <cell r="E15">
-            <v>2019</v>
-          </cell>
-          <cell r="I15">
-            <v>98</v>
-          </cell>
-          <cell r="J15">
-            <v>98.54</v>
-          </cell>
-          <cell r="L15"/>
-          <cell r="M15"/>
-        </row>
-        <row r="16">
-          <cell r="B16" t="str">
-            <v>Care seeking for suspected pneumonia</v>
-          </cell>
-          <cell r="C16"/>
-          <cell r="D16" t="str">
-            <v/>
-          </cell>
-          <cell r="E16"/>
-          <cell r="I16">
-            <v>89.91</v>
-          </cell>
-          <cell r="J16">
-            <v>90.82</v>
-          </cell>
-          <cell r="L16"/>
-          <cell r="M16"/>
-        </row>
-        <row r="17">
-          <cell r="B17" t="str">
-            <v>Average RMNCH</v>
-          </cell>
-          <cell r="C17"/>
-          <cell r="D17"/>
-          <cell r="E17"/>
-          <cell r="I17"/>
-          <cell r="J17"/>
-          <cell r="L17"/>
-          <cell r="M17"/>
-        </row>
-        <row r="18">
-          <cell r="B18"/>
-          <cell r="C18"/>
-          <cell r="D18"/>
-          <cell r="E18"/>
-          <cell r="I18"/>
-          <cell r="J18"/>
-          <cell r="L18"/>
-          <cell r="M18"/>
-        </row>
-        <row r="19">
-          <cell r="B19" t="str">
-            <v>TB treatment coverage</v>
-          </cell>
-          <cell r="C19">
-            <v>86.96</v>
-          </cell>
-          <cell r="D19" t="str">
-            <v/>
-          </cell>
-          <cell r="E19">
-            <v>2019</v>
-          </cell>
-          <cell r="I19">
-            <v>86.96</v>
-          </cell>
-          <cell r="J19">
-            <v>86.96</v>
-          </cell>
-          <cell r="L19"/>
-          <cell r="M19"/>
-        </row>
-        <row r="20">
-          <cell r="B20" t="str">
-            <v>HIV ART coverage</v>
-          </cell>
-          <cell r="C20">
-            <v>84.01</v>
-          </cell>
-          <cell r="D20" t="str">
-            <v/>
-          </cell>
-          <cell r="E20">
-            <v>2019</v>
-          </cell>
-          <cell r="I20">
-            <v>83.01</v>
-          </cell>
-          <cell r="J20">
-            <v>90.99</v>
-          </cell>
-          <cell r="L20"/>
-          <cell r="M20"/>
-        </row>
-        <row r="21">
-          <cell r="B21" t="str">
-            <v>ITN use 4</v>
-          </cell>
-          <cell r="C21"/>
-          <cell r="D21" t="str">
-            <v/>
-          </cell>
-          <cell r="E21"/>
-          <cell r="I21"/>
-          <cell r="J21"/>
-          <cell r="L21"/>
-          <cell r="M21"/>
-        </row>
-        <row r="22">
-          <cell r="B22" t="str">
-            <v>Use of basic sanitation</v>
-          </cell>
-          <cell r="C22">
-            <v>99.89</v>
-          </cell>
-          <cell r="D22" t="str">
-            <v/>
-          </cell>
-          <cell r="E22">
-            <v>2017</v>
-          </cell>
-          <cell r="I22">
-            <v>99.9</v>
-          </cell>
-          <cell r="J22">
-            <v>99.9</v>
-          </cell>
-          <cell r="L22"/>
-          <cell r="M22"/>
-        </row>
-        <row r="23">
-          <cell r="B23" t="str">
-            <v>Average Infectious diseases</v>
-          </cell>
-          <cell r="C23"/>
-          <cell r="D23"/>
-          <cell r="E23"/>
-          <cell r="I23"/>
-          <cell r="J23"/>
-          <cell r="L23"/>
-          <cell r="M23"/>
-        </row>
-        <row r="24">
-          <cell r="B24"/>
-          <cell r="C24"/>
-          <cell r="D24"/>
-          <cell r="E24"/>
-          <cell r="I24"/>
-          <cell r="J24"/>
-          <cell r="L24"/>
-          <cell r="M24"/>
-        </row>
-        <row r="25">
-          <cell r="B25" t="str">
-            <v>Prevalence of raised blood pressure*</v>
-          </cell>
-          <cell r="C25">
-            <v>17.55</v>
-          </cell>
-          <cell r="D25"/>
-          <cell r="E25">
-            <v>2015</v>
-          </cell>
-          <cell r="I25">
-            <v>16.68</v>
-          </cell>
-          <cell r="J25">
-            <v>15.29</v>
-          </cell>
-          <cell r="L25"/>
-          <cell r="M25"/>
-        </row>
-        <row r="26">
-          <cell r="B26" t="str">
-            <v>Mean fasting blood glucose (mmol/l)*</v>
-          </cell>
-          <cell r="C26">
-            <v>5.2</v>
-          </cell>
-          <cell r="D26"/>
-          <cell r="E26">
-            <v>2014</v>
-          </cell>
-          <cell r="I26">
-            <v>5.12</v>
-          </cell>
-          <cell r="J26">
-            <v>5.03</v>
-          </cell>
-          <cell r="L26"/>
-          <cell r="M26"/>
-        </row>
-        <row r="27">
-          <cell r="B27" t="str">
-            <v>Tobacco use prevalence* 3</v>
-          </cell>
-          <cell r="C27">
-            <v>21.9</v>
-          </cell>
-          <cell r="D27"/>
-          <cell r="E27">
-            <v>2018</v>
-          </cell>
-          <cell r="I27">
-            <v>21.9</v>
-          </cell>
-          <cell r="J27">
-            <v>19.5</v>
-          </cell>
-          <cell r="L27"/>
-          <cell r="M27"/>
-        </row>
-        <row r="28">
-          <cell r="B28" t="str">
-            <v>Average NCDs</v>
-          </cell>
-          <cell r="C28"/>
-          <cell r="D28"/>
-          <cell r="E28"/>
-          <cell r="I28"/>
-          <cell r="J28"/>
-          <cell r="L28"/>
-          <cell r="M28"/>
-        </row>
-        <row r="29">
-          <cell r="B29"/>
-          <cell r="C29"/>
-          <cell r="D29"/>
-          <cell r="E29"/>
-          <cell r="I29"/>
-          <cell r="J29"/>
-          <cell r="L29"/>
-          <cell r="M29"/>
-        </row>
-        <row r="30">
-          <cell r="B30" t="str">
-            <v>Hospital beds density*</v>
-          </cell>
-          <cell r="C30">
-            <v>129.04</v>
-          </cell>
-          <cell r="D30"/>
-          <cell r="E30">
-            <v>2018</v>
-          </cell>
-          <cell r="I30">
-            <v>129.04</v>
-          </cell>
-          <cell r="J30">
-            <v>130.5</v>
-          </cell>
-          <cell r="L30"/>
-          <cell r="M30"/>
-        </row>
-        <row r="31">
-          <cell r="B31" t="str">
-            <v>Health worker density*</v>
-          </cell>
-          <cell r="C31">
-            <v>151.77000000000001</v>
-          </cell>
-          <cell r="D31"/>
-          <cell r="E31">
-            <v>2018</v>
-          </cell>
-          <cell r="I31">
-            <v>151.77000000000001</v>
-          </cell>
-          <cell r="J31">
-            <v>172.69</v>
-          </cell>
-          <cell r="L31"/>
-          <cell r="M31"/>
-        </row>
-        <row r="32">
-          <cell r="B32" t="str">
-            <v>Density of doctors</v>
-          </cell>
-          <cell r="C32">
-            <v>24.8</v>
-          </cell>
-          <cell r="D32"/>
-          <cell r="E32">
-            <v>2018</v>
-          </cell>
-          <cell r="I32">
-            <v>24.8</v>
-          </cell>
-          <cell r="J32">
-            <v>27.38</v>
-          </cell>
-          <cell r="L32"/>
-          <cell r="M32"/>
-        </row>
-        <row r="33">
-          <cell r="B33" t="str">
-            <v>Density of nurses/midwives</v>
-          </cell>
-          <cell r="C33">
-            <v>126.98</v>
-          </cell>
-          <cell r="D33"/>
-          <cell r="E33">
-            <v>2018</v>
-          </cell>
-          <cell r="I33">
-            <v>126.98</v>
-          </cell>
-          <cell r="J33">
-            <v>145.31</v>
-          </cell>
-          <cell r="L33"/>
-          <cell r="M33"/>
-        </row>
-        <row r="34">
-          <cell r="B34" t="str">
-            <v>IHR core capacity index*</v>
-          </cell>
-          <cell r="C34">
-            <v>95</v>
-          </cell>
-          <cell r="D34"/>
-          <cell r="E34">
-            <v>2020</v>
-          </cell>
-          <cell r="I34">
-            <v>95</v>
-          </cell>
-          <cell r="J34">
-            <v>94.99</v>
-          </cell>
-          <cell r="L34"/>
-          <cell r="M34"/>
-        </row>
-        <row r="35">
-          <cell r="B35" t="str">
-            <v>Average Service capacity and access</v>
-          </cell>
-          <cell r="C35"/>
-          <cell r="D35"/>
-          <cell r="E35"/>
-          <cell r="I35"/>
-          <cell r="J35"/>
-          <cell r="L35"/>
-          <cell r="M35"/>
-        </row>
-        <row r="36">
-          <cell r="B36"/>
-          <cell r="C36"/>
-          <cell r="D36"/>
-          <cell r="E36"/>
-          <cell r="I36"/>
-          <cell r="J36"/>
-          <cell r="L36"/>
-          <cell r="M36"/>
-        </row>
-        <row r="37">
-          <cell r="B37" t="str">
-            <v>SDG 3.8.2 Proportion of population with household expenditures on health &gt;10% of total household expenditure or income **</v>
-          </cell>
-          <cell r="C37">
-            <v>4.3600000000000003</v>
-          </cell>
-          <cell r="D37" t="str">
-            <v/>
-          </cell>
-          <cell r="E37">
-            <v>2015</v>
-          </cell>
-          <cell r="I37">
-            <v>4.2300000000000004</v>
-          </cell>
-          <cell r="J37">
-            <v>4.0599999999999996</v>
-          </cell>
-          <cell r="L37"/>
-          <cell r="M37"/>
-        </row>
-        <row r="38">
-          <cell r="B38" t="str">
-            <v>UHC single measure</v>
-          </cell>
-          <cell r="C38"/>
-          <cell r="D38"/>
-          <cell r="E38"/>
-          <cell r="I38"/>
-          <cell r="J38"/>
-          <cell r="L38">
-            <v>61.09664039777099</v>
-          </cell>
-          <cell r="M38">
-            <v>63.310803650646406</v>
-          </cell>
-        </row>
-        <row r="39">
-          <cell r="B39" t="str">
-            <v>Change in UHC single measure over 2018-2023</v>
-          </cell>
-          <cell r="C39"/>
-          <cell r="D39"/>
-          <cell r="E39"/>
-          <cell r="I39"/>
-          <cell r="J39"/>
-          <cell r="L39"/>
-          <cell r="M39"/>
-        </row>
-        <row r="40">
-          <cell r="B40" t="str">
-            <v>UN Population 2023 (thousand)</v>
-          </cell>
-          <cell r="C40"/>
-          <cell r="D40"/>
-          <cell r="E40"/>
-          <cell r="I40"/>
-          <cell r="J40"/>
-          <cell r="L40"/>
-          <cell r="M40"/>
-        </row>
-        <row r="41">
-          <cell r="B41" t="str">
-            <v>Country contribution to UHC billion target (population - thousand)</v>
-          </cell>
-          <cell r="C41"/>
-          <cell r="D41"/>
-          <cell r="E41"/>
-          <cell r="I41"/>
-          <cell r="J41"/>
-          <cell r="L41"/>
-          <cell r="M41"/>
-        </row>
-        <row r="42">
-          <cell r="B42" t="str">
-            <v>% of country population newly covered by universal healthcare</v>
-          </cell>
-          <cell r="C42"/>
-          <cell r="D42"/>
-          <cell r="E42"/>
-          <cell r="I42"/>
-          <cell r="J42"/>
-          <cell r="L42"/>
-          <cell r="M42"/>
-        </row>
-        <row r="43">
-          <cell r="B43"/>
-          <cell r="C43"/>
-          <cell r="D43"/>
-          <cell r="E43"/>
-          <cell r="I43"/>
-          <cell r="J43"/>
-          <cell r="L43"/>
-          <cell r="M43"/>
-        </row>
-        <row r="44">
-          <cell r="B44"/>
-          <cell r="C44"/>
-          <cell r="D44"/>
-          <cell r="E44"/>
-          <cell r="I44"/>
-          <cell r="J44"/>
-          <cell r="L44"/>
-          <cell r="M44"/>
-        </row>
-        <row r="45">
-          <cell r="B45"/>
-          <cell r="C45"/>
-          <cell r="D45"/>
-          <cell r="E45"/>
-          <cell r="I45"/>
-          <cell r="J45"/>
-          <cell r="L45"/>
-          <cell r="M45"/>
-        </row>
-        <row r="46">
-          <cell r="B46"/>
-          <cell r="C46"/>
-          <cell r="D46"/>
-          <cell r="E46"/>
-          <cell r="I46"/>
-          <cell r="J46"/>
-          <cell r="L46"/>
-          <cell r="M46"/>
-        </row>
-        <row r="47">
-          <cell r="B47"/>
-          <cell r="C47"/>
-          <cell r="D47"/>
-          <cell r="E47"/>
-          <cell r="I47"/>
-          <cell r="J47"/>
-          <cell r="L47"/>
-          <cell r="M47"/>
-        </row>
-        <row r="48">
-          <cell r="B48"/>
-          <cell r="C48"/>
-          <cell r="D48"/>
-          <cell r="E48"/>
-          <cell r="I48"/>
-          <cell r="J48"/>
-          <cell r="L48"/>
-          <cell r="M48"/>
-        </row>
-        <row r="49">
-          <cell r="B49"/>
-          <cell r="C49"/>
-          <cell r="D49"/>
-          <cell r="E49"/>
-          <cell r="I49"/>
-          <cell r="J49"/>
-          <cell r="L49"/>
-          <cell r="M49"/>
-        </row>
-        <row r="50">
-          <cell r="B50"/>
-          <cell r="C50"/>
-          <cell r="D50"/>
-          <cell r="E50"/>
-          <cell r="I50"/>
-          <cell r="J50"/>
-          <cell r="L50"/>
-          <cell r="M50"/>
-        </row>
-        <row r="51">
-          <cell r="B51"/>
-          <cell r="C51"/>
-          <cell r="D51"/>
-          <cell r="E51"/>
-          <cell r="I51"/>
-          <cell r="J51"/>
-          <cell r="L51"/>
-          <cell r="M51"/>
-        </row>
-        <row r="52">
-          <cell r="B52"/>
-          <cell r="C52"/>
-          <cell r="D52"/>
-          <cell r="E52"/>
-          <cell r="I52"/>
-          <cell r="J52"/>
-          <cell r="L52"/>
-          <cell r="M52"/>
-        </row>
-        <row r="53">
-          <cell r="B53"/>
-          <cell r="C53"/>
-          <cell r="D53"/>
-          <cell r="E53"/>
-          <cell r="I53"/>
-          <cell r="J53"/>
-          <cell r="L53"/>
-          <cell r="M53"/>
-        </row>
-        <row r="54">
-          <cell r="B54"/>
-          <cell r="C54"/>
-          <cell r="D54"/>
-          <cell r="E54"/>
-          <cell r="I54"/>
-          <cell r="J54"/>
-          <cell r="L54"/>
-          <cell r="M54"/>
-        </row>
-        <row r="55">
-          <cell r="B55"/>
-          <cell r="C55"/>
-          <cell r="D55"/>
-          <cell r="E55"/>
-          <cell r="I55"/>
-          <cell r="J55"/>
-          <cell r="L55"/>
-          <cell r="M55"/>
-        </row>
-        <row r="56">
-          <cell r="B56"/>
-          <cell r="C56"/>
-          <cell r="D56"/>
-          <cell r="E56"/>
-          <cell r="I56"/>
-          <cell r="J56"/>
-          <cell r="L56"/>
-          <cell r="M56"/>
-        </row>
-        <row r="57">
-          <cell r="B57"/>
-          <cell r="C57"/>
-          <cell r="D57"/>
-          <cell r="E57"/>
-          <cell r="I57"/>
-          <cell r="J57"/>
-          <cell r="L57"/>
-          <cell r="M57"/>
-        </row>
-        <row r="58">
-          <cell r="B58"/>
-          <cell r="C58"/>
-          <cell r="D58"/>
-          <cell r="E58"/>
-          <cell r="I58"/>
-          <cell r="J58"/>
-          <cell r="L58"/>
-          <cell r="M58"/>
-        </row>
-        <row r="59">
-          <cell r="B59"/>
-          <cell r="C59"/>
-          <cell r="D59"/>
-          <cell r="E59"/>
-          <cell r="I59"/>
-          <cell r="J59"/>
-          <cell r="L59"/>
-          <cell r="M59"/>
-        </row>
-        <row r="60">
-          <cell r="B60"/>
-          <cell r="C60"/>
-          <cell r="D60"/>
-          <cell r="E60"/>
-          <cell r="I60"/>
-          <cell r="J60"/>
-          <cell r="L60"/>
-          <cell r="M60"/>
-        </row>
-        <row r="61">
-          <cell r="B61"/>
-          <cell r="C61"/>
-          <cell r="D61"/>
-          <cell r="E61"/>
-          <cell r="I61"/>
-          <cell r="J61"/>
-          <cell r="L61"/>
-          <cell r="M61"/>
-        </row>
-        <row r="62">
-          <cell r="B62"/>
-          <cell r="C62"/>
-          <cell r="D62"/>
-          <cell r="E62"/>
-          <cell r="I62"/>
-          <cell r="J62"/>
-          <cell r="L62"/>
-          <cell r="M62"/>
-        </row>
-        <row r="63">
-          <cell r="B63"/>
-          <cell r="C63"/>
-          <cell r="D63"/>
-          <cell r="E63"/>
-          <cell r="I63"/>
-          <cell r="J63"/>
-          <cell r="L63"/>
-          <cell r="M63"/>
-        </row>
-        <row r="64">
-          <cell r="B64"/>
-          <cell r="C64"/>
-          <cell r="D64"/>
-          <cell r="E64"/>
-          <cell r="I64"/>
-          <cell r="J64"/>
-          <cell r="L64"/>
-          <cell r="M64"/>
-        </row>
-        <row r="65">
-          <cell r="B65"/>
-          <cell r="C65"/>
-          <cell r="D65"/>
-          <cell r="E65"/>
-          <cell r="I65"/>
-          <cell r="J65"/>
-          <cell r="L65"/>
-          <cell r="M65"/>
-        </row>
-        <row r="66">
-          <cell r="B66"/>
-          <cell r="C66"/>
-          <cell r="D66"/>
-          <cell r="E66"/>
-          <cell r="I66"/>
-          <cell r="J66"/>
-          <cell r="L66"/>
-          <cell r="M66"/>
-        </row>
-        <row r="67">
-          <cell r="B67"/>
-          <cell r="C67"/>
-          <cell r="D67"/>
-          <cell r="E67"/>
-          <cell r="I67"/>
-          <cell r="J67"/>
-          <cell r="L67"/>
-          <cell r="M67"/>
-        </row>
-        <row r="68">
-          <cell r="B68"/>
-          <cell r="C68"/>
-          <cell r="D68"/>
-          <cell r="E68"/>
-          <cell r="I68"/>
-          <cell r="J68"/>
-          <cell r="L68"/>
-          <cell r="M68"/>
-        </row>
-        <row r="69">
-          <cell r="B69"/>
-          <cell r="C69"/>
-          <cell r="D69"/>
-          <cell r="E69"/>
-          <cell r="I69"/>
-          <cell r="J69"/>
-          <cell r="L69"/>
-          <cell r="M69"/>
-        </row>
-      </sheetData>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5">
-        <row r="3">
-          <cell r="A3" t="str">
-            <v>Demand satisfied with modern methods (married women or in-union) 1</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="A4" t="str">
-            <v>Antenatal care coverage (+4 visits) 2</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="A5" t="str">
-            <v>DPT3 Immunization coverage</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="A6" t="str">
-            <v>Care seeking for suspected pneumonia</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="A7" t="str">
-            <v>TB treatment coverage</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="A8" t="str">
-            <v>HIV ART coverage 4</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="A9" t="str">
-            <v>Use of basic sanitation</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="A10" t="str">
-            <v>Prevalence of raised blood pressure*</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="A11" t="str">
-            <v>Mean fasting blood glucose (mmol/l)*</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="A12" t="str">
-            <v>Tobacco use prevalence* 3</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="A13" t="str">
-            <v>Hospital beds density*</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="A14" t="str">
-            <v>Health worker density*</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="A15" t="str">
-            <v>IHR core capacity index*</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="A16"/>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -8896,678 +7881,678 @@
   </sheetPr>
   <dimension ref="B1:O47"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34:M34"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31:M31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="1.77734375" style="13" customWidth="1"/>
-    <col min="2" max="12" width="9.21875" style="13"/>
-    <col min="13" max="13" width="25.109375" style="13" customWidth="1"/>
-    <col min="14" max="16384" width="9.21875" style="13"/>
+    <col min="1" max="1" width="1.81640625" style="13" customWidth="1"/>
+    <col min="2" max="12" width="9.1796875" style="13"/>
+    <col min="13" max="13" width="25.08984375" style="13" customWidth="1"/>
+    <col min="14" max="16384" width="9.1796875" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:15" ht="10.5" customHeight="1"/>
     <row r="2" spans="2:15" ht="36" customHeight="1">
-      <c r="B2" s="323" t="s">
+      <c r="B2" s="324" t="s">
         <v>337</v>
       </c>
-      <c r="C2" s="323"/>
-      <c r="D2" s="323"/>
-      <c r="E2" s="323"/>
-      <c r="F2" s="323"/>
-      <c r="G2" s="323"/>
-      <c r="H2" s="323"/>
-      <c r="I2" s="323"/>
-      <c r="J2" s="323"/>
-      <c r="K2" s="323"/>
-      <c r="L2" s="323"/>
-      <c r="M2" s="323"/>
+      <c r="C2" s="324"/>
+      <c r="D2" s="324"/>
+      <c r="E2" s="324"/>
+      <c r="F2" s="324"/>
+      <c r="G2" s="324"/>
+      <c r="H2" s="324"/>
+      <c r="I2" s="324"/>
+      <c r="J2" s="324"/>
+      <c r="K2" s="324"/>
+      <c r="L2" s="324"/>
+      <c r="M2" s="324"/>
       <c r="N2" s="61"/>
       <c r="O2" s="61"/>
     </row>
     <row r="3" spans="2:15" ht="15" customHeight="1">
-      <c r="B3" s="324" t="s">
+      <c r="B3" s="325" t="s">
         <v>435</v>
       </c>
-      <c r="C3" s="324"/>
-      <c r="D3" s="324"/>
-      <c r="E3" s="324"/>
-      <c r="F3" s="324"/>
-      <c r="G3" s="324"/>
-      <c r="H3" s="324"/>
-      <c r="I3" s="324"/>
-      <c r="J3" s="324"/>
-      <c r="K3" s="324"/>
-      <c r="L3" s="324"/>
-      <c r="M3" s="324"/>
+      <c r="C3" s="325"/>
+      <c r="D3" s="325"/>
+      <c r="E3" s="325"/>
+      <c r="F3" s="325"/>
+      <c r="G3" s="325"/>
+      <c r="H3" s="325"/>
+      <c r="I3" s="325"/>
+      <c r="J3" s="325"/>
+      <c r="K3" s="325"/>
+      <c r="L3" s="325"/>
+      <c r="M3" s="325"/>
       <c r="N3" s="200"/>
       <c r="O3" s="200"/>
     </row>
     <row r="4" spans="2:15" ht="18.75" customHeight="1">
-      <c r="B4" s="320" t="s">
+      <c r="B4" s="321" t="s">
         <v>338</v>
       </c>
-      <c r="C4" s="320"/>
-      <c r="D4" s="320"/>
-      <c r="E4" s="320"/>
-      <c r="F4" s="320"/>
-      <c r="G4" s="320"/>
-      <c r="H4" s="320"/>
-      <c r="I4" s="320"/>
-      <c r="J4" s="320"/>
-      <c r="K4" s="320"/>
-      <c r="L4" s="320"/>
-      <c r="M4" s="320"/>
+      <c r="C4" s="321"/>
+      <c r="D4" s="321"/>
+      <c r="E4" s="321"/>
+      <c r="F4" s="321"/>
+      <c r="G4" s="321"/>
+      <c r="H4" s="321"/>
+      <c r="I4" s="321"/>
+      <c r="J4" s="321"/>
+      <c r="K4" s="321"/>
+      <c r="L4" s="321"/>
+      <c r="M4" s="321"/>
       <c r="N4" s="201"/>
       <c r="O4" s="201"/>
     </row>
     <row r="5" spans="2:15" ht="15" customHeight="1">
-      <c r="B5" s="317" t="s">
+      <c r="B5" s="318" t="s">
         <v>358</v>
       </c>
-      <c r="C5" s="317"/>
-      <c r="D5" s="317"/>
-      <c r="E5" s="317"/>
-      <c r="F5" s="317"/>
-      <c r="G5" s="317"/>
-      <c r="H5" s="317"/>
-      <c r="I5" s="317"/>
-      <c r="J5" s="317"/>
-      <c r="K5" s="317"/>
-      <c r="L5" s="317"/>
-      <c r="M5" s="317"/>
+      <c r="C5" s="318"/>
+      <c r="D5" s="318"/>
+      <c r="E5" s="318"/>
+      <c r="F5" s="318"/>
+      <c r="G5" s="318"/>
+      <c r="H5" s="318"/>
+      <c r="I5" s="318"/>
+      <c r="J5" s="318"/>
+      <c r="K5" s="318"/>
+      <c r="L5" s="318"/>
+      <c r="M5" s="318"/>
       <c r="N5" s="200"/>
       <c r="O5" s="200"/>
     </row>
     <row r="6" spans="2:15" ht="15" customHeight="1">
-      <c r="B6" s="322" t="s">
+      <c r="B6" s="323" t="s">
         <v>359</v>
       </c>
-      <c r="C6" s="322"/>
-      <c r="D6" s="322"/>
-      <c r="E6" s="322"/>
-      <c r="F6" s="322"/>
-      <c r="G6" s="322"/>
-      <c r="H6" s="322"/>
-      <c r="I6" s="322"/>
-      <c r="J6" s="322"/>
-      <c r="K6" s="322"/>
-      <c r="L6" s="322"/>
-      <c r="M6" s="322"/>
+      <c r="C6" s="323"/>
+      <c r="D6" s="323"/>
+      <c r="E6" s="323"/>
+      <c r="F6" s="323"/>
+      <c r="G6" s="323"/>
+      <c r="H6" s="323"/>
+      <c r="I6" s="323"/>
+      <c r="J6" s="323"/>
+      <c r="K6" s="323"/>
+      <c r="L6" s="323"/>
+      <c r="M6" s="323"/>
       <c r="N6" s="202"/>
       <c r="O6" s="202"/>
     </row>
     <row r="7" spans="2:15" ht="15" customHeight="1">
-      <c r="B7" s="322" t="s">
+      <c r="B7" s="323" t="s">
         <v>360</v>
       </c>
-      <c r="C7" s="322"/>
-      <c r="D7" s="322"/>
-      <c r="E7" s="322"/>
-      <c r="F7" s="322"/>
-      <c r="G7" s="322"/>
-      <c r="H7" s="322"/>
-      <c r="I7" s="322"/>
-      <c r="J7" s="322"/>
-      <c r="K7" s="322"/>
-      <c r="L7" s="322"/>
-      <c r="M7" s="322"/>
+      <c r="C7" s="323"/>
+      <c r="D7" s="323"/>
+      <c r="E7" s="323"/>
+      <c r="F7" s="323"/>
+      <c r="G7" s="323"/>
+      <c r="H7" s="323"/>
+      <c r="I7" s="323"/>
+      <c r="J7" s="323"/>
+      <c r="K7" s="323"/>
+      <c r="L7" s="323"/>
+      <c r="M7" s="323"/>
       <c r="N7" s="202"/>
       <c r="O7" s="202"/>
     </row>
     <row r="8" spans="2:15" ht="21.75" customHeight="1">
-      <c r="B8" s="322" t="s">
+      <c r="B8" s="323" t="s">
         <v>361</v>
       </c>
-      <c r="C8" s="322"/>
-      <c r="D8" s="322"/>
-      <c r="E8" s="322"/>
-      <c r="F8" s="322"/>
-      <c r="G8" s="322"/>
-      <c r="H8" s="322"/>
-      <c r="I8" s="322"/>
-      <c r="J8" s="322"/>
-      <c r="K8" s="322"/>
-      <c r="L8" s="322"/>
-      <c r="M8" s="322"/>
+      <c r="C8" s="323"/>
+      <c r="D8" s="323"/>
+      <c r="E8" s="323"/>
+      <c r="F8" s="323"/>
+      <c r="G8" s="323"/>
+      <c r="H8" s="323"/>
+      <c r="I8" s="323"/>
+      <c r="J8" s="323"/>
+      <c r="K8" s="323"/>
+      <c r="L8" s="323"/>
+      <c r="M8" s="323"/>
       <c r="N8" s="202"/>
       <c r="O8" s="202"/>
     </row>
     <row r="9" spans="2:15" ht="30" customHeight="1">
-      <c r="B9" s="317" t="s">
+      <c r="B9" s="318" t="s">
         <v>339</v>
       </c>
-      <c r="C9" s="317"/>
-      <c r="D9" s="317"/>
-      <c r="E9" s="317"/>
-      <c r="F9" s="317"/>
-      <c r="G9" s="317"/>
-      <c r="H9" s="317"/>
-      <c r="I9" s="317"/>
-      <c r="J9" s="317"/>
-      <c r="K9" s="317"/>
-      <c r="L9" s="317"/>
+      <c r="C9" s="318"/>
+      <c r="D9" s="318"/>
+      <c r="E9" s="318"/>
+      <c r="F9" s="318"/>
+      <c r="G9" s="318"/>
+      <c r="H9" s="318"/>
+      <c r="I9" s="318"/>
+      <c r="J9" s="318"/>
+      <c r="K9" s="318"/>
+      <c r="L9" s="318"/>
     </row>
     <row r="10" spans="2:15" ht="33.75" customHeight="1">
-      <c r="B10" s="317" t="s">
+      <c r="B10" s="318" t="s">
         <v>340</v>
       </c>
-      <c r="C10" s="317"/>
-      <c r="D10" s="317"/>
-      <c r="E10" s="317"/>
-      <c r="F10" s="317"/>
-      <c r="G10" s="317"/>
-      <c r="H10" s="317"/>
-      <c r="I10" s="317"/>
-      <c r="J10" s="317"/>
-      <c r="K10" s="317"/>
-      <c r="L10" s="317"/>
+      <c r="C10" s="318"/>
+      <c r="D10" s="318"/>
+      <c r="E10" s="318"/>
+      <c r="F10" s="318"/>
+      <c r="G10" s="318"/>
+      <c r="H10" s="318"/>
+      <c r="I10" s="318"/>
+      <c r="J10" s="318"/>
+      <c r="K10" s="318"/>
+      <c r="L10" s="318"/>
     </row>
     <row r="11" spans="2:15" ht="21" customHeight="1">
-      <c r="B11" s="320" t="s">
+      <c r="B11" s="321" t="s">
         <v>341</v>
       </c>
-      <c r="C11" s="320"/>
-      <c r="D11" s="320"/>
-      <c r="E11" s="320"/>
-      <c r="F11" s="320"/>
-      <c r="G11" s="320"/>
-      <c r="H11" s="320"/>
-      <c r="I11" s="320"/>
-      <c r="J11" s="320"/>
-      <c r="K11" s="320"/>
-      <c r="L11" s="320"/>
-      <c r="M11" s="320"/>
+      <c r="C11" s="321"/>
+      <c r="D11" s="321"/>
+      <c r="E11" s="321"/>
+      <c r="F11" s="321"/>
+      <c r="G11" s="321"/>
+      <c r="H11" s="321"/>
+      <c r="I11" s="321"/>
+      <c r="J11" s="321"/>
+      <c r="K11" s="321"/>
+      <c r="L11" s="321"/>
+      <c r="M11" s="321"/>
       <c r="N11" s="62"/>
       <c r="O11" s="62"/>
     </row>
     <row r="12" spans="2:15">
-      <c r="B12" s="317" t="s">
+      <c r="B12" s="318" t="s">
         <v>342</v>
       </c>
-      <c r="C12" s="317"/>
-      <c r="D12" s="317"/>
-      <c r="E12" s="317"/>
-      <c r="F12" s="317"/>
-      <c r="G12" s="317"/>
-      <c r="H12" s="317"/>
-      <c r="I12" s="317"/>
-      <c r="J12" s="317"/>
-      <c r="K12" s="317"/>
-      <c r="L12" s="317"/>
-      <c r="M12" s="317"/>
+      <c r="C12" s="318"/>
+      <c r="D12" s="318"/>
+      <c r="E12" s="318"/>
+      <c r="F12" s="318"/>
+      <c r="G12" s="318"/>
+      <c r="H12" s="318"/>
+      <c r="I12" s="318"/>
+      <c r="J12" s="318"/>
+      <c r="K12" s="318"/>
+      <c r="L12" s="318"/>
+      <c r="M12" s="318"/>
     </row>
     <row r="13" spans="2:15">
-      <c r="B13" s="321" t="s">
+      <c r="B13" s="322" t="s">
         <v>367</v>
       </c>
-      <c r="C13" s="322"/>
-      <c r="D13" s="322"/>
-      <c r="E13" s="322"/>
-      <c r="F13" s="322"/>
-      <c r="G13" s="322"/>
-      <c r="H13" s="322"/>
-      <c r="I13" s="322"/>
-      <c r="J13" s="322"/>
-      <c r="K13" s="322"/>
-      <c r="L13" s="322"/>
-      <c r="M13" s="322"/>
+      <c r="C13" s="323"/>
+      <c r="D13" s="323"/>
+      <c r="E13" s="323"/>
+      <c r="F13" s="323"/>
+      <c r="G13" s="323"/>
+      <c r="H13" s="323"/>
+      <c r="I13" s="323"/>
+      <c r="J13" s="323"/>
+      <c r="K13" s="323"/>
+      <c r="L13" s="323"/>
+      <c r="M13" s="323"/>
     </row>
     <row r="14" spans="2:15">
-      <c r="B14" s="321" t="s">
+      <c r="B14" s="322" t="s">
         <v>368</v>
       </c>
-      <c r="C14" s="322"/>
-      <c r="D14" s="322"/>
-      <c r="E14" s="322"/>
-      <c r="F14" s="322"/>
-      <c r="G14" s="322"/>
-      <c r="H14" s="322"/>
-      <c r="I14" s="322"/>
-      <c r="J14" s="322"/>
-      <c r="K14" s="322"/>
-      <c r="L14" s="322"/>
-      <c r="M14" s="322"/>
+      <c r="C14" s="323"/>
+      <c r="D14" s="323"/>
+      <c r="E14" s="323"/>
+      <c r="F14" s="323"/>
+      <c r="G14" s="323"/>
+      <c r="H14" s="323"/>
+      <c r="I14" s="323"/>
+      <c r="J14" s="323"/>
+      <c r="K14" s="323"/>
+      <c r="L14" s="323"/>
+      <c r="M14" s="323"/>
     </row>
     <row r="15" spans="2:15" ht="17.25" customHeight="1">
-      <c r="B15" s="321" t="s">
+      <c r="B15" s="322" t="s">
         <v>369</v>
       </c>
-      <c r="C15" s="322"/>
-      <c r="D15" s="322"/>
-      <c r="E15" s="322"/>
-      <c r="F15" s="322"/>
-      <c r="G15" s="322"/>
-      <c r="H15" s="322"/>
-      <c r="I15" s="322"/>
-      <c r="J15" s="322"/>
-      <c r="K15" s="322"/>
-      <c r="L15" s="322"/>
-      <c r="M15" s="322"/>
+      <c r="C15" s="323"/>
+      <c r="D15" s="323"/>
+      <c r="E15" s="323"/>
+      <c r="F15" s="323"/>
+      <c r="G15" s="323"/>
+      <c r="H15" s="323"/>
+      <c r="I15" s="323"/>
+      <c r="J15" s="323"/>
+      <c r="K15" s="323"/>
+      <c r="L15" s="323"/>
+      <c r="M15" s="323"/>
     </row>
     <row r="16" spans="2:15">
-      <c r="B16" s="317" t="s">
+      <c r="B16" s="318" t="s">
         <v>366</v>
       </c>
-      <c r="C16" s="317"/>
-      <c r="D16" s="317"/>
-      <c r="E16" s="317"/>
-      <c r="F16" s="317"/>
-      <c r="G16" s="317"/>
-      <c r="H16" s="317"/>
-      <c r="I16" s="317"/>
-      <c r="J16" s="317"/>
-      <c r="K16" s="317"/>
-      <c r="L16" s="317"/>
-      <c r="M16" s="317"/>
-    </row>
-    <row r="17" spans="2:13" ht="18">
-      <c r="B17" s="320" t="s">
+      <c r="C16" s="318"/>
+      <c r="D16" s="318"/>
+      <c r="E16" s="318"/>
+      <c r="F16" s="318"/>
+      <c r="G16" s="318"/>
+      <c r="H16" s="318"/>
+      <c r="I16" s="318"/>
+      <c r="J16" s="318"/>
+      <c r="K16" s="318"/>
+      <c r="L16" s="318"/>
+      <c r="M16" s="318"/>
+    </row>
+    <row r="17" spans="2:13" ht="18.5">
+      <c r="B17" s="321" t="s">
         <v>343</v>
       </c>
-      <c r="C17" s="320"/>
-      <c r="D17" s="320"/>
-      <c r="E17" s="320"/>
-      <c r="F17" s="320"/>
-      <c r="G17" s="320"/>
-      <c r="H17" s="320"/>
-      <c r="I17" s="320"/>
-      <c r="J17" s="320"/>
-      <c r="K17" s="320"/>
-      <c r="L17" s="320"/>
-      <c r="M17" s="320"/>
+      <c r="C17" s="321"/>
+      <c r="D17" s="321"/>
+      <c r="E17" s="321"/>
+      <c r="F17" s="321"/>
+      <c r="G17" s="321"/>
+      <c r="H17" s="321"/>
+      <c r="I17" s="321"/>
+      <c r="J17" s="321"/>
+      <c r="K17" s="321"/>
+      <c r="L17" s="321"/>
+      <c r="M17" s="321"/>
     </row>
     <row r="18" spans="2:13">
-      <c r="B18" s="317" t="s">
+      <c r="B18" s="318" t="s">
         <v>344</v>
       </c>
-      <c r="C18" s="317"/>
-      <c r="D18" s="317"/>
-      <c r="E18" s="317"/>
-      <c r="F18" s="317"/>
-      <c r="G18" s="317"/>
-      <c r="H18" s="317"/>
-      <c r="I18" s="317"/>
-      <c r="J18" s="317"/>
-      <c r="K18" s="317"/>
-      <c r="L18" s="317"/>
-      <c r="M18" s="317"/>
+      <c r="C18" s="318"/>
+      <c r="D18" s="318"/>
+      <c r="E18" s="318"/>
+      <c r="F18" s="318"/>
+      <c r="G18" s="318"/>
+      <c r="H18" s="318"/>
+      <c r="I18" s="318"/>
+      <c r="J18" s="318"/>
+      <c r="K18" s="318"/>
+      <c r="L18" s="318"/>
+      <c r="M18" s="318"/>
     </row>
     <row r="19" spans="2:13" ht="14.4" customHeight="1">
       <c r="B19" s="258"/>
-      <c r="C19" s="316" t="s">
+      <c r="C19" s="317" t="s">
         <v>362</v>
       </c>
-      <c r="D19" s="316"/>
-      <c r="E19" s="316"/>
-      <c r="F19" s="316"/>
-      <c r="G19" s="316"/>
-      <c r="H19" s="316"/>
-      <c r="I19" s="316"/>
-      <c r="J19" s="316"/>
-      <c r="K19" s="316"/>
-      <c r="L19" s="316"/>
-      <c r="M19" s="316"/>
+      <c r="D19" s="317"/>
+      <c r="E19" s="317"/>
+      <c r="F19" s="317"/>
+      <c r="G19" s="317"/>
+      <c r="H19" s="317"/>
+      <c r="I19" s="317"/>
+      <c r="J19" s="317"/>
+      <c r="K19" s="317"/>
+      <c r="L19" s="317"/>
+      <c r="M19" s="317"/>
     </row>
     <row r="20" spans="2:13">
       <c r="B20" s="258"/>
-      <c r="C20" s="316" t="s">
+      <c r="C20" s="317" t="s">
         <v>363</v>
       </c>
-      <c r="D20" s="316"/>
-      <c r="E20" s="316"/>
-      <c r="F20" s="316"/>
-      <c r="G20" s="316"/>
-      <c r="H20" s="316"/>
-      <c r="I20" s="316"/>
-      <c r="J20" s="316"/>
-      <c r="K20" s="316"/>
-      <c r="L20" s="316"/>
-      <c r="M20" s="316"/>
+      <c r="D20" s="317"/>
+      <c r="E20" s="317"/>
+      <c r="F20" s="317"/>
+      <c r="G20" s="317"/>
+      <c r="H20" s="317"/>
+      <c r="I20" s="317"/>
+      <c r="J20" s="317"/>
+      <c r="K20" s="317"/>
+      <c r="L20" s="317"/>
+      <c r="M20" s="317"/>
     </row>
     <row r="21" spans="2:13" ht="14.4" customHeight="1">
       <c r="B21" s="258"/>
-      <c r="C21" s="316" t="s">
+      <c r="C21" s="317" t="s">
         <v>462</v>
       </c>
-      <c r="D21" s="316"/>
-      <c r="E21" s="316"/>
-      <c r="F21" s="316"/>
-      <c r="G21" s="316"/>
-      <c r="H21" s="316"/>
-      <c r="I21" s="316"/>
-      <c r="J21" s="316"/>
-      <c r="K21" s="316"/>
-      <c r="L21" s="316"/>
-      <c r="M21" s="316"/>
+      <c r="D21" s="317"/>
+      <c r="E21" s="317"/>
+      <c r="F21" s="317"/>
+      <c r="G21" s="317"/>
+      <c r="H21" s="317"/>
+      <c r="I21" s="317"/>
+      <c r="J21" s="317"/>
+      <c r="K21" s="317"/>
+      <c r="L21" s="317"/>
+      <c r="M21" s="317"/>
     </row>
     <row r="22" spans="2:13">
       <c r="B22" s="258"/>
-      <c r="C22" s="316" t="s">
+      <c r="C22" s="317" t="s">
         <v>458</v>
       </c>
-      <c r="D22" s="316"/>
-      <c r="E22" s="316"/>
-      <c r="F22" s="316"/>
-      <c r="G22" s="316"/>
-      <c r="H22" s="316"/>
-      <c r="I22" s="316"/>
-      <c r="J22" s="316"/>
-      <c r="K22" s="316"/>
-      <c r="L22" s="316"/>
-      <c r="M22" s="316"/>
+      <c r="D22" s="317"/>
+      <c r="E22" s="317"/>
+      <c r="F22" s="317"/>
+      <c r="G22" s="317"/>
+      <c r="H22" s="317"/>
+      <c r="I22" s="317"/>
+      <c r="J22" s="317"/>
+      <c r="K22" s="317"/>
+      <c r="L22" s="317"/>
+      <c r="M22" s="317"/>
     </row>
     <row r="23" spans="2:13" ht="14.4" customHeight="1">
       <c r="B23" s="258"/>
       <c r="C23" s="258"/>
-      <c r="D23" s="316" t="s">
+      <c r="D23" s="317" t="s">
         <v>454</v>
       </c>
-      <c r="E23" s="316"/>
-      <c r="F23" s="316"/>
-      <c r="G23" s="316"/>
-      <c r="H23" s="316"/>
-      <c r="I23" s="316"/>
-      <c r="J23" s="316"/>
-      <c r="K23" s="316"/>
-      <c r="L23" s="316"/>
-      <c r="M23" s="316"/>
+      <c r="E23" s="317"/>
+      <c r="F23" s="317"/>
+      <c r="G23" s="317"/>
+      <c r="H23" s="317"/>
+      <c r="I23" s="317"/>
+      <c r="J23" s="317"/>
+      <c r="K23" s="317"/>
+      <c r="L23" s="317"/>
+      <c r="M23" s="317"/>
     </row>
     <row r="24" spans="2:13" ht="14.4" customHeight="1">
       <c r="B24" s="258"/>
       <c r="C24" s="258"/>
-      <c r="D24" s="316" t="s">
+      <c r="D24" s="317" t="s">
         <v>455</v>
       </c>
-      <c r="E24" s="316"/>
-      <c r="F24" s="316"/>
-      <c r="G24" s="316"/>
-      <c r="H24" s="316"/>
-      <c r="I24" s="316"/>
-      <c r="J24" s="316"/>
-      <c r="K24" s="316"/>
-      <c r="L24" s="316"/>
-      <c r="M24" s="316"/>
+      <c r="E24" s="317"/>
+      <c r="F24" s="317"/>
+      <c r="G24" s="317"/>
+      <c r="H24" s="317"/>
+      <c r="I24" s="317"/>
+      <c r="J24" s="317"/>
+      <c r="K24" s="317"/>
+      <c r="L24" s="317"/>
+      <c r="M24" s="317"/>
     </row>
     <row r="25" spans="2:13">
       <c r="B25" s="255"/>
       <c r="C25" s="256"/>
-      <c r="D25" s="317" t="s">
+      <c r="D25" s="318" t="s">
         <v>456</v>
       </c>
-      <c r="E25" s="317"/>
-      <c r="F25" s="317"/>
-      <c r="G25" s="317"/>
-      <c r="H25" s="317"/>
-      <c r="I25" s="317"/>
-      <c r="J25" s="317"/>
-      <c r="K25" s="317"/>
-      <c r="L25" s="317"/>
-      <c r="M25" s="317"/>
+      <c r="E25" s="318"/>
+      <c r="F25" s="318"/>
+      <c r="G25" s="318"/>
+      <c r="H25" s="318"/>
+      <c r="I25" s="318"/>
+      <c r="J25" s="318"/>
+      <c r="K25" s="318"/>
+      <c r="L25" s="318"/>
+      <c r="M25" s="318"/>
     </row>
     <row r="26" spans="2:13">
       <c r="B26" s="255"/>
       <c r="C26" s="256"/>
-      <c r="D26" s="316" t="s">
+      <c r="D26" s="317" t="s">
         <v>457</v>
       </c>
-      <c r="E26" s="316"/>
-      <c r="F26" s="316"/>
-      <c r="G26" s="316"/>
-      <c r="H26" s="316"/>
-      <c r="I26" s="316"/>
-      <c r="J26" s="316"/>
-      <c r="K26" s="316"/>
-      <c r="L26" s="316"/>
-      <c r="M26" s="316"/>
+      <c r="E26" s="317"/>
+      <c r="F26" s="317"/>
+      <c r="G26" s="317"/>
+      <c r="H26" s="317"/>
+      <c r="I26" s="317"/>
+      <c r="J26" s="317"/>
+      <c r="K26" s="317"/>
+      <c r="L26" s="317"/>
+      <c r="M26" s="317"/>
     </row>
     <row r="27" spans="2:13" ht="15" customHeight="1">
-      <c r="B27" s="321" t="s">
+      <c r="B27" s="322" t="s">
         <v>364</v>
       </c>
-      <c r="C27" s="322"/>
-      <c r="D27" s="322"/>
-      <c r="E27" s="322"/>
-      <c r="F27" s="322"/>
-      <c r="G27" s="322"/>
-      <c r="H27" s="322"/>
-      <c r="I27" s="322"/>
-      <c r="J27" s="322"/>
-      <c r="K27" s="322"/>
-      <c r="L27" s="322"/>
-      <c r="M27" s="322"/>
+      <c r="C27" s="323"/>
+      <c r="D27" s="323"/>
+      <c r="E27" s="323"/>
+      <c r="F27" s="323"/>
+      <c r="G27" s="323"/>
+      <c r="H27" s="323"/>
+      <c r="I27" s="323"/>
+      <c r="J27" s="323"/>
+      <c r="K27" s="323"/>
+      <c r="L27" s="323"/>
+      <c r="M27" s="323"/>
     </row>
     <row r="28" spans="2:13" ht="15" customHeight="1">
-      <c r="B28" s="321" t="s">
+      <c r="B28" s="322" t="s">
         <v>365</v>
       </c>
-      <c r="C28" s="322"/>
-      <c r="D28" s="322"/>
-      <c r="E28" s="322"/>
-      <c r="F28" s="322"/>
-      <c r="G28" s="322"/>
-      <c r="H28" s="322"/>
-      <c r="I28" s="322"/>
-      <c r="J28" s="322"/>
-      <c r="K28" s="322"/>
-      <c r="L28" s="322"/>
-      <c r="M28" s="322"/>
+      <c r="C28" s="323"/>
+      <c r="D28" s="323"/>
+      <c r="E28" s="323"/>
+      <c r="F28" s="323"/>
+      <c r="G28" s="323"/>
+      <c r="H28" s="323"/>
+      <c r="I28" s="323"/>
+      <c r="J28" s="323"/>
+      <c r="K28" s="323"/>
+      <c r="L28" s="323"/>
+      <c r="M28" s="323"/>
     </row>
     <row r="29" spans="2:13">
       <c r="B29" s="199"/>
     </row>
-    <row r="30" spans="2:13" ht="18">
-      <c r="B30" s="320" t="s">
+    <row r="30" spans="2:13" ht="18.5">
+      <c r="B30" s="321" t="s">
         <v>345</v>
       </c>
-      <c r="C30" s="320"/>
-      <c r="D30" s="320"/>
-      <c r="E30" s="320"/>
-      <c r="F30" s="320"/>
-      <c r="G30" s="320"/>
-      <c r="H30" s="320"/>
-      <c r="I30" s="320"/>
-      <c r="J30" s="320"/>
-      <c r="K30" s="320"/>
-      <c r="L30" s="320"/>
-      <c r="M30" s="320"/>
+      <c r="C30" s="321"/>
+      <c r="D30" s="321"/>
+      <c r="E30" s="321"/>
+      <c r="F30" s="321"/>
+      <c r="G30" s="321"/>
+      <c r="H30" s="321"/>
+      <c r="I30" s="321"/>
+      <c r="J30" s="321"/>
+      <c r="K30" s="321"/>
+      <c r="L30" s="321"/>
+      <c r="M30" s="321"/>
     </row>
     <row r="31" spans="2:13" ht="15" customHeight="1">
-      <c r="B31" s="317" t="s">
+      <c r="B31" s="318" t="s">
         <v>370</v>
       </c>
-      <c r="C31" s="317"/>
-      <c r="D31" s="317"/>
-      <c r="E31" s="317"/>
-      <c r="F31" s="317"/>
-      <c r="G31" s="317"/>
-      <c r="H31" s="317"/>
-      <c r="I31" s="317"/>
-      <c r="J31" s="317"/>
-      <c r="K31" s="317"/>
-      <c r="L31" s="317"/>
-      <c r="M31" s="317"/>
+      <c r="C31" s="318"/>
+      <c r="D31" s="318"/>
+      <c r="E31" s="318"/>
+      <c r="F31" s="318"/>
+      <c r="G31" s="318"/>
+      <c r="H31" s="318"/>
+      <c r="I31" s="318"/>
+      <c r="J31" s="318"/>
+      <c r="K31" s="318"/>
+      <c r="L31" s="318"/>
+      <c r="M31" s="318"/>
     </row>
     <row r="32" spans="2:13" ht="31.5" customHeight="1">
-      <c r="B32" s="317" t="s">
+      <c r="B32" s="318" t="s">
         <v>346</v>
       </c>
-      <c r="C32" s="317"/>
-      <c r="D32" s="317"/>
-      <c r="E32" s="317"/>
-      <c r="F32" s="317"/>
-      <c r="G32" s="317"/>
-      <c r="H32" s="317"/>
-      <c r="I32" s="317"/>
-      <c r="J32" s="317"/>
-      <c r="K32" s="317"/>
-      <c r="L32" s="317"/>
-      <c r="M32" s="317"/>
+      <c r="C32" s="318"/>
+      <c r="D32" s="318"/>
+      <c r="E32" s="318"/>
+      <c r="F32" s="318"/>
+      <c r="G32" s="318"/>
+      <c r="H32" s="318"/>
+      <c r="I32" s="318"/>
+      <c r="J32" s="318"/>
+      <c r="K32" s="318"/>
+      <c r="L32" s="318"/>
+      <c r="M32" s="318"/>
     </row>
     <row r="33" spans="2:13" ht="28.5" customHeight="1">
-      <c r="B33" s="317" t="s">
+      <c r="B33" s="318" t="s">
         <v>347</v>
       </c>
-      <c r="C33" s="317"/>
-      <c r="D33" s="317"/>
-      <c r="E33" s="317"/>
-      <c r="F33" s="317"/>
-      <c r="G33" s="317"/>
-      <c r="H33" s="317"/>
-      <c r="I33" s="317"/>
-      <c r="J33" s="317"/>
-      <c r="K33" s="317"/>
-      <c r="L33" s="317"/>
-      <c r="M33" s="317"/>
+      <c r="C33" s="318"/>
+      <c r="D33" s="318"/>
+      <c r="E33" s="318"/>
+      <c r="F33" s="318"/>
+      <c r="G33" s="318"/>
+      <c r="H33" s="318"/>
+      <c r="I33" s="318"/>
+      <c r="J33" s="318"/>
+      <c r="K33" s="318"/>
+      <c r="L33" s="318"/>
+      <c r="M33" s="318"/>
     </row>
     <row r="34" spans="2:13">
-      <c r="B34" s="317" t="s">
+      <c r="B34" s="318" t="s">
         <v>348</v>
       </c>
-      <c r="C34" s="317"/>
-      <c r="D34" s="317"/>
-      <c r="E34" s="317"/>
-      <c r="F34" s="317"/>
-      <c r="G34" s="317"/>
-      <c r="H34" s="317"/>
-      <c r="I34" s="317"/>
-      <c r="J34" s="317"/>
-      <c r="K34" s="317"/>
-      <c r="L34" s="317"/>
-      <c r="M34" s="317"/>
+      <c r="C34" s="318"/>
+      <c r="D34" s="318"/>
+      <c r="E34" s="318"/>
+      <c r="F34" s="318"/>
+      <c r="G34" s="318"/>
+      <c r="H34" s="318"/>
+      <c r="I34" s="318"/>
+      <c r="J34" s="318"/>
+      <c r="K34" s="318"/>
+      <c r="L34" s="318"/>
+      <c r="M34" s="318"/>
     </row>
     <row r="35" spans="2:13">
-      <c r="B35" s="317" t="s">
+      <c r="B35" s="318" t="s">
         <v>349</v>
       </c>
-      <c r="C35" s="317"/>
-      <c r="D35" s="317"/>
-      <c r="E35" s="317"/>
-      <c r="F35" s="317"/>
-      <c r="G35" s="317"/>
-      <c r="H35" s="317"/>
-      <c r="I35" s="317"/>
-      <c r="J35" s="317"/>
-      <c r="K35" s="317"/>
-      <c r="L35" s="317"/>
-      <c r="M35" s="317"/>
-    </row>
-    <row r="36" spans="2:13" ht="18">
-      <c r="B36" s="320" t="s">
+      <c r="C35" s="318"/>
+      <c r="D35" s="318"/>
+      <c r="E35" s="318"/>
+      <c r="F35" s="318"/>
+      <c r="G35" s="318"/>
+      <c r="H35" s="318"/>
+      <c r="I35" s="318"/>
+      <c r="J35" s="318"/>
+      <c r="K35" s="318"/>
+      <c r="L35" s="318"/>
+      <c r="M35" s="318"/>
+    </row>
+    <row r="36" spans="2:13" ht="18.5">
+      <c r="B36" s="321" t="s">
         <v>350</v>
       </c>
-      <c r="C36" s="320"/>
-      <c r="D36" s="320"/>
-      <c r="E36" s="320"/>
-      <c r="F36" s="320"/>
-      <c r="G36" s="320"/>
-      <c r="H36" s="320"/>
-      <c r="I36" s="320"/>
-      <c r="J36" s="320"/>
-      <c r="K36" s="320"/>
-      <c r="L36" s="320"/>
-      <c r="M36" s="320"/>
+      <c r="C36" s="321"/>
+      <c r="D36" s="321"/>
+      <c r="E36" s="321"/>
+      <c r="F36" s="321"/>
+      <c r="G36" s="321"/>
+      <c r="H36" s="321"/>
+      <c r="I36" s="321"/>
+      <c r="J36" s="321"/>
+      <c r="K36" s="321"/>
+      <c r="L36" s="321"/>
+      <c r="M36" s="321"/>
     </row>
     <row r="37" spans="2:13" ht="30.75" customHeight="1">
-      <c r="B37" s="317" t="s">
+      <c r="B37" s="318" t="s">
         <v>351</v>
       </c>
-      <c r="C37" s="317"/>
-      <c r="D37" s="317"/>
-      <c r="E37" s="317"/>
-      <c r="F37" s="317"/>
-      <c r="G37" s="317"/>
-      <c r="H37" s="317"/>
-      <c r="I37" s="317"/>
-      <c r="J37" s="317"/>
-      <c r="K37" s="317"/>
-      <c r="L37" s="317"/>
-      <c r="M37" s="317"/>
+      <c r="C37" s="318"/>
+      <c r="D37" s="318"/>
+      <c r="E37" s="318"/>
+      <c r="F37" s="318"/>
+      <c r="G37" s="318"/>
+      <c r="H37" s="318"/>
+      <c r="I37" s="318"/>
+      <c r="J37" s="318"/>
+      <c r="K37" s="318"/>
+      <c r="L37" s="318"/>
+      <c r="M37" s="318"/>
     </row>
     <row r="38" spans="2:13">
-      <c r="B38" s="317" t="s">
+      <c r="B38" s="318" t="s">
         <v>352</v>
       </c>
-      <c r="C38" s="317"/>
-      <c r="D38" s="317"/>
-      <c r="E38" s="317"/>
-      <c r="F38" s="317"/>
-      <c r="G38" s="317"/>
-      <c r="H38" s="317"/>
-      <c r="I38" s="317"/>
-      <c r="J38" s="317"/>
-      <c r="K38" s="317"/>
-      <c r="L38" s="317"/>
-      <c r="M38" s="317"/>
+      <c r="C38" s="318"/>
+      <c r="D38" s="318"/>
+      <c r="E38" s="318"/>
+      <c r="F38" s="318"/>
+      <c r="G38" s="318"/>
+      <c r="H38" s="318"/>
+      <c r="I38" s="318"/>
+      <c r="J38" s="318"/>
+      <c r="K38" s="318"/>
+      <c r="L38" s="318"/>
+      <c r="M38" s="318"/>
     </row>
     <row r="39" spans="2:13">
       <c r="B39" s="199"/>
     </row>
-    <row r="40" spans="2:13" ht="18">
-      <c r="B40" s="320" t="s">
+    <row r="40" spans="2:13" ht="18.5">
+      <c r="B40" s="321" t="s">
         <v>353</v>
       </c>
-      <c r="C40" s="320"/>
-      <c r="D40" s="320"/>
-      <c r="E40" s="320"/>
-      <c r="F40" s="320"/>
-      <c r="G40" s="320"/>
-      <c r="H40" s="320"/>
-      <c r="I40" s="320"/>
-      <c r="J40" s="320"/>
-      <c r="K40" s="320"/>
-      <c r="L40" s="320"/>
-      <c r="M40" s="320"/>
+      <c r="C40" s="321"/>
+      <c r="D40" s="321"/>
+      <c r="E40" s="321"/>
+      <c r="F40" s="321"/>
+      <c r="G40" s="321"/>
+      <c r="H40" s="321"/>
+      <c r="I40" s="321"/>
+      <c r="J40" s="321"/>
+      <c r="K40" s="321"/>
+      <c r="L40" s="321"/>
+      <c r="M40" s="321"/>
     </row>
     <row r="41" spans="2:13">
-      <c r="B41" s="319" t="s">
+      <c r="B41" s="320" t="s">
         <v>354</v>
       </c>
-      <c r="C41" s="319"/>
-      <c r="D41" s="319"/>
-      <c r="E41" s="319"/>
-      <c r="F41" s="319"/>
-      <c r="G41" s="319"/>
-      <c r="H41" s="319"/>
-      <c r="I41" s="319"/>
-      <c r="J41" s="319"/>
-      <c r="K41" s="319"/>
-      <c r="L41" s="319"/>
-      <c r="M41" s="319"/>
+      <c r="C41" s="320"/>
+      <c r="D41" s="320"/>
+      <c r="E41" s="320"/>
+      <c r="F41" s="320"/>
+      <c r="G41" s="320"/>
+      <c r="H41" s="320"/>
+      <c r="I41" s="320"/>
+      <c r="J41" s="320"/>
+      <c r="K41" s="320"/>
+      <c r="L41" s="320"/>
+      <c r="M41" s="320"/>
     </row>
     <row r="42" spans="2:13">
-      <c r="B42" s="319" t="s">
+      <c r="B42" s="320" t="s">
         <v>355</v>
       </c>
-      <c r="C42" s="319"/>
-      <c r="D42" s="319"/>
-      <c r="E42" s="319"/>
-      <c r="F42" s="319"/>
-      <c r="G42" s="319"/>
-      <c r="H42" s="319"/>
-      <c r="I42" s="319"/>
-      <c r="J42" s="319"/>
-      <c r="K42" s="319"/>
-      <c r="L42" s="319"/>
-      <c r="M42" s="319"/>
+      <c r="C42" s="320"/>
+      <c r="D42" s="320"/>
+      <c r="E42" s="320"/>
+      <c r="F42" s="320"/>
+      <c r="G42" s="320"/>
+      <c r="H42" s="320"/>
+      <c r="I42" s="320"/>
+      <c r="J42" s="320"/>
+      <c r="K42" s="320"/>
+      <c r="L42" s="320"/>
+      <c r="M42" s="320"/>
     </row>
     <row r="43" spans="2:13">
-      <c r="B43" s="319" t="s">
+      <c r="B43" s="320" t="s">
         <v>356</v>
       </c>
-      <c r="C43" s="319"/>
-      <c r="D43" s="319"/>
-      <c r="E43" s="319"/>
-      <c r="F43" s="319"/>
-      <c r="G43" s="319"/>
-      <c r="H43" s="319"/>
-      <c r="I43" s="319"/>
-      <c r="J43" s="319"/>
-      <c r="K43" s="319"/>
-      <c r="L43" s="319"/>
-      <c r="M43" s="319"/>
+      <c r="C43" s="320"/>
+      <c r="D43" s="320"/>
+      <c r="E43" s="320"/>
+      <c r="F43" s="320"/>
+      <c r="G43" s="320"/>
+      <c r="H43" s="320"/>
+      <c r="I43" s="320"/>
+      <c r="J43" s="320"/>
+      <c r="K43" s="320"/>
+      <c r="L43" s="320"/>
+      <c r="M43" s="320"/>
     </row>
     <row r="44" spans="2:13">
       <c r="B44" s="249" t="s">
@@ -9585,53 +8570,53 @@
       <c r="L44" s="247"/>
       <c r="M44" s="247"/>
     </row>
-    <row r="45" spans="2:13" ht="18">
-      <c r="B45" s="320" t="s">
+    <row r="45" spans="2:13" ht="18.5">
+      <c r="B45" s="321" t="s">
         <v>357</v>
       </c>
-      <c r="C45" s="320"/>
-      <c r="D45" s="320"/>
-      <c r="E45" s="320"/>
-      <c r="F45" s="320"/>
-      <c r="G45" s="320"/>
-      <c r="H45" s="320"/>
-      <c r="I45" s="320"/>
-      <c r="J45" s="320"/>
-      <c r="K45" s="320"/>
-      <c r="L45" s="320"/>
-      <c r="M45" s="320"/>
+      <c r="C45" s="321"/>
+      <c r="D45" s="321"/>
+      <c r="E45" s="321"/>
+      <c r="F45" s="321"/>
+      <c r="G45" s="321"/>
+      <c r="H45" s="321"/>
+      <c r="I45" s="321"/>
+      <c r="J45" s="321"/>
+      <c r="K45" s="321"/>
+      <c r="L45" s="321"/>
+      <c r="M45" s="321"/>
     </row>
     <row r="46" spans="2:13">
-      <c r="B46" s="317" t="s">
+      <c r="B46" s="318" t="s">
         <v>461</v>
       </c>
-      <c r="C46" s="317"/>
-      <c r="D46" s="317"/>
-      <c r="E46" s="317"/>
-      <c r="F46" s="317"/>
-      <c r="G46" s="317"/>
-      <c r="H46" s="317"/>
-      <c r="I46" s="317"/>
-      <c r="J46" s="317"/>
-      <c r="K46" s="317"/>
-      <c r="L46" s="317"/>
-      <c r="M46" s="317"/>
+      <c r="C46" s="318"/>
+      <c r="D46" s="318"/>
+      <c r="E46" s="318"/>
+      <c r="F46" s="318"/>
+      <c r="G46" s="318"/>
+      <c r="H46" s="318"/>
+      <c r="I46" s="318"/>
+      <c r="J46" s="318"/>
+      <c r="K46" s="318"/>
+      <c r="L46" s="318"/>
+      <c r="M46" s="318"/>
     </row>
     <row r="47" spans="2:13">
-      <c r="B47" s="318" t="s">
+      <c r="B47" s="319" t="s">
         <v>447</v>
       </c>
-      <c r="C47" s="318"/>
-      <c r="D47" s="318"/>
-      <c r="E47" s="318"/>
-      <c r="F47" s="318"/>
-      <c r="G47" s="318"/>
-      <c r="H47" s="318"/>
-      <c r="I47" s="318"/>
-      <c r="J47" s="318"/>
-      <c r="K47" s="318"/>
-      <c r="L47" s="318"/>
-      <c r="M47" s="318"/>
+      <c r="C47" s="319"/>
+      <c r="D47" s="319"/>
+      <c r="E47" s="319"/>
+      <c r="F47" s="319"/>
+      <c r="G47" s="319"/>
+      <c r="H47" s="319"/>
+      <c r="I47" s="319"/>
+      <c r="J47" s="319"/>
+      <c r="K47" s="319"/>
+      <c r="L47" s="319"/>
+      <c r="M47" s="319"/>
     </row>
   </sheetData>
   <mergeCells count="43">
@@ -9703,9 +8688,9 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="35.77734375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="35.81640625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:11">
@@ -10100,15 +9085,15 @@
   </sheetPr>
   <dimension ref="A1:V115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:C6"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="0.77734375" customWidth="1"/>
-    <col min="2" max="2" width="16.77734375" customWidth="1"/>
-    <col min="3" max="3" width="34.21875" customWidth="1"/>
+    <col min="1" max="1" width="0.81640625" customWidth="1"/>
+    <col min="2" max="2" width="16.81640625" customWidth="1"/>
+    <col min="3" max="3" width="34.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" s="13" customFormat="1">
@@ -10142,18 +9127,18 @@
     </row>
     <row r="4" spans="1:22" ht="15" customHeight="1">
       <c r="A4" s="13"/>
-      <c r="B4" s="348" t="s">
+      <c r="B4" s="349" t="s">
         <v>466</v>
       </c>
-      <c r="C4" s="348" t="s">
+      <c r="C4" s="349" t="s">
         <v>121</v>
       </c>
-      <c r="D4" s="350"/>
-      <c r="E4" s="350"/>
-      <c r="F4" s="350"/>
-      <c r="G4" s="350"/>
-      <c r="H4" s="350"/>
-      <c r="I4" s="350"/>
+      <c r="D4" s="351"/>
+      <c r="E4" s="351"/>
+      <c r="F4" s="351"/>
+      <c r="G4" s="351"/>
+      <c r="H4" s="351"/>
+      <c r="I4" s="351"/>
       <c r="J4" s="13"/>
       <c r="K4" s="13"/>
       <c r="L4" s="13"/>
@@ -10170,8 +9155,8 @@
     </row>
     <row r="5" spans="1:22">
       <c r="A5" s="13"/>
-      <c r="B5" s="349"/>
-      <c r="C5" s="349"/>
+      <c r="B5" s="350"/>
+      <c r="C5" s="350"/>
       <c r="D5" s="172" t="s">
         <v>88</v>
       </c>
@@ -10205,10 +9190,10 @@
       <c r="V5" s="13"/>
     </row>
     <row r="6" spans="1:22">
-      <c r="B6" s="366" t="s">
+      <c r="B6" s="316" t="s">
         <v>467</v>
       </c>
-      <c r="C6" s="366" t="s">
+      <c r="C6" s="316" t="s">
         <v>205</v>
       </c>
       <c r="D6" s="176">
@@ -13473,29 +12458,29 @@
       <selection pane="topRight" activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="9.77734375" customWidth="1"/>
-    <col min="2" max="2" width="22.77734375" customWidth="1"/>
-    <col min="3" max="3" width="9.5546875" customWidth="1"/>
-    <col min="4" max="4" width="9.21875" customWidth="1"/>
-    <col min="5" max="5" width="6.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29.77734375" customWidth="1"/>
-    <col min="8" max="9" width="10.21875" customWidth="1"/>
-    <col min="10" max="10" width="0.77734375" style="17" customWidth="1"/>
-    <col min="11" max="12" width="6.77734375" customWidth="1"/>
-    <col min="13" max="13" width="0.77734375" customWidth="1"/>
-    <col min="14" max="15" width="6.77734375" customWidth="1"/>
-    <col min="16" max="16" width="0.77734375" customWidth="1"/>
-    <col min="17" max="17" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="0.77734375" customWidth="1"/>
-    <col min="20" max="21" width="29.77734375" customWidth="1"/>
-    <col min="22" max="22" width="0.77734375" style="17" customWidth="1"/>
-    <col min="23" max="23" width="15.33203125" customWidth="1"/>
-    <col min="24" max="26" width="13.21875" customWidth="1"/>
-    <col min="27" max="32" width="11.44140625" style="13"/>
+    <col min="1" max="1" width="9.81640625" customWidth="1"/>
+    <col min="2" max="2" width="22.81640625" customWidth="1"/>
+    <col min="3" max="3" width="9.54296875" customWidth="1"/>
+    <col min="4" max="4" width="9.1796875" customWidth="1"/>
+    <col min="5" max="5" width="6.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.81640625" customWidth="1"/>
+    <col min="8" max="9" width="10.1796875" customWidth="1"/>
+    <col min="10" max="10" width="0.81640625" style="17" customWidth="1"/>
+    <col min="11" max="12" width="6.81640625" customWidth="1"/>
+    <col min="13" max="13" width="0.81640625" customWidth="1"/>
+    <col min="14" max="15" width="6.81640625" customWidth="1"/>
+    <col min="16" max="16" width="0.81640625" customWidth="1"/>
+    <col min="17" max="17" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="0.81640625" customWidth="1"/>
+    <col min="20" max="21" width="29.81640625" customWidth="1"/>
+    <col min="22" max="22" width="0.81640625" style="17" customWidth="1"/>
+    <col min="23" max="23" width="15.36328125" customWidth="1"/>
+    <col min="24" max="26" width="13.1796875" customWidth="1"/>
+    <col min="27" max="32" width="11.453125" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:32">
@@ -13524,7 +12509,7 @@
       <c r="Y1" s="13"/>
       <c r="Z1" s="13"/>
     </row>
-    <row r="2" spans="1:32" ht="23.4">
+    <row r="2" spans="1:32" ht="23.5">
       <c r="A2" s="154" t="s">
         <v>336</v>
       </c>
@@ -13737,121 +12722,121 @@
       <c r="Z8" s="13"/>
     </row>
     <row r="9" spans="1:32" ht="15" customHeight="1">
-      <c r="A9" s="351" t="s">
+      <c r="A9" s="352" t="s">
         <v>77</v>
       </c>
-      <c r="B9" s="351"/>
-      <c r="C9" s="358" t="s">
+      <c r="B9" s="352"/>
+      <c r="C9" s="359" t="s">
         <v>80</v>
       </c>
-      <c r="D9" s="358"/>
-      <c r="E9" s="358"/>
-      <c r="F9" s="358"/>
-      <c r="G9" s="358"/>
-      <c r="H9" s="358"/>
-      <c r="I9" s="358"/>
+      <c r="D9" s="359"/>
+      <c r="E9" s="359"/>
+      <c r="F9" s="359"/>
+      <c r="G9" s="359"/>
+      <c r="H9" s="359"/>
+      <c r="I9" s="359"/>
       <c r="J9" s="29"/>
-      <c r="K9" s="359" t="s">
+      <c r="K9" s="360" t="s">
         <v>78</v>
       </c>
-      <c r="L9" s="359"/>
-      <c r="M9" s="359"/>
-      <c r="N9" s="359"/>
-      <c r="O9" s="359"/>
-      <c r="P9" s="359"/>
-      <c r="Q9" s="359"/>
-      <c r="R9" s="359"/>
-      <c r="S9" s="359"/>
-      <c r="T9" s="359"/>
-      <c r="U9" s="359"/>
+      <c r="L9" s="360"/>
+      <c r="M9" s="360"/>
+      <c r="N9" s="360"/>
+      <c r="O9" s="360"/>
+      <c r="P9" s="360"/>
+      <c r="Q9" s="360"/>
+      <c r="R9" s="360"/>
+      <c r="S9" s="360"/>
+      <c r="T9" s="360"/>
+      <c r="U9" s="360"/>
       <c r="V9" s="29"/>
-      <c r="W9" s="355" t="s">
+      <c r="W9" s="356" t="s">
         <v>79</v>
       </c>
-      <c r="X9" s="356"/>
-      <c r="Y9" s="356"/>
-      <c r="Z9" s="357"/>
+      <c r="X9" s="357"/>
+      <c r="Y9" s="357"/>
+      <c r="Z9" s="358"/>
     </row>
     <row r="10" spans="1:32">
-      <c r="A10" s="352" t="s">
+      <c r="A10" s="353" t="s">
         <v>122</v>
       </c>
-      <c r="B10" s="352" t="s">
+      <c r="B10" s="353" t="s">
         <v>121</v>
       </c>
-      <c r="C10" s="352" t="s">
+      <c r="C10" s="353" t="s">
         <v>81</v>
       </c>
-      <c r="D10" s="352" t="s">
+      <c r="D10" s="353" t="s">
         <v>86</v>
       </c>
-      <c r="E10" s="352" t="s">
+      <c r="E10" s="353" t="s">
         <v>120</v>
       </c>
-      <c r="F10" s="352" t="s">
+      <c r="F10" s="353" t="s">
         <v>84</v>
       </c>
-      <c r="G10" s="352" t="s">
+      <c r="G10" s="353" t="s">
         <v>85</v>
       </c>
-      <c r="H10" s="360" t="s">
+      <c r="H10" s="361" t="s">
         <v>113</v>
       </c>
-      <c r="I10" s="360" t="s">
+      <c r="I10" s="361" t="s">
         <v>114</v>
       </c>
       <c r="J10" s="30"/>
-      <c r="K10" s="361" t="s">
+      <c r="K10" s="362" t="s">
         <v>81</v>
       </c>
-      <c r="L10" s="361" t="s">
+      <c r="L10" s="362" t="s">
         <v>82</v>
       </c>
       <c r="M10" s="78"/>
-      <c r="N10" s="361" t="s">
+      <c r="N10" s="362" t="s">
         <v>83</v>
       </c>
-      <c r="O10" s="361" t="s">
+      <c r="O10" s="362" t="s">
         <v>82</v>
       </c>
       <c r="P10" s="78"/>
-      <c r="Q10" s="361" t="s">
+      <c r="Q10" s="362" t="s">
         <v>84</v>
       </c>
-      <c r="R10" s="361" t="s">
+      <c r="R10" s="362" t="s">
         <v>82</v>
       </c>
       <c r="S10" s="78"/>
-      <c r="T10" s="361" t="s">
+      <c r="T10" s="362" t="s">
         <v>85</v>
       </c>
-      <c r="U10" s="361" t="s">
+      <c r="U10" s="362" t="s">
         <v>82</v>
       </c>
       <c r="V10" s="30"/>
-      <c r="W10" s="354" t="s">
+      <c r="W10" s="355" t="s">
         <v>118</v>
       </c>
-      <c r="X10" s="354" t="s">
+      <c r="X10" s="355" t="s">
         <v>115</v>
       </c>
-      <c r="Y10" s="354" t="s">
+      <c r="Y10" s="355" t="s">
         <v>116</v>
       </c>
-      <c r="Z10" s="352" t="s">
+      <c r="Z10" s="353" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:32" ht="15" customHeight="1">
-      <c r="A11" s="353"/>
-      <c r="B11" s="353"/>
-      <c r="C11" s="353"/>
-      <c r="D11" s="353"/>
-      <c r="E11" s="353"/>
-      <c r="F11" s="353"/>
-      <c r="G11" s="353"/>
-      <c r="H11" s="353"/>
-      <c r="I11" s="353"/>
+      <c r="A11" s="354"/>
+      <c r="B11" s="354"/>
+      <c r="C11" s="354"/>
+      <c r="D11" s="354"/>
+      <c r="E11" s="354"/>
+      <c r="F11" s="354"/>
+      <c r="G11" s="354"/>
+      <c r="H11" s="354"/>
+      <c r="I11" s="354"/>
       <c r="J11" s="30"/>
       <c r="K11" s="287">
         <v>2018</v>
@@ -13881,12 +12866,12 @@
         <v>2023</v>
       </c>
       <c r="V11" s="30"/>
-      <c r="W11" s="353"/>
-      <c r="X11" s="353"/>
-      <c r="Y11" s="353"/>
-      <c r="Z11" s="353"/>
-    </row>
-    <row r="12" spans="1:32" s="3" customFormat="1" ht="22.05" customHeight="1">
+      <c r="W11" s="354"/>
+      <c r="X11" s="354"/>
+      <c r="Y11" s="354"/>
+      <c r="Z11" s="354"/>
+    </row>
+    <row r="12" spans="1:32" s="3" customFormat="1" ht="22" customHeight="1">
       <c r="A12" s="288" t="s">
         <v>44</v>
       </c>
@@ -13962,7 +12947,7 @@
       <c r="AE12" s="33"/>
       <c r="AF12" s="33"/>
     </row>
-    <row r="13" spans="1:32" s="3" customFormat="1" ht="22.05" customHeight="1">
+    <row r="13" spans="1:32" s="3" customFormat="1" ht="22" customHeight="1">
       <c r="A13" s="174" t="s">
         <v>47</v>
       </c>
@@ -14000,7 +12985,7 @@
       <c r="AE13" s="33"/>
       <c r="AF13" s="33"/>
     </row>
-    <row r="14" spans="1:32" s="3" customFormat="1" ht="22.05" customHeight="1">
+    <row r="14" spans="1:32" s="3" customFormat="1" ht="22" customHeight="1">
       <c r="A14" s="174" t="s">
         <v>49</v>
       </c>
@@ -14076,7 +13061,7 @@
       <c r="AE14" s="33"/>
       <c r="AF14" s="33"/>
     </row>
-    <row r="15" spans="1:32" s="3" customFormat="1" ht="22.05" customHeight="1">
+    <row r="15" spans="1:32" s="3" customFormat="1" ht="22" customHeight="1">
       <c r="A15" s="174" t="s">
         <v>123</v>
       </c>
@@ -14118,7 +13103,7 @@
       <c r="AE15" s="33"/>
       <c r="AF15" s="33"/>
     </row>
-    <row r="16" spans="1:32" s="3" customFormat="1" ht="22.05" customHeight="1">
+    <row r="16" spans="1:32" s="3" customFormat="1" ht="22" customHeight="1">
       <c r="A16" s="174" t="s">
         <v>51</v>
       </c>
@@ -14194,7 +13179,7 @@
       <c r="AE16" s="33"/>
       <c r="AF16" s="33"/>
     </row>
-    <row r="17" spans="1:32" s="3" customFormat="1" ht="22.05" customHeight="1">
+    <row r="17" spans="1:32" s="3" customFormat="1" ht="22" customHeight="1">
       <c r="A17" s="174" t="s">
         <v>53</v>
       </c>
@@ -14254,7 +13239,7 @@
       <c r="AE17" s="33"/>
       <c r="AF17" s="33"/>
     </row>
-    <row r="18" spans="1:32" s="3" customFormat="1" ht="22.05" customHeight="1">
+    <row r="18" spans="1:32" s="3" customFormat="1" ht="22" customHeight="1">
       <c r="A18" s="174" t="s">
         <v>55</v>
       </c>
@@ -14292,7 +13277,7 @@
       <c r="AE18" s="33"/>
       <c r="AF18" s="33"/>
     </row>
-    <row r="19" spans="1:32" s="3" customFormat="1" ht="22.05" customHeight="1">
+    <row r="19" spans="1:32" s="3" customFormat="1" ht="22" customHeight="1">
       <c r="A19" s="174" t="s">
         <v>57</v>
       </c>
@@ -14368,7 +13353,7 @@
       <c r="AE19" s="33"/>
       <c r="AF19" s="33"/>
     </row>
-    <row r="20" spans="1:32" s="3" customFormat="1" ht="22.05" customHeight="1">
+    <row r="20" spans="1:32" s="3" customFormat="1" ht="22" customHeight="1">
       <c r="A20" s="174" t="s">
         <v>59</v>
       </c>
@@ -14444,7 +13429,7 @@
       <c r="AE20" s="33"/>
       <c r="AF20" s="33"/>
     </row>
-    <row r="21" spans="1:32" s="3" customFormat="1" ht="22.05" customHeight="1">
+    <row r="21" spans="1:32" s="3" customFormat="1" ht="22" customHeight="1">
       <c r="A21" s="174" t="s">
         <v>61</v>
       </c>
@@ -14520,7 +13505,7 @@
       <c r="AE21" s="33"/>
       <c r="AF21" s="33"/>
     </row>
-    <row r="22" spans="1:32" s="3" customFormat="1" ht="22.05" customHeight="1">
+    <row r="22" spans="1:32" s="3" customFormat="1" ht="22" customHeight="1">
       <c r="A22" s="174" t="s">
         <v>63</v>
       </c>
@@ -14596,7 +13581,7 @@
       <c r="AE22" s="33"/>
       <c r="AF22" s="33"/>
     </row>
-    <row r="23" spans="1:32" s="3" customFormat="1" ht="22.05" customHeight="1">
+    <row r="23" spans="1:32" s="3" customFormat="1" ht="22" customHeight="1">
       <c r="A23" s="174" t="s">
         <v>65</v>
       </c>
@@ -14672,7 +13657,7 @@
       <c r="AE23" s="33"/>
       <c r="AF23" s="33"/>
     </row>
-    <row r="24" spans="1:32" s="3" customFormat="1" ht="22.05" customHeight="1">
+    <row r="24" spans="1:32" s="3" customFormat="1" ht="22" customHeight="1">
       <c r="A24" s="174" t="s">
         <v>67</v>
       </c>
@@ -14748,7 +13733,7 @@
       <c r="AE24" s="33"/>
       <c r="AF24" s="33"/>
     </row>
-    <row r="25" spans="1:32" s="3" customFormat="1" ht="22.05" customHeight="1">
+    <row r="25" spans="1:32" s="3" customFormat="1" ht="22" customHeight="1">
       <c r="A25" s="174" t="s">
         <v>69</v>
       </c>
@@ -14824,7 +13809,7 @@
       <c r="AE25" s="33"/>
       <c r="AF25" s="33"/>
     </row>
-    <row r="26" spans="1:32" s="3" customFormat="1" ht="22.05" customHeight="1">
+    <row r="26" spans="1:32" s="3" customFormat="1" ht="22" customHeight="1">
       <c r="A26" s="174" t="s">
         <v>71</v>
       </c>
@@ -14900,7 +13885,7 @@
       <c r="AE26" s="33"/>
       <c r="AF26" s="33"/>
     </row>
-    <row r="27" spans="1:32" s="3" customFormat="1" ht="22.05" customHeight="1">
+    <row r="27" spans="1:32" s="3" customFormat="1" ht="22" customHeight="1">
       <c r="A27" s="174" t="s">
         <v>73</v>
       </c>
@@ -14976,7 +13961,7 @@
       <c r="AE27" s="33"/>
       <c r="AF27" s="33"/>
     </row>
-    <row r="28" spans="1:32" s="3" customFormat="1" ht="22.05" customHeight="1">
+    <row r="28" spans="1:32" s="3" customFormat="1" ht="22" customHeight="1">
       <c r="A28" s="175" t="s">
         <v>51</v>
       </c>
@@ -15682,7 +14667,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="40" orientation="landscape" horizontalDpi="4294967293" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="37" orientation="landscape" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -15697,10 +14682,10 @@
       <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="0.77734375" customWidth="1"/>
-    <col min="2" max="2" width="27.77734375" customWidth="1"/>
+    <col min="1" max="1" width="0.81640625" customWidth="1"/>
+    <col min="2" max="2" width="27.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:39" s="13" customFormat="1">
@@ -15788,35 +14773,35 @@
     </row>
     <row r="4" spans="1:39" ht="15" customHeight="1">
       <c r="A4" s="13"/>
-      <c r="B4" s="363" t="s">
+      <c r="B4" s="364" t="s">
         <v>121</v>
       </c>
-      <c r="C4" s="362" t="s">
+      <c r="C4" s="363" t="s">
         <v>267</v>
       </c>
-      <c r="D4" s="362"/>
-      <c r="E4" s="362"/>
-      <c r="F4" s="362"/>
-      <c r="G4" s="362"/>
-      <c r="H4" s="362"/>
-      <c r="I4" s="362"/>
-      <c r="J4" s="362"/>
-      <c r="K4" s="362"/>
-      <c r="L4" s="362"/>
-      <c r="M4" s="362"/>
-      <c r="N4" s="362"/>
-      <c r="O4" s="362"/>
-      <c r="P4" s="362"/>
-      <c r="Q4" s="362"/>
-      <c r="R4" s="362"/>
-      <c r="S4" s="362"/>
-      <c r="T4" s="362"/>
-      <c r="U4" s="362"/>
-      <c r="V4" s="362"/>
-      <c r="W4" s="362"/>
-      <c r="X4" s="362"/>
-      <c r="Y4" s="362"/>
-      <c r="Z4" s="362"/>
+      <c r="D4" s="363"/>
+      <c r="E4" s="363"/>
+      <c r="F4" s="363"/>
+      <c r="G4" s="363"/>
+      <c r="H4" s="363"/>
+      <c r="I4" s="363"/>
+      <c r="J4" s="363"/>
+      <c r="K4" s="363"/>
+      <c r="L4" s="363"/>
+      <c r="M4" s="363"/>
+      <c r="N4" s="363"/>
+      <c r="O4" s="363"/>
+      <c r="P4" s="363"/>
+      <c r="Q4" s="363"/>
+      <c r="R4" s="363"/>
+      <c r="S4" s="363"/>
+      <c r="T4" s="363"/>
+      <c r="U4" s="363"/>
+      <c r="V4" s="363"/>
+      <c r="W4" s="363"/>
+      <c r="X4" s="363"/>
+      <c r="Y4" s="363"/>
+      <c r="Z4" s="363"/>
       <c r="AA4" s="13"/>
       <c r="AB4" s="13"/>
       <c r="AC4" s="13"/>
@@ -15833,7 +14818,7 @@
     </row>
     <row r="5" spans="1:39">
       <c r="A5" s="13"/>
-      <c r="B5" s="364"/>
+      <c r="B5" s="365"/>
       <c r="C5" s="240" t="s">
         <v>127</v>
       </c>
@@ -16972,28 +15957,28 @@
       <c r="Z22" s="241"/>
     </row>
     <row r="23" spans="2:26">
-      <c r="B23" s="365"/>
-      <c r="C23" s="365"/>
-      <c r="D23" s="365"/>
-      <c r="E23" s="365"/>
-      <c r="F23" s="365"/>
-      <c r="G23" s="365"/>
-      <c r="H23" s="365"/>
-      <c r="I23" s="365"/>
-      <c r="J23" s="365"/>
-      <c r="K23" s="365"/>
-      <c r="L23" s="365"/>
-      <c r="M23" s="365"/>
-      <c r="N23" s="365"/>
-      <c r="O23" s="365"/>
-      <c r="P23" s="365"/>
-      <c r="Q23" s="365"/>
-      <c r="R23" s="365"/>
-      <c r="S23" s="365"/>
-      <c r="T23" s="365"/>
-      <c r="U23" s="365"/>
-      <c r="V23" s="365"/>
-      <c r="W23" s="365"/>
+      <c r="B23" s="366"/>
+      <c r="C23" s="366"/>
+      <c r="D23" s="366"/>
+      <c r="E23" s="366"/>
+      <c r="F23" s="366"/>
+      <c r="G23" s="366"/>
+      <c r="H23" s="366"/>
+      <c r="I23" s="366"/>
+      <c r="J23" s="366"/>
+      <c r="K23" s="366"/>
+      <c r="L23" s="366"/>
+      <c r="M23" s="366"/>
+      <c r="N23" s="366"/>
+      <c r="O23" s="366"/>
+      <c r="P23" s="366"/>
+      <c r="Q23" s="366"/>
+      <c r="R23" s="366"/>
+      <c r="S23" s="366"/>
+      <c r="T23" s="366"/>
+      <c r="U23" s="366"/>
+      <c r="V23" s="366"/>
+      <c r="W23" s="366"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -17017,7 +16002,7 @@
       <selection activeCell="V12" sqref="V12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="20" max="20" width="7" customWidth="1"/>
   </cols>
@@ -17142,9 +16127,9 @@
       <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="35.77734375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="35.81640625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:12">
@@ -17873,18 +16858,18 @@
   <dimension ref="A2:G64"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="0.77734375" customWidth="1"/>
+    <col min="1" max="1" width="0.81640625" customWidth="1"/>
     <col min="2" max="2" width="7" customWidth="1"/>
     <col min="3" max="3" width="12" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.81640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="86" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="63.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="63.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="30" customHeight="1">
@@ -18993,30 +17978,30 @@
   </sheetPr>
   <dimension ref="A1:AE79"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D37" sqref="D37"/>
+      <selection pane="topRight" activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="32.5546875" customWidth="1"/>
-    <col min="2" max="2" width="28.6640625" customWidth="1"/>
-    <col min="3" max="4" width="10.21875" customWidth="1"/>
-    <col min="5" max="5" width="6.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.54296875" customWidth="1"/>
+    <col min="2" max="2" width="28.6328125" customWidth="1"/>
+    <col min="3" max="4" width="10.1796875" customWidth="1"/>
+    <col min="5" max="5" width="6.1796875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8" customWidth="1"/>
-    <col min="7" max="7" width="26.77734375" style="37" customWidth="1"/>
-    <col min="8" max="8" width="0.77734375" style="17" customWidth="1"/>
-    <col min="9" max="10" width="6.21875" customWidth="1"/>
-    <col min="11" max="11" width="0.77734375" customWidth="1"/>
-    <col min="12" max="13" width="6.21875" customWidth="1"/>
-    <col min="14" max="14" width="0.77734375" customWidth="1"/>
-    <col min="15" max="15" width="7.6640625" customWidth="1"/>
-    <col min="16" max="16" width="0.77734375" customWidth="1"/>
+    <col min="7" max="7" width="26.81640625" style="37" customWidth="1"/>
+    <col min="8" max="8" width="0.81640625" style="17" customWidth="1"/>
+    <col min="9" max="10" width="6.1796875" customWidth="1"/>
+    <col min="11" max="11" width="0.81640625" customWidth="1"/>
+    <col min="12" max="13" width="6.1796875" customWidth="1"/>
+    <col min="14" max="14" width="0.81640625" customWidth="1"/>
+    <col min="15" max="15" width="7.6328125" customWidth="1"/>
+    <col min="16" max="16" width="0.81640625" customWidth="1"/>
     <col min="17" max="17" width="8" customWidth="1"/>
-    <col min="18" max="18" width="7.5546875" customWidth="1"/>
-    <col min="19" max="19" width="0.77734375" customWidth="1"/>
-    <col min="20" max="21" width="26.77734375" style="37" customWidth="1"/>
+    <col min="18" max="18" width="7.54296875" customWidth="1"/>
+    <col min="19" max="19" width="0.81640625" customWidth="1"/>
+    <col min="20" max="21" width="26.81640625" style="37" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="9" customHeight="1">
@@ -19153,7 +18138,7 @@
       <c r="AD4" s="13"/>
       <c r="AE4" s="13"/>
     </row>
-    <row r="5" spans="1:31" ht="18">
+    <row r="5" spans="1:31" ht="18.5">
       <c r="A5" s="125" t="s">
         <v>333</v>
       </c>
@@ -19193,7 +18178,7 @@
       <c r="AD5" s="13"/>
       <c r="AE5" s="13"/>
     </row>
-    <row r="6" spans="1:31" ht="18">
+    <row r="6" spans="1:31" ht="18.5">
       <c r="A6" s="125" t="s">
         <v>444</v>
       </c>
@@ -19233,7 +18218,7 @@
       <c r="AD6" s="13"/>
       <c r="AE6" s="13"/>
     </row>
-    <row r="7" spans="1:31" ht="18">
+    <row r="7" spans="1:31" ht="18.5">
       <c r="A7" s="267" t="s">
         <v>449</v>
       </c>
@@ -19303,32 +18288,32 @@
       <c r="AD8" s="13"/>
       <c r="AE8" s="13"/>
     </row>
-    <row r="9" spans="1:31" ht="18">
+    <row r="9" spans="1:31" ht="18.5">
       <c r="A9" s="76"/>
       <c r="B9" s="266"/>
-      <c r="C9" s="330" t="s">
+      <c r="C9" s="331" t="s">
         <v>80</v>
       </c>
-      <c r="D9" s="330"/>
-      <c r="E9" s="330"/>
-      <c r="F9" s="330"/>
-      <c r="G9" s="330"/>
+      <c r="D9" s="331"/>
+      <c r="E9" s="331"/>
+      <c r="F9" s="331"/>
+      <c r="G9" s="331"/>
       <c r="H9" s="28"/>
-      <c r="I9" s="330" t="s">
+      <c r="I9" s="331" t="s">
         <v>78</v>
       </c>
-      <c r="J9" s="330"/>
-      <c r="K9" s="330"/>
-      <c r="L9" s="330"/>
-      <c r="M9" s="330"/>
-      <c r="N9" s="330"/>
-      <c r="O9" s="330"/>
-      <c r="P9" s="330"/>
-      <c r="Q9" s="330"/>
-      <c r="R9" s="330"/>
-      <c r="S9" s="330"/>
-      <c r="T9" s="330"/>
-      <c r="U9" s="330"/>
+      <c r="J9" s="331"/>
+      <c r="K9" s="331"/>
+      <c r="L9" s="331"/>
+      <c r="M9" s="331"/>
+      <c r="N9" s="331"/>
+      <c r="O9" s="331"/>
+      <c r="P9" s="331"/>
+      <c r="Q9" s="331"/>
+      <c r="R9" s="331"/>
+      <c r="S9" s="331"/>
+      <c r="T9" s="331"/>
+      <c r="U9" s="331"/>
       <c r="V9" s="13"/>
       <c r="W9" s="13"/>
       <c r="X9" s="13"/>
@@ -19340,48 +18325,48 @@
       <c r="AD9" s="13"/>
       <c r="AE9" s="13"/>
     </row>
-    <row r="10" spans="1:31" ht="14.55" customHeight="1">
+    <row r="10" spans="1:31" ht="14.5" customHeight="1">
       <c r="A10" s="77"/>
       <c r="B10" s="77"/>
-      <c r="C10" s="331" t="s">
+      <c r="C10" s="332" t="s">
         <v>81</v>
       </c>
-      <c r="D10" s="331" t="s">
+      <c r="D10" s="332" t="s">
         <v>86</v>
       </c>
-      <c r="E10" s="325" t="s">
+      <c r="E10" s="326" t="s">
         <v>87</v>
       </c>
-      <c r="F10" s="325" t="s">
+      <c r="F10" s="326" t="s">
         <v>84</v>
       </c>
-      <c r="G10" s="325" t="s">
+      <c r="G10" s="326" t="s">
         <v>85</v>
       </c>
       <c r="H10" s="54"/>
-      <c r="I10" s="325" t="s">
+      <c r="I10" s="326" t="s">
         <v>81</v>
       </c>
-      <c r="J10" s="325"/>
+      <c r="J10" s="326"/>
       <c r="K10" s="257"/>
-      <c r="L10" s="325" t="s">
+      <c r="L10" s="326" t="s">
         <v>228</v>
       </c>
-      <c r="M10" s="325"/>
+      <c r="M10" s="326"/>
       <c r="N10" s="257"/>
-      <c r="O10" s="334" t="s">
+      <c r="O10" s="335" t="s">
         <v>453</v>
       </c>
       <c r="P10" s="257"/>
-      <c r="Q10" s="325" t="s">
+      <c r="Q10" s="326" t="s">
         <v>84</v>
       </c>
-      <c r="R10" s="325"/>
+      <c r="R10" s="326"/>
       <c r="S10" s="257"/>
-      <c r="T10" s="325" t="s">
+      <c r="T10" s="326" t="s">
         <v>85</v>
       </c>
-      <c r="U10" s="325"/>
+      <c r="U10" s="326"/>
       <c r="V10" s="45"/>
       <c r="W10" s="45"/>
       <c r="X10" s="45"/>
@@ -19400,11 +18385,11 @@
       <c r="B11" s="77" t="s">
         <v>156</v>
       </c>
-      <c r="C11" s="332"/>
-      <c r="D11" s="332"/>
-      <c r="E11" s="333"/>
-      <c r="F11" s="333"/>
-      <c r="G11" s="333"/>
+      <c r="C11" s="333"/>
+      <c r="D11" s="333"/>
+      <c r="E11" s="334"/>
+      <c r="F11" s="334"/>
+      <c r="G11" s="334"/>
       <c r="H11" s="29"/>
       <c r="I11" s="99">
         <v>2018</v>
@@ -19420,7 +18405,7 @@
         <v>2023</v>
       </c>
       <c r="N11" s="100"/>
-      <c r="O11" s="335"/>
+      <c r="O11" s="336"/>
       <c r="P11" s="100"/>
       <c r="Q11" s="99">
         <v>2018</v>
@@ -20446,7 +19431,7 @@
       <c r="AE30" s="13"/>
     </row>
     <row r="31" spans="1:31" ht="25.5" customHeight="1">
-      <c r="A31" s="327" t="s">
+      <c r="A31" s="328" t="s">
         <v>199</v>
       </c>
       <c r="B31" s="82" t="s">
@@ -20507,7 +19492,7 @@
       <c r="AE31" s="13"/>
     </row>
     <row r="32" spans="1:31" ht="25.5" customHeight="1">
-      <c r="A32" s="328"/>
+      <c r="A32" s="329"/>
       <c r="B32" s="82" t="s">
         <v>201</v>
       </c>
@@ -20565,7 +19550,7 @@
       <c r="AE32" s="13"/>
     </row>
     <row r="33" spans="1:31" ht="25.5" customHeight="1">
-      <c r="A33" s="329"/>
+      <c r="A33" s="330"/>
       <c r="B33" s="82" t="s">
         <v>204</v>
       </c>
@@ -20764,7 +19749,7 @@
       <c r="AD36" s="13"/>
       <c r="AE36" s="13"/>
     </row>
-    <row r="37" spans="1:31" ht="37.049999999999997" customHeight="1">
+    <row r="37" spans="1:31" ht="37" customHeight="1">
       <c r="A37" s="299" t="s">
         <v>210</v>
       </c>
@@ -21254,29 +20239,29 @@
       <c r="AE49" s="13"/>
     </row>
     <row r="50" spans="1:31" ht="15" customHeight="1">
-      <c r="A50" s="326" t="s">
+      <c r="A50" s="327" t="s">
         <v>263</v>
       </c>
-      <c r="B50" s="326"/>
-      <c r="C50" s="326"/>
-      <c r="D50" s="326"/>
-      <c r="E50" s="326"/>
-      <c r="F50" s="326"/>
-      <c r="G50" s="326"/>
-      <c r="H50" s="326"/>
-      <c r="I50" s="326"/>
-      <c r="J50" s="326"/>
-      <c r="K50" s="326"/>
-      <c r="L50" s="326"/>
-      <c r="M50" s="326"/>
-      <c r="N50" s="326"/>
-      <c r="O50" s="326"/>
-      <c r="P50" s="326"/>
-      <c r="Q50" s="326"/>
-      <c r="R50" s="326"/>
-      <c r="S50" s="326"/>
-      <c r="T50" s="326"/>
-      <c r="U50" s="326"/>
+      <c r="B50" s="327"/>
+      <c r="C50" s="327"/>
+      <c r="D50" s="327"/>
+      <c r="E50" s="327"/>
+      <c r="F50" s="327"/>
+      <c r="G50" s="327"/>
+      <c r="H50" s="327"/>
+      <c r="I50" s="327"/>
+      <c r="J50" s="327"/>
+      <c r="K50" s="327"/>
+      <c r="L50" s="327"/>
+      <c r="M50" s="327"/>
+      <c r="N50" s="327"/>
+      <c r="O50" s="327"/>
+      <c r="P50" s="327"/>
+      <c r="Q50" s="327"/>
+      <c r="R50" s="327"/>
+      <c r="S50" s="327"/>
+      <c r="T50" s="327"/>
+      <c r="U50" s="327"/>
       <c r="V50" s="68"/>
       <c r="W50" s="13"/>
       <c r="X50" s="13"/>
@@ -21289,27 +20274,27 @@
       <c r="AE50" s="13"/>
     </row>
     <row r="51" spans="1:31" ht="15" customHeight="1">
-      <c r="A51" s="326"/>
-      <c r="B51" s="326"/>
-      <c r="C51" s="326"/>
-      <c r="D51" s="326"/>
-      <c r="E51" s="326"/>
-      <c r="F51" s="326"/>
-      <c r="G51" s="326"/>
-      <c r="H51" s="326"/>
-      <c r="I51" s="326"/>
-      <c r="J51" s="326"/>
-      <c r="K51" s="326"/>
-      <c r="L51" s="326"/>
-      <c r="M51" s="326"/>
-      <c r="N51" s="326"/>
-      <c r="O51" s="326"/>
-      <c r="P51" s="326"/>
-      <c r="Q51" s="326"/>
-      <c r="R51" s="326"/>
-      <c r="S51" s="326"/>
-      <c r="T51" s="326"/>
-      <c r="U51" s="326"/>
+      <c r="A51" s="327"/>
+      <c r="B51" s="327"/>
+      <c r="C51" s="327"/>
+      <c r="D51" s="327"/>
+      <c r="E51" s="327"/>
+      <c r="F51" s="327"/>
+      <c r="G51" s="327"/>
+      <c r="H51" s="327"/>
+      <c r="I51" s="327"/>
+      <c r="J51" s="327"/>
+      <c r="K51" s="327"/>
+      <c r="L51" s="327"/>
+      <c r="M51" s="327"/>
+      <c r="N51" s="327"/>
+      <c r="O51" s="327"/>
+      <c r="P51" s="327"/>
+      <c r="Q51" s="327"/>
+      <c r="R51" s="327"/>
+      <c r="S51" s="327"/>
+      <c r="T51" s="327"/>
+      <c r="U51" s="327"/>
       <c r="V51" s="68"/>
       <c r="W51" s="13"/>
       <c r="X51" s="13"/>
@@ -21322,27 +20307,27 @@
       <c r="AE51" s="13"/>
     </row>
     <row r="52" spans="1:31" ht="15" customHeight="1">
-      <c r="A52" s="326"/>
-      <c r="B52" s="326"/>
-      <c r="C52" s="326"/>
-      <c r="D52" s="326"/>
-      <c r="E52" s="326"/>
-      <c r="F52" s="326"/>
-      <c r="G52" s="326"/>
-      <c r="H52" s="326"/>
-      <c r="I52" s="326"/>
-      <c r="J52" s="326"/>
-      <c r="K52" s="326"/>
-      <c r="L52" s="326"/>
-      <c r="M52" s="326"/>
-      <c r="N52" s="326"/>
-      <c r="O52" s="326"/>
-      <c r="P52" s="326"/>
-      <c r="Q52" s="326"/>
-      <c r="R52" s="326"/>
-      <c r="S52" s="326"/>
-      <c r="T52" s="326"/>
-      <c r="U52" s="326"/>
+      <c r="A52" s="327"/>
+      <c r="B52" s="327"/>
+      <c r="C52" s="327"/>
+      <c r="D52" s="327"/>
+      <c r="E52" s="327"/>
+      <c r="F52" s="327"/>
+      <c r="G52" s="327"/>
+      <c r="H52" s="327"/>
+      <c r="I52" s="327"/>
+      <c r="J52" s="327"/>
+      <c r="K52" s="327"/>
+      <c r="L52" s="327"/>
+      <c r="M52" s="327"/>
+      <c r="N52" s="327"/>
+      <c r="O52" s="327"/>
+      <c r="P52" s="327"/>
+      <c r="Q52" s="327"/>
+      <c r="R52" s="327"/>
+      <c r="S52" s="327"/>
+      <c r="T52" s="327"/>
+      <c r="U52" s="327"/>
       <c r="V52" s="68"/>
       <c r="W52" s="13"/>
       <c r="X52" s="13"/>
@@ -21987,7 +20972,7 @@
     <hyperlink ref="A63" r:id="rId1" xr:uid="{3D365E1F-648B-4044-B158-7612880E9167}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="40" orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId2"/>
+  <pageSetup paperSize="9" scale="34" orientation="landscape" horizontalDpi="4294967293" r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
@@ -22100,13 +21085,13 @@
   <dimension ref="A1:AM25"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I50" sqref="I50"/>
+      <selection activeCell="C4" sqref="C4:Z4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="0.77734375" customWidth="1"/>
-    <col min="2" max="2" width="27.77734375" customWidth="1"/>
+    <col min="1" max="1" width="0.81640625" customWidth="1"/>
+    <col min="2" max="2" width="27.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:39" s="13" customFormat="1">
@@ -22194,35 +21179,35 @@
     </row>
     <row r="4" spans="1:39" ht="15" customHeight="1">
       <c r="A4" s="13"/>
-      <c r="B4" s="336" t="s">
+      <c r="B4" s="337" t="s">
         <v>121</v>
       </c>
-      <c r="C4" s="338" t="s">
+      <c r="C4" s="339" t="s">
         <v>267</v>
       </c>
-      <c r="D4" s="338"/>
-      <c r="E4" s="338"/>
-      <c r="F4" s="338"/>
-      <c r="G4" s="338"/>
-      <c r="H4" s="338"/>
-      <c r="I4" s="338"/>
-      <c r="J4" s="338"/>
-      <c r="K4" s="338"/>
-      <c r="L4" s="338"/>
-      <c r="M4" s="338"/>
-      <c r="N4" s="338"/>
-      <c r="O4" s="338"/>
-      <c r="P4" s="338"/>
-      <c r="Q4" s="338"/>
-      <c r="R4" s="338"/>
-      <c r="S4" s="338"/>
-      <c r="T4" s="338"/>
-      <c r="U4" s="338"/>
-      <c r="V4" s="338"/>
-      <c r="W4" s="338"/>
-      <c r="X4" s="338"/>
-      <c r="Y4" s="338"/>
-      <c r="Z4" s="338"/>
+      <c r="D4" s="339"/>
+      <c r="E4" s="339"/>
+      <c r="F4" s="339"/>
+      <c r="G4" s="339"/>
+      <c r="H4" s="339"/>
+      <c r="I4" s="339"/>
+      <c r="J4" s="339"/>
+      <c r="K4" s="339"/>
+      <c r="L4" s="339"/>
+      <c r="M4" s="339"/>
+      <c r="N4" s="339"/>
+      <c r="O4" s="339"/>
+      <c r="P4" s="339"/>
+      <c r="Q4" s="339"/>
+      <c r="R4" s="339"/>
+      <c r="S4" s="339"/>
+      <c r="T4" s="339"/>
+      <c r="U4" s="339"/>
+      <c r="V4" s="339"/>
+      <c r="W4" s="339"/>
+      <c r="X4" s="339"/>
+      <c r="Y4" s="339"/>
+      <c r="Z4" s="339"/>
       <c r="AA4" s="13"/>
       <c r="AB4" s="13"/>
       <c r="AC4" s="13"/>
@@ -22239,7 +21224,7 @@
     </row>
     <row r="5" spans="1:39">
       <c r="A5" s="13"/>
-      <c r="B5" s="337"/>
+      <c r="B5" s="338"/>
       <c r="C5" s="75" t="s">
         <v>127</v>
       </c>
@@ -23194,7 +22179,7 @@
         <v>6.8542512999999996</v>
       </c>
     </row>
-    <row r="20" spans="2:26" ht="21.6">
+    <row r="20" spans="2:26" ht="22">
       <c r="B20" s="22" t="s">
         <v>257</v>
       </c>
@@ -23532,30 +22517,30 @@
       </c>
     </row>
     <row r="25" spans="2:26">
-      <c r="B25" s="339" t="s">
+      <c r="B25" s="340" t="s">
         <v>149</v>
       </c>
-      <c r="C25" s="339"/>
-      <c r="D25" s="339"/>
-      <c r="E25" s="339"/>
-      <c r="F25" s="339"/>
-      <c r="G25" s="339"/>
-      <c r="H25" s="339"/>
-      <c r="I25" s="339"/>
-      <c r="J25" s="339"/>
-      <c r="K25" s="339"/>
-      <c r="L25" s="339"/>
-      <c r="M25" s="339"/>
-      <c r="N25" s="339"/>
-      <c r="O25" s="339"/>
-      <c r="P25" s="339"/>
-      <c r="Q25" s="339"/>
-      <c r="R25" s="339"/>
-      <c r="S25" s="339"/>
-      <c r="T25" s="339"/>
-      <c r="U25" s="339"/>
-      <c r="V25" s="339"/>
-      <c r="W25" s="339"/>
+      <c r="C25" s="340"/>
+      <c r="D25" s="340"/>
+      <c r="E25" s="340"/>
+      <c r="F25" s="340"/>
+      <c r="G25" s="340"/>
+      <c r="H25" s="340"/>
+      <c r="I25" s="340"/>
+      <c r="J25" s="340"/>
+      <c r="K25" s="340"/>
+      <c r="L25" s="340"/>
+      <c r="M25" s="340"/>
+      <c r="N25" s="340"/>
+      <c r="O25" s="340"/>
+      <c r="P25" s="340"/>
+      <c r="Q25" s="340"/>
+      <c r="R25" s="340"/>
+      <c r="S25" s="340"/>
+      <c r="T25" s="340"/>
+      <c r="U25" s="340"/>
+      <c r="V25" s="340"/>
+      <c r="W25" s="340"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -23579,10 +22564,10 @@
       <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="17" max="17" width="7.5546875" customWidth="1"/>
-    <col min="18" max="25" width="9.21875" style="13"/>
+    <col min="17" max="17" width="7.54296875" customWidth="1"/>
+    <col min="18" max="25" width="9.1796875" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24">
@@ -23698,9 +22683,9 @@
       <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="35.77734375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="35.81640625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:12">
@@ -23739,11 +22724,9 @@
         <v>1</v>
       </c>
       <c r="C3" s="50">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!L$1:L$101,MATCH([1]UHC_Inter!$A3,[1]UHC_summary!$B$1:$B$101,0))=0,INDEX([1]UHC_summary!I$1:I$101,MATCH([1]UHC_Inter!$A3,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!L$1:L$101,MATCH([1]UHC_Inter!$A3,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>56.35</v>
       </c>
       <c r="D3" s="50">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!M$1:M$101,MATCH([1]UHC_Inter!$A3,[1]UHC_summary!$B$1:$B$101,0))=0,INDEX([1]UHC_summary!J$1:J$101,MATCH([1]UHC_Inter!$A3,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!M$1:M$101,MATCH([1]UHC_Inter!$A3,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>60.55</v>
       </c>
       <c r="E3" s="50">
@@ -23763,16 +22746,13 @@
         <v>#N/A</v>
       </c>
       <c r="I3" s="50">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!D$1:D$101,MATCH([1]UHC_Inter!$A3,[1]UHC_summary!$B$1:$B$101,0))="",INDEX([1]UHC_summary!C$1:C$101,MATCH([1]UHC_Inter!$A3,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!D$1:D$101,MATCH([1]UHC_Inter!$A3,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>57.99</v>
       </c>
       <c r="J3" s="198">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!E$1:E$101,MATCH([1]UHC_Inter!$A3,[1]UHC_summary!$B$1:$B$101,0))=0,"",INDEX([1]UHC_summary!E$1:E$101,MATCH([1]UHC_Inter!$A3,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>2020</v>
       </c>
-      <c r="K3" t="str">
-        <f>INDEX([1]UHC_summary!D$1:D$101,MATCH([1]UHC_Inter!$A3,[1]UHC_summary!$B$1:$B$101,0))</f>
-        <v/>
+      <c r="K3" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -23783,11 +22763,9 @@
         <v>2</v>
       </c>
       <c r="C4" s="50">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!L$1:L$101,MATCH([1]UHC_Inter!$A4,[1]UHC_summary!$B$1:$B$101,0))=0,INDEX([1]UHC_summary!I$1:I$101,MATCH([1]UHC_Inter!$A4,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!L$1:L$101,MATCH([1]UHC_Inter!$A4,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>98.58</v>
       </c>
       <c r="D4" s="50">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!M$1:M$101,MATCH([1]UHC_Inter!$A4,[1]UHC_summary!$B$1:$B$101,0))=0,INDEX([1]UHC_summary!J$1:J$101,MATCH([1]UHC_Inter!$A4,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!M$1:M$101,MATCH([1]UHC_Inter!$A4,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>98.46</v>
       </c>
       <c r="E4" s="50" t="e">
@@ -23807,12 +22785,10 @@
         <v>0.12000000000000455</v>
       </c>
       <c r="I4" s="50">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!D$1:D$101,MATCH([1]UHC_Inter!$A4,[1]UHC_summary!$B$1:$B$101,0))="",INDEX([1]UHC_summary!C$1:C$101,MATCH([1]UHC_Inter!$A4,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!D$1:D$101,MATCH([1]UHC_Inter!$A4,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>0</v>
       </c>
-      <c r="J4" s="198" t="str">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!E$1:E$101,MATCH([1]UHC_Inter!$A4,[1]UHC_summary!$B$1:$B$101,0))=0,"",INDEX([1]UHC_summary!E$1:E$101,MATCH([1]UHC_Inter!$A4,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
-        <v/>
+      <c r="J4" s="198" t="s">
+        <v>82</v>
       </c>
       <c r="L4" s="21"/>
     </row>
@@ -23824,11 +22800,9 @@
         <v>3</v>
       </c>
       <c r="C5" s="50">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!L$1:L$101,MATCH([1]UHC_Inter!$A5,[1]UHC_summary!$B$1:$B$101,0))=0,INDEX([1]UHC_summary!I$1:I$101,MATCH([1]UHC_Inter!$A5,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!L$1:L$101,MATCH([1]UHC_Inter!$A5,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>98</v>
       </c>
       <c r="D5" s="50">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!M$1:M$101,MATCH([1]UHC_Inter!$A5,[1]UHC_summary!$B$1:$B$101,0))=0,INDEX([1]UHC_summary!J$1:J$101,MATCH([1]UHC_Inter!$A5,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!M$1:M$101,MATCH([1]UHC_Inter!$A5,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>98.54</v>
       </c>
       <c r="E5" s="50">
@@ -23848,11 +22822,9 @@
         <v>#N/A</v>
       </c>
       <c r="I5" s="50">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!D$1:D$101,MATCH([1]UHC_Inter!$A5,[1]UHC_summary!$B$1:$B$101,0))="",INDEX([1]UHC_summary!C$1:C$101,MATCH([1]UHC_Inter!$A5,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!D$1:D$101,MATCH([1]UHC_Inter!$A5,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>98</v>
       </c>
       <c r="J5" s="198">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!E$1:E$101,MATCH([1]UHC_Inter!$A5,[1]UHC_summary!$B$1:$B$101,0))=0,"",INDEX([1]UHC_summary!E$1:E$101,MATCH([1]UHC_Inter!$A5,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>2019</v>
       </c>
     </row>
@@ -23864,11 +22836,9 @@
         <v>4</v>
       </c>
       <c r="C6" s="50">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!L$1:L$101,MATCH([1]UHC_Inter!$A6,[1]UHC_summary!$B$1:$B$101,0))=0,INDEX([1]UHC_summary!I$1:I$101,MATCH([1]UHC_Inter!$A6,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!L$1:L$101,MATCH([1]UHC_Inter!$A6,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>89.91</v>
       </c>
       <c r="D6" s="50">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!M$1:M$101,MATCH([1]UHC_Inter!$A6,[1]UHC_summary!$B$1:$B$101,0))=0,INDEX([1]UHC_summary!J$1:J$101,MATCH([1]UHC_Inter!$A6,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!M$1:M$101,MATCH([1]UHC_Inter!$A6,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>90.82</v>
       </c>
       <c r="E6" s="50">
@@ -23888,12 +22858,10 @@
         <v>#N/A</v>
       </c>
       <c r="I6" s="50">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!D$1:D$101,MATCH([1]UHC_Inter!$A6,[1]UHC_summary!$B$1:$B$101,0))="",INDEX([1]UHC_summary!C$1:C$101,MATCH([1]UHC_Inter!$A6,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!D$1:D$101,MATCH([1]UHC_Inter!$A6,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>0</v>
       </c>
-      <c r="J6" s="198" t="str">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!E$1:E$101,MATCH([1]UHC_Inter!$A6,[1]UHC_summary!$B$1:$B$101,0))=0,"",INDEX([1]UHC_summary!E$1:E$101,MATCH([1]UHC_Inter!$A6,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
-        <v/>
+      <c r="J6" s="198" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -23904,11 +22872,9 @@
         <v>5</v>
       </c>
       <c r="C7" s="50">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!L$1:L$101,MATCH([1]UHC_Inter!$A7,[1]UHC_summary!$B$1:$B$101,0))=0,INDEX([1]UHC_summary!I$1:I$101,MATCH([1]UHC_Inter!$A7,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!L$1:L$101,MATCH([1]UHC_Inter!$A7,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>86.96</v>
       </c>
       <c r="D7" s="50">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!M$1:M$101,MATCH([1]UHC_Inter!$A7,[1]UHC_summary!$B$1:$B$101,0))=0,INDEX([1]UHC_summary!J$1:J$101,MATCH([1]UHC_Inter!$A7,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!M$1:M$101,MATCH([1]UHC_Inter!$A7,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>86.96</v>
       </c>
       <c r="E7" s="50" t="e">
@@ -23928,11 +22894,9 @@
         <v>#N/A</v>
       </c>
       <c r="I7" s="50">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!D$1:D$101,MATCH([1]UHC_Inter!$A7,[1]UHC_summary!$B$1:$B$101,0))="",INDEX([1]UHC_summary!C$1:C$101,MATCH([1]UHC_Inter!$A7,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!D$1:D$101,MATCH([1]UHC_Inter!$A7,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>86.96</v>
       </c>
       <c r="J7" s="198">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!E$1:E$101,MATCH([1]UHC_Inter!$A7,[1]UHC_summary!$B$1:$B$101,0))=0,"",INDEX([1]UHC_summary!E$1:E$101,MATCH([1]UHC_Inter!$A7,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>2019</v>
       </c>
     </row>
@@ -23943,13 +22907,11 @@
       <c r="B8" s="49">
         <v>6</v>
       </c>
-      <c r="C8" s="50" t="str">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!L$1:L$101,MATCH([1]UHC_Inter!$A8,[1]UHC_summary!$B$1:$B$101,0))=0,INDEX([1]UHC_summary!I$1:I$101,MATCH([1]UHC_Inter!$A8,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!L$1:L$101,MATCH([1]UHC_Inter!$A8,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
-        <v/>
-      </c>
-      <c r="D8" s="50" t="str">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!M$1:M$101,MATCH([1]UHC_Inter!$A8,[1]UHC_summary!$B$1:$B$101,0))=0,INDEX([1]UHC_summary!J$1:J$101,MATCH([1]UHC_Inter!$A8,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!M$1:M$101,MATCH([1]UHC_Inter!$A8,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
-        <v/>
+      <c r="C8" s="50" t="s">
+        <v>82</v>
+      </c>
+      <c r="D8" s="50" t="s">
+        <v>82</v>
       </c>
       <c r="E8" s="50" t="e">
         <f t="shared" si="0"/>
@@ -23967,13 +22929,11 @@
         <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
-      <c r="I8" s="50" t="str">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!D$1:D$101,MATCH([1]UHC_Inter!$A8,[1]UHC_summary!$B$1:$B$101,0))="",INDEX([1]UHC_summary!C$1:C$101,MATCH([1]UHC_Inter!$A8,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!D$1:D$101,MATCH([1]UHC_Inter!$A8,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
-        <v/>
-      </c>
-      <c r="J8" s="198" t="str">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!E$1:E$101,MATCH([1]UHC_Inter!$A8,[1]UHC_summary!$B$1:$B$101,0))=0,"",INDEX([1]UHC_summary!E$1:E$101,MATCH([1]UHC_Inter!$A8,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
-        <v/>
+      <c r="I8" s="50" t="s">
+        <v>82</v>
+      </c>
+      <c r="J8" s="198" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -23984,11 +22944,9 @@
         <v>7</v>
       </c>
       <c r="C9" s="50">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!L$1:L$101,MATCH([1]UHC_Inter!$A9,[1]UHC_summary!$B$1:$B$101,0))=0,INDEX([1]UHC_summary!I$1:I$101,MATCH([1]UHC_Inter!$A9,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!L$1:L$101,MATCH([1]UHC_Inter!$A9,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>99.9</v>
       </c>
       <c r="D9" s="50">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!M$1:M$101,MATCH([1]UHC_Inter!$A9,[1]UHC_summary!$B$1:$B$101,0))=0,INDEX([1]UHC_summary!J$1:J$101,MATCH([1]UHC_Inter!$A9,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!M$1:M$101,MATCH([1]UHC_Inter!$A9,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>99.9</v>
       </c>
       <c r="E9" s="50" t="e">
@@ -24008,11 +22966,9 @@
         <v>#N/A</v>
       </c>
       <c r="I9" s="50">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!D$1:D$101,MATCH([1]UHC_Inter!$A9,[1]UHC_summary!$B$1:$B$101,0))="",INDEX([1]UHC_summary!C$1:C$101,MATCH([1]UHC_Inter!$A9,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!D$1:D$101,MATCH([1]UHC_Inter!$A9,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>99.89</v>
       </c>
       <c r="J9" s="198">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!E$1:E$101,MATCH([1]UHC_Inter!$A9,[1]UHC_summary!$B$1:$B$101,0))=0,"",INDEX([1]UHC_summary!E$1:E$101,MATCH([1]UHC_Inter!$A9,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>2017</v>
       </c>
     </row>
@@ -24024,11 +22980,9 @@
         <v>8</v>
       </c>
       <c r="C10" s="50">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!L$1:L$101,MATCH([1]UHC_Inter!$A10,[1]UHC_summary!$B$1:$B$101,0))=0,INDEX([1]UHC_summary!I$1:I$101,MATCH([1]UHC_Inter!$A10,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!L$1:L$101,MATCH([1]UHC_Inter!$A10,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>16.68</v>
       </c>
       <c r="D10" s="50">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!M$1:M$101,MATCH([1]UHC_Inter!$A10,[1]UHC_summary!$B$1:$B$101,0))=0,INDEX([1]UHC_summary!J$1:J$101,MATCH([1]UHC_Inter!$A10,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!M$1:M$101,MATCH([1]UHC_Inter!$A10,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>15.29</v>
       </c>
       <c r="E10" s="50" t="e">
@@ -24048,11 +23002,9 @@
         <v>1.3900000000000006</v>
       </c>
       <c r="I10" s="50">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!D$1:D$101,MATCH([1]UHC_Inter!$A10,[1]UHC_summary!$B$1:$B$101,0))="",INDEX([1]UHC_summary!C$1:C$101,MATCH([1]UHC_Inter!$A10,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!D$1:D$101,MATCH([1]UHC_Inter!$A10,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>17.55</v>
       </c>
       <c r="J10" s="198">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!E$1:E$101,MATCH([1]UHC_Inter!$A10,[1]UHC_summary!$B$1:$B$101,0))=0,"",INDEX([1]UHC_summary!E$1:E$101,MATCH([1]UHC_Inter!$A10,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>2015</v>
       </c>
     </row>
@@ -24064,11 +23016,9 @@
         <v>9</v>
       </c>
       <c r="C11" s="50">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!L$1:L$101,MATCH([1]UHC_Inter!$A11,[1]UHC_summary!$B$1:$B$101,0))=0,INDEX([1]UHC_summary!I$1:I$101,MATCH([1]UHC_Inter!$A11,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!L$1:L$101,MATCH([1]UHC_Inter!$A11,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>5.12</v>
       </c>
       <c r="D11" s="50">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!M$1:M$101,MATCH([1]UHC_Inter!$A11,[1]UHC_summary!$B$1:$B$101,0))=0,INDEX([1]UHC_summary!J$1:J$101,MATCH([1]UHC_Inter!$A11,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!M$1:M$101,MATCH([1]UHC_Inter!$A11,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>5.03</v>
       </c>
       <c r="E11" s="50" t="e">
@@ -24088,11 +23038,9 @@
         <v>8.9999999999999858E-2</v>
       </c>
       <c r="I11" s="50">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!D$1:D$101,MATCH([1]UHC_Inter!$A11,[1]UHC_summary!$B$1:$B$101,0))="",INDEX([1]UHC_summary!C$1:C$101,MATCH([1]UHC_Inter!$A11,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!D$1:D$101,MATCH([1]UHC_Inter!$A11,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>5.2</v>
       </c>
       <c r="J11" s="198">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!E$1:E$101,MATCH([1]UHC_Inter!$A11,[1]UHC_summary!$B$1:$B$101,0))=0,"",INDEX([1]UHC_summary!E$1:E$101,MATCH([1]UHC_Inter!$A11,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>2014</v>
       </c>
     </row>
@@ -24104,11 +23052,9 @@
         <v>10</v>
       </c>
       <c r="C12" s="50">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!L$1:L$101,MATCH([1]UHC_Inter!$A12,[1]UHC_summary!$B$1:$B$101,0))=0,INDEX([1]UHC_summary!I$1:I$101,MATCH([1]UHC_Inter!$A12,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!L$1:L$101,MATCH([1]UHC_Inter!$A12,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>21.9</v>
       </c>
       <c r="D12" s="50">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!M$1:M$101,MATCH([1]UHC_Inter!$A12,[1]UHC_summary!$B$1:$B$101,0))=0,INDEX([1]UHC_summary!J$1:J$101,MATCH([1]UHC_Inter!$A12,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!M$1:M$101,MATCH([1]UHC_Inter!$A12,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>19.5</v>
       </c>
       <c r="E12" s="50" t="e">
@@ -24128,11 +23074,9 @@
         <v>2.3999999999999986</v>
       </c>
       <c r="I12" s="50">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!D$1:D$101,MATCH([1]UHC_Inter!$A12,[1]UHC_summary!$B$1:$B$101,0))="",INDEX([1]UHC_summary!C$1:C$101,MATCH([1]UHC_Inter!$A12,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!D$1:D$101,MATCH([1]UHC_Inter!$A12,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>21.9</v>
       </c>
       <c r="J12" s="198">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!E$1:E$101,MATCH([1]UHC_Inter!$A12,[1]UHC_summary!$B$1:$B$101,0))=0,"",INDEX([1]UHC_summary!E$1:E$101,MATCH([1]UHC_Inter!$A12,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>2018</v>
       </c>
     </row>
@@ -24144,11 +23088,9 @@
         <v>11</v>
       </c>
       <c r="C13" s="50">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!L$1:L$101,MATCH([1]UHC_Inter!$A13,[1]UHC_summary!$B$1:$B$101,0))=0,INDEX([1]UHC_summary!I$1:I$101,MATCH([1]UHC_Inter!$A13,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!L$1:L$101,MATCH([1]UHC_Inter!$A13,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>129.04</v>
       </c>
       <c r="D13" s="50">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!M$1:M$101,MATCH([1]UHC_Inter!$A13,[1]UHC_summary!$B$1:$B$101,0))=0,INDEX([1]UHC_summary!J$1:J$101,MATCH([1]UHC_Inter!$A13,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!M$1:M$101,MATCH([1]UHC_Inter!$A13,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>130.5</v>
       </c>
       <c r="E13" s="50">
@@ -24168,11 +23110,9 @@
         <v>#N/A</v>
       </c>
       <c r="I13" s="50">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!D$1:D$101,MATCH([1]UHC_Inter!$A13,[1]UHC_summary!$B$1:$B$101,0))="",INDEX([1]UHC_summary!C$1:C$101,MATCH([1]UHC_Inter!$A13,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!D$1:D$101,MATCH([1]UHC_Inter!$A13,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>129.04</v>
       </c>
       <c r="J13" s="198">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!E$1:E$101,MATCH([1]UHC_Inter!$A13,[1]UHC_summary!$B$1:$B$101,0))=0,"",INDEX([1]UHC_summary!E$1:E$101,MATCH([1]UHC_Inter!$A13,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>2018</v>
       </c>
     </row>
@@ -24184,11 +23124,9 @@
         <v>12</v>
       </c>
       <c r="C14" s="50">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!L$1:L$101,MATCH([1]UHC_Inter!$A14,[1]UHC_summary!$B$1:$B$101,0))=0,INDEX([1]UHC_summary!I$1:I$101,MATCH([1]UHC_Inter!$A14,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!L$1:L$101,MATCH([1]UHC_Inter!$A14,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>151.77000000000001</v>
       </c>
       <c r="D14" s="50">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!M$1:M$101,MATCH([1]UHC_Inter!$A14,[1]UHC_summary!$B$1:$B$101,0))=0,INDEX([1]UHC_summary!J$1:J$101,MATCH([1]UHC_Inter!$A14,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!M$1:M$101,MATCH([1]UHC_Inter!$A14,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>172.69</v>
       </c>
       <c r="E14" s="50">
@@ -24208,11 +23146,9 @@
         <v>#N/A</v>
       </c>
       <c r="I14" s="50">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!D$1:D$101,MATCH([1]UHC_Inter!$A14,[1]UHC_summary!$B$1:$B$101,0))="",INDEX([1]UHC_summary!C$1:C$101,MATCH([1]UHC_Inter!$A14,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!D$1:D$101,MATCH([1]UHC_Inter!$A14,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>151.77000000000001</v>
       </c>
       <c r="J14" s="198">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!E$1:E$101,MATCH([1]UHC_Inter!$A14,[1]UHC_summary!$B$1:$B$101,0))=0,"",INDEX([1]UHC_summary!E$1:E$101,MATCH([1]UHC_Inter!$A14,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>2018</v>
       </c>
     </row>
@@ -24224,11 +23160,9 @@
         <v>13</v>
       </c>
       <c r="C15" s="50">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!L$1:L$101,MATCH([1]UHC_Inter!$A15,[1]UHC_summary!$B$1:$B$101,0))=0,INDEX([1]UHC_summary!I$1:I$101,MATCH([1]UHC_Inter!$A15,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!L$1:L$101,MATCH([1]UHC_Inter!$A15,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>95</v>
       </c>
       <c r="D15" s="50">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!M$1:M$101,MATCH([1]UHC_Inter!$A15,[1]UHC_summary!$B$1:$B$101,0))=0,INDEX([1]UHC_summary!J$1:J$101,MATCH([1]UHC_Inter!$A15,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!M$1:M$101,MATCH([1]UHC_Inter!$A15,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>94.99</v>
       </c>
       <c r="E15" s="50" t="e">
@@ -24248,11 +23182,9 @@
         <v>1.0000000000005116E-2</v>
       </c>
       <c r="I15" s="50">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!D$1:D$101,MATCH([1]UHC_Inter!$A15,[1]UHC_summary!$B$1:$B$101,0))="",INDEX([1]UHC_summary!C$1:C$101,MATCH([1]UHC_Inter!$A15,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!D$1:D$101,MATCH([1]UHC_Inter!$A15,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>95</v>
       </c>
       <c r="J15" s="198">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!E$1:E$101,MATCH([1]UHC_Inter!$A15,[1]UHC_summary!$B$1:$B$101,0))=0,"",INDEX([1]UHC_summary!E$1:E$101,MATCH([1]UHC_Inter!$A15,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>2020</v>
       </c>
     </row>
@@ -24261,13 +23193,11 @@
       <c r="B16" s="49">
         <v>14</v>
       </c>
-      <c r="C16" s="50" t="str">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!L$1:L$101,MATCH([1]UHC_Inter!$A16,[1]UHC_summary!$B$1:$B$101,0))=0,INDEX([1]UHC_summary!I$1:I$101,MATCH([1]UHC_Inter!$A16,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!L$1:L$101,MATCH([1]UHC_Inter!$A16,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
-        <v/>
-      </c>
-      <c r="D16" s="50" t="str">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!M$1:M$101,MATCH([1]UHC_Inter!$A16,[1]UHC_summary!$B$1:$B$101,0))=0,INDEX([1]UHC_summary!J$1:J$101,MATCH([1]UHC_Inter!$A16,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!M$1:M$101,MATCH([1]UHC_Inter!$A16,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
-        <v/>
+      <c r="C16" s="50" t="s">
+        <v>82</v>
+      </c>
+      <c r="D16" s="50" t="s">
+        <v>82</v>
       </c>
       <c r="E16" s="50" t="e">
         <f t="shared" si="0"/>
@@ -24285,13 +23215,11 @@
         <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
-      <c r="I16" s="50" t="str">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!D$1:D$101,MATCH([1]UHC_Inter!$A16,[1]UHC_summary!$B$1:$B$101,0))="",INDEX([1]UHC_summary!C$1:C$101,MATCH([1]UHC_Inter!$A16,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!D$1:D$101,MATCH([1]UHC_Inter!$A16,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
-        <v/>
-      </c>
-      <c r="J16" s="198" t="str">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!E$1:E$101,MATCH([1]UHC_Inter!$A16,[1]UHC_summary!$B$1:$B$101,0))=0,"",INDEX([1]UHC_summary!E$1:E$101,MATCH([1]UHC_Inter!$A16,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
-        <v/>
+      <c r="I16" s="50" t="s">
+        <v>82</v>
+      </c>
+      <c r="J16" s="198" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -24398,35 +23326,35 @@
   <dimension ref="A1:AE83"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="12" topLeftCell="C31" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="12" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B26" sqref="B26"/>
       <selection pane="topRight" activeCell="B26" sqref="B26"/>
       <selection pane="bottomLeft" activeCell="B26" sqref="B26"/>
-      <selection pane="bottomRight" activeCell="B37" sqref="B37"/>
+      <selection pane="bottomRight" activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" customWidth="1"/>
-    <col min="2" max="2" width="28.21875" customWidth="1"/>
-    <col min="3" max="3" width="7.77734375" customWidth="1"/>
-    <col min="4" max="4" width="7.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.453125" customWidth="1"/>
+    <col min="2" max="2" width="28.1796875" customWidth="1"/>
+    <col min="3" max="3" width="7.81640625" customWidth="1"/>
+    <col min="4" max="4" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.453125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.77734375" customWidth="1"/>
-    <col min="8" max="8" width="0.77734375" style="17" customWidth="1"/>
-    <col min="9" max="10" width="6.21875" customWidth="1"/>
-    <col min="11" max="11" width="0.77734375" customWidth="1"/>
-    <col min="12" max="13" width="4.77734375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="0.77734375" customWidth="1"/>
+    <col min="7" max="7" width="26.81640625" customWidth="1"/>
+    <col min="8" max="8" width="0.81640625" style="17" customWidth="1"/>
+    <col min="9" max="10" width="6.1796875" customWidth="1"/>
+    <col min="11" max="11" width="0.81640625" customWidth="1"/>
+    <col min="12" max="13" width="4.81640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="0.81640625" customWidth="1"/>
     <col min="15" max="15" width="8" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.77734375" customWidth="1"/>
-    <col min="17" max="17" width="0.77734375" customWidth="1"/>
-    <col min="18" max="18" width="26.77734375" customWidth="1"/>
-    <col min="19" max="19" width="32.21875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="26.77734375" style="13" customWidth="1"/>
-    <col min="21" max="21" width="48.5546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="22" max="24" width="11.44140625" style="13"/>
+    <col min="16" max="16" width="10.81640625" customWidth="1"/>
+    <col min="17" max="17" width="0.81640625" customWidth="1"/>
+    <col min="18" max="18" width="26.81640625" customWidth="1"/>
+    <col min="19" max="19" width="32.1796875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="26.81640625" style="13" customWidth="1"/>
+    <col min="21" max="21" width="48.54296875" style="13" bestFit="1" customWidth="1"/>
+    <col min="22" max="24" width="11.453125" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="9" customHeight="1">
@@ -24566,11 +23494,11 @@
         <f>F47/1000</f>
         <v>0</v>
       </c>
-      <c r="H5" s="344" t="s">
+      <c r="H5" s="345" t="s">
         <v>152</v>
       </c>
-      <c r="I5" s="345"/>
-      <c r="J5" s="345"/>
+      <c r="I5" s="346"/>
+      <c r="J5" s="346"/>
       <c r="K5" s="13"/>
       <c r="L5" s="13"/>
       <c r="M5" s="13"/>
@@ -24606,11 +23534,11 @@
         <f>F48</f>
         <v>0</v>
       </c>
-      <c r="H6" s="344" t="s">
+      <c r="H6" s="345" t="s">
         <v>46</v>
       </c>
-      <c r="I6" s="345"/>
-      <c r="J6" s="345"/>
+      <c r="I6" s="346"/>
+      <c r="J6" s="346"/>
       <c r="K6" s="13"/>
       <c r="L6" s="13"/>
       <c r="M6" s="13"/>
@@ -24646,11 +23574,11 @@
         <f>F49/1000</f>
         <v>0</v>
       </c>
-      <c r="H7" s="344" t="s">
+      <c r="H7" s="345" t="s">
         <v>152</v>
       </c>
-      <c r="I7" s="345"/>
-      <c r="J7" s="345"/>
+      <c r="I7" s="346"/>
+      <c r="J7" s="346"/>
       <c r="K7" s="66"/>
       <c r="L7" s="66"/>
       <c r="M7" s="66"/>
@@ -24707,31 +23635,31 @@
       <c r="AE8" s="13"/>
     </row>
     <row r="9" spans="1:31" ht="15" customHeight="1">
-      <c r="A9" s="347" t="s">
+      <c r="A9" s="348" t="s">
         <v>77</v>
       </c>
-      <c r="B9" s="347"/>
-      <c r="C9" s="343" t="s">
+      <c r="B9" s="348"/>
+      <c r="C9" s="344" t="s">
         <v>80</v>
       </c>
-      <c r="D9" s="343"/>
-      <c r="E9" s="343"/>
-      <c r="F9" s="343"/>
-      <c r="G9" s="343"/>
+      <c r="D9" s="344"/>
+      <c r="E9" s="344"/>
+      <c r="F9" s="344"/>
+      <c r="G9" s="344"/>
       <c r="H9" s="156"/>
-      <c r="I9" s="346" t="s">
+      <c r="I9" s="347" t="s">
         <v>153</v>
       </c>
-      <c r="J9" s="346"/>
-      <c r="K9" s="346"/>
-      <c r="L9" s="346"/>
-      <c r="M9" s="346"/>
-      <c r="N9" s="346"/>
-      <c r="O9" s="346"/>
-      <c r="P9" s="346"/>
-      <c r="Q9" s="346"/>
-      <c r="R9" s="346"/>
-      <c r="S9" s="346"/>
+      <c r="J9" s="347"/>
+      <c r="K9" s="347"/>
+      <c r="L9" s="347"/>
+      <c r="M9" s="347"/>
+      <c r="N9" s="347"/>
+      <c r="O9" s="347"/>
+      <c r="P9" s="347"/>
+      <c r="Q9" s="347"/>
+      <c r="R9" s="347"/>
+      <c r="S9" s="347"/>
       <c r="T9" s="115"/>
       <c r="U9" s="115"/>
       <c r="V9" s="115"/>
@@ -24746,47 +23674,47 @@
       <c r="AE9" s="13"/>
     </row>
     <row r="10" spans="1:31">
-      <c r="A10" s="341" t="s">
+      <c r="A10" s="342" t="s">
         <v>121</v>
       </c>
-      <c r="B10" s="341" t="s">
+      <c r="B10" s="342" t="s">
         <v>270</v>
       </c>
-      <c r="C10" s="342" t="s">
+      <c r="C10" s="343" t="s">
         <v>268</v>
       </c>
-      <c r="D10" s="341" t="s">
+      <c r="D10" s="342" t="s">
         <v>269</v>
       </c>
-      <c r="E10" s="342" t="s">
+      <c r="E10" s="343" t="s">
         <v>87</v>
       </c>
-      <c r="F10" s="342" t="s">
+      <c r="F10" s="343" t="s">
         <v>84</v>
       </c>
-      <c r="G10" s="341" t="s">
+      <c r="G10" s="342" t="s">
         <v>154</v>
       </c>
       <c r="H10" s="127"/>
-      <c r="I10" s="340" t="s">
+      <c r="I10" s="341" t="s">
         <v>268</v>
       </c>
-      <c r="J10" s="340"/>
+      <c r="J10" s="341"/>
       <c r="K10" s="132"/>
-      <c r="L10" s="340" t="s">
+      <c r="L10" s="341" t="s">
         <v>269</v>
       </c>
-      <c r="M10" s="340"/>
+      <c r="M10" s="341"/>
       <c r="N10" s="132"/>
-      <c r="O10" s="340" t="s">
+      <c r="O10" s="341" t="s">
         <v>84</v>
       </c>
-      <c r="P10" s="340"/>
+      <c r="P10" s="341"/>
       <c r="Q10" s="132"/>
-      <c r="R10" s="340" t="s">
+      <c r="R10" s="341" t="s">
         <v>85</v>
       </c>
-      <c r="S10" s="340"/>
+      <c r="S10" s="341"/>
       <c r="Y10" s="13"/>
       <c r="Z10" s="13"/>
       <c r="AA10" s="13"/>
@@ -24796,13 +23724,13 @@
       <c r="AE10" s="13"/>
     </row>
     <row r="11" spans="1:31">
-      <c r="A11" s="341"/>
-      <c r="B11" s="341"/>
-      <c r="C11" s="342"/>
-      <c r="D11" s="341"/>
-      <c r="E11" s="342"/>
-      <c r="F11" s="342"/>
-      <c r="G11" s="341"/>
+      <c r="A11" s="342"/>
+      <c r="B11" s="342"/>
+      <c r="C11" s="343"/>
+      <c r="D11" s="342"/>
+      <c r="E11" s="343"/>
+      <c r="F11" s="343"/>
+      <c r="G11" s="342"/>
       <c r="H11" s="127"/>
       <c r="I11" s="131">
         <v>2018</v>
@@ -24936,7 +23864,7 @@
       <c r="AD13" s="13"/>
       <c r="AE13" s="13"/>
     </row>
-    <row r="14" spans="1:31" ht="30.6">
+    <row r="14" spans="1:31" ht="31.5">
       <c r="A14" s="140" t="s">
         <v>302</v>
       </c>
@@ -24997,7 +23925,7 @@
       <c r="AD14" s="13"/>
       <c r="AE14" s="13"/>
     </row>
-    <row r="15" spans="1:31" ht="30.6">
+    <row r="15" spans="1:31" ht="31.5">
       <c r="A15" s="140" t="s">
         <v>304</v>
       </c>
@@ -25302,7 +24230,7 @@
       <c r="AD19" s="13"/>
       <c r="AE19" s="13"/>
     </row>
-    <row r="20" spans="1:31" ht="20.399999999999999">
+    <row r="20" spans="1:31" ht="21">
       <c r="A20" s="140" t="s">
         <v>309</v>
       </c>
@@ -25363,7 +24291,7 @@
       <c r="AD20" s="13"/>
       <c r="AE20" s="13"/>
     </row>
-    <row r="21" spans="1:31" ht="20.399999999999999">
+    <row r="21" spans="1:31" ht="21">
       <c r="A21" s="140" t="s">
         <v>310</v>
       </c>
@@ -26227,7 +25155,7 @@
       <c r="AD38" s="13"/>
       <c r="AE38" s="13"/>
     </row>
-    <row r="39" spans="1:31" ht="40.049999999999997" customHeight="1">
+    <row r="39" spans="1:31" ht="40" customHeight="1">
       <c r="A39" s="116" t="s">
         <v>281</v>
       </c>
@@ -26260,7 +25188,7 @@
       <c r="AD39" s="13"/>
       <c r="AE39" s="13"/>
     </row>
-    <row r="40" spans="1:31" ht="20.399999999999999">
+    <row r="40" spans="1:31">
       <c r="A40" s="140" t="s">
         <v>282</v>
       </c>
@@ -26313,7 +25241,7 @@
       <c r="AD40" s="13"/>
       <c r="AE40" s="13"/>
     </row>
-    <row r="41" spans="1:31" ht="20.399999999999999">
+    <row r="41" spans="1:31">
       <c r="A41" s="140" t="s">
         <v>285</v>
       </c>
@@ -26366,7 +25294,7 @@
       <c r="AD41" s="13"/>
       <c r="AE41" s="13"/>
     </row>
-    <row r="42" spans="1:31" ht="20.399999999999999">
+    <row r="42" spans="1:31">
       <c r="A42" s="140" t="s">
         <v>286</v>
       </c>
@@ -26995,7 +25923,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="40" orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="33" orientation="landscape" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -27010,7 +25938,7 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -27028,11 +25956,11 @@
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="3" max="3" width="9.21875" customWidth="1"/>
-    <col min="10" max="10" width="12.77734375" customWidth="1"/>
-    <col min="12" max="12" width="5.21875" customWidth="1"/>
+    <col min="3" max="3" width="9.1796875" customWidth="1"/>
+    <col min="10" max="10" width="12.81640625" customWidth="1"/>
+    <col min="12" max="12" width="5.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -27050,7 +25978,7 @@
       <c r="L1" s="224"/>
     </row>
     <row r="21" spans="2:20" ht="33.75" customHeight="1"/>
-    <row r="22" spans="2:20" ht="50.4">
+    <row r="22" spans="2:20" ht="50.5">
       <c r="B22" s="5"/>
       <c r="D22" s="197" t="str">
         <f>HEP_Inter!A3</f>
@@ -27095,6 +26023,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FB6FBD5E95BAB542B810C32545CA4E3B" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c88f4da8c98e9c6f14dc759bd92b3b9d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="f244dd4c-ee25-4b14-a7cd-a89d47e877b9" xmlns:ns4="7d5efbb1-7b5c-4600-961f-d0c91f173691" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e11dd0c1a7b4f1799f1daf73497fb7c0" ns3:_="" ns4:_="">
     <xsd:import namespace="f244dd4c-ee25-4b14-a7cd-a89d47e877b9"/>
@@ -27305,22 +26248,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B8C5798F-31D9-455C-A266-3CF2A88C6872}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="7d5efbb1-7b5c-4600-961f-d0c91f173691"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="f244dd4c-ee25-4b14-a7cd-a89d47e877b9"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5668EAE9-BE2F-449B-83FE-5638B2ED2DF4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B491DB35-4E91-4B2D-816E-03001B21F1D3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -27337,29 +26290,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B8C5798F-31D9-455C-A266-3CF2A88C6872}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="7d5efbb1-7b5c-4600-961f-d0c91f173691"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="f244dd4c-ee25-4b14-a7cd-a89d47e877b9"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5668EAE9-BE2F-449B-83FE-5638B2ED2DF4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
delete broken link in country_summary_template
</commit_message>
<xml_diff>
--- a/inst/extdata/country_summary_template.xlsx
+++ b/inst/extdata/country_summary_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ellio\Documents\WHO\rapporteuR\inst\extdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ellio\Documents\WHO\rapporteur\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A23BA88B-A81E-4C03-8162-29006B3F7CEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D894AC6C-DCAE-4F02-A5BC-EA82A31E349C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32280" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="942" activeTab="14" xr2:uid="{A0469F42-B2BF-41E9-9270-FEA8E2D23640}"/>
   </bookViews>
@@ -31,9 +31,6 @@
     <sheet name="HPOP_Chart" sheetId="6" r:id="rId16"/>
     <sheet name="HPOP_Inter" sheetId="5" state="hidden" r:id="rId17"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId18"/>
-  </externalReferences>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="7">HEP_summary!$A$1:$C$31</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="12">HPOP_summary!$A$1:$D$28</definedName>
@@ -57,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1550" uniqueCount="474">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1561" uniqueCount="474">
   <si>
     <t>Magnitude +</t>
   </si>
@@ -3518,33 +3515,33 @@
     <xf numFmtId="1" fontId="12" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="42" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="42" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="51" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="45" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="30" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3588,18 +3585,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="54" fillId="18" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -3610,6 +3595,18 @@
     <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3619,15 +3616,18 @@
     <xf numFmtId="0" fontId="11" fillId="11" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3648,9 +3648,6 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -4348,7 +4345,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D46FBF52-8A26-487C-98CF-D5A88341DD45}" type="CELLRANGE">
+                    <a:fld id="{7CD41B26-5B89-4B26-99D3-F32FE9793116}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4409,7 +4406,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2685782D-E226-4D2B-B7ED-6AF2D77D4CD3}" type="CELLRANGE">
+                    <a:fld id="{7D43EB9A-16A2-48BF-8EC2-0F70E6FB58C7}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4470,7 +4467,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E77EA9C8-8F42-4B18-B879-681D2F9EDE1D}" type="CELLRANGE">
+                    <a:fld id="{CE3BD3F8-12FB-47BB-A931-F733C043F3E0}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4564,7 +4561,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{18FCB81D-10F2-4EFE-A608-E6EEE6F4D650}" type="CELLRANGE">
+                    <a:fld id="{7543386A-08E4-4D81-80A8-39FA76087125}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4598,7 +4595,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{05CAAF9D-8042-432A-B972-E684D432F0D2}" type="CELLRANGE">
+                    <a:fld id="{93C81047-E3FD-4455-BD45-902E2B3E9327}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4632,7 +4629,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{543A6EE3-56BE-423D-8DA4-B3BE2B5C1BE5}" type="CELLRANGE">
+                    <a:fld id="{EC6238FC-B931-4ACB-AA62-ED8192F4E785}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4666,7 +4663,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B8A4983A-C6AF-4966-ACFF-DEE80D3253AA}" type="CELLRANGE">
+                    <a:fld id="{DFED8290-2DAE-4821-9B5F-2D03B0E6F570}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4700,7 +4697,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{543A6DE8-BD56-40B2-96AA-9364EC6D46CB}" type="CELLRANGE">
+                    <a:fld id="{95601DEF-067D-42C6-A835-36B5BD26AA14}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4734,7 +4731,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2A039E77-CCD1-4CC0-9277-A6075434D9B3}" type="CELLRANGE">
+                    <a:fld id="{78348F83-33A8-4FF5-9693-D8FFEA3623DB}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6529,7 +6526,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6DB60B51-E936-4B87-B9CA-A4CDAB68776C}" type="CELLRANGE">
+                    <a:fld id="{80C1B1F2-7BC9-4293-B67C-1818915E95D7}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6590,7 +6587,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{888A7EEF-CF81-462A-95A8-618C8E84F726}" type="CELLRANGE">
+                    <a:fld id="{9963BF99-9784-4F90-AB7C-2A394907BB7C}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6651,7 +6648,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AFF4B3AA-CD23-435D-998D-B32AF333204C}" type="CELLRANGE">
+                    <a:fld id="{1756A048-20D2-4183-9949-778D453F15A7}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6685,7 +6682,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{15285AF3-2EF2-44D6-9C30-1934F1CF07C9}" type="CELLRANGE">
+                    <a:fld id="{E23CD415-24F0-4F9F-B4A5-964A4F0D6249}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6746,7 +6743,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0117289B-D39B-48C6-B2DE-505882F25FAD}" type="CELLRANGE">
+                    <a:fld id="{CBCB9C1D-BCCC-42C5-A7F2-E727E5635F33}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6780,7 +6777,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5FDC3543-2791-4ECC-8B80-3D39F63DA944}" type="CELLRANGE">
+                    <a:fld id="{711CFD37-F0D6-46F0-B442-845144571E32}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6814,7 +6811,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{59E3B28C-3B47-4968-9AA0-EFE3B177C0B3}" type="CELLRANGE">
+                    <a:fld id="{D1EAE4CD-D115-445E-9B64-62F670B4050E}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6848,7 +6845,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{52A0D1A2-EB75-4ECF-9BE7-FB1398249193}" type="CELLRANGE">
+                    <a:fld id="{6ED1C1CE-637B-4BDF-941E-B518B9A2ACDB}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6882,7 +6879,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{95E0333F-62EB-4C49-B7B2-1FA183BEDFA6}" type="CELLRANGE">
+                    <a:fld id="{ADF89E48-1440-4D39-A2B4-9133CA501404}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6916,7 +6913,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7CA3B187-CF4D-4752-BEFA-287F764AE8E4}" type="CELLRANGE">
+                    <a:fld id="{EC73FE3D-365C-43A8-AACA-87BE0F09E51B}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6950,7 +6947,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D8C6516A-5B52-45BA-8669-96ED841CC4B8}" type="CELLRANGE">
+                    <a:fld id="{33CCE893-3630-4D53-9263-367AAB67DEA2}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6984,7 +6981,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E5C2971E-C331-4B02-9A80-9229C8CCA8A7}" type="CELLRANGE">
+                    <a:fld id="{F02702FB-4AC4-4E37-975C-16235C32BBE7}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7018,7 +7015,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{00584802-52D9-43A1-BAF6-3889C067DC36}" type="CELLRANGE">
+                    <a:fld id="{6CEB851D-1C6C-4DBD-A7B5-1A0DEFCCC43A}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7602,1011 +7599,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Intro"/>
-      <sheetName val="Indicator List"/>
-      <sheetName val="UHC_summary"/>
-      <sheetName val="UHC_Time Series"/>
-      <sheetName val="UHC_Chart"/>
-      <sheetName val="UHC_Inter"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2">
-        <row r="1">
-          <cell r="B1"/>
-          <cell r="C1"/>
-          <cell r="D1"/>
-          <cell r="E1"/>
-          <cell r="I1"/>
-          <cell r="J1"/>
-          <cell r="L1"/>
-          <cell r="M1"/>
-        </row>
-        <row r="2">
-          <cell r="B2"/>
-          <cell r="C2"/>
-          <cell r="D2"/>
-          <cell r="E2"/>
-          <cell r="I2"/>
-          <cell r="J2"/>
-          <cell r="L2"/>
-          <cell r="M2"/>
-        </row>
-        <row r="3">
-          <cell r="B3"/>
-          <cell r="C3"/>
-          <cell r="D3"/>
-          <cell r="E3"/>
-          <cell r="I3"/>
-          <cell r="J3"/>
-          <cell r="L3"/>
-          <cell r="M3"/>
-        </row>
-        <row r="4">
-          <cell r="B4"/>
-          <cell r="C4"/>
-          <cell r="D4"/>
-          <cell r="E4"/>
-          <cell r="I4"/>
-          <cell r="J4"/>
-          <cell r="L4"/>
-          <cell r="M4"/>
-        </row>
-        <row r="5">
-          <cell r="B5"/>
-          <cell r="C5"/>
-          <cell r="D5"/>
-          <cell r="E5"/>
-          <cell r="I5"/>
-          <cell r="J5"/>
-          <cell r="L5"/>
-          <cell r="M5"/>
-        </row>
-        <row r="6">
-          <cell r="B6"/>
-          <cell r="C6"/>
-          <cell r="D6"/>
-          <cell r="E6"/>
-          <cell r="I6"/>
-          <cell r="J6"/>
-          <cell r="L6"/>
-          <cell r="M6"/>
-        </row>
-        <row r="7">
-          <cell r="B7"/>
-          <cell r="C7"/>
-          <cell r="D7"/>
-          <cell r="E7"/>
-          <cell r="I7"/>
-          <cell r="J7"/>
-          <cell r="L7"/>
-          <cell r="M7"/>
-        </row>
-        <row r="8">
-          <cell r="B8"/>
-          <cell r="C8"/>
-          <cell r="D8"/>
-          <cell r="E8"/>
-          <cell r="I8"/>
-          <cell r="J8"/>
-          <cell r="L8"/>
-          <cell r="M8"/>
-        </row>
-        <row r="9">
-          <cell r="B9"/>
-          <cell r="C9" t="str">
-            <v>Latest Reported/Estimated Data Available</v>
-          </cell>
-          <cell r="D9"/>
-          <cell r="E9"/>
-          <cell r="I9" t="str">
-            <v>2018 Baseline, and 2023 Projection</v>
-          </cell>
-          <cell r="J9"/>
-          <cell r="L9"/>
-          <cell r="M9"/>
-        </row>
-        <row r="10">
-          <cell r="B10"/>
-          <cell r="C10" t="str">
-            <v>Raw Value</v>
-          </cell>
-          <cell r="D10" t="str">
-            <v>Transformed Value</v>
-          </cell>
-          <cell r="E10" t="str">
-            <v>Year</v>
-          </cell>
-          <cell r="I10" t="str">
-            <v>Raw Value</v>
-          </cell>
-          <cell r="J10" t="str">
-            <v/>
-          </cell>
-          <cell r="L10" t="str">
-            <v>Transformed Value</v>
-          </cell>
-          <cell r="M10" t="str">
-            <v/>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="B11" t="str">
-            <v>Tracer Indicator</v>
-          </cell>
-          <cell r="C11"/>
-          <cell r="D11"/>
-          <cell r="E11"/>
-          <cell r="I11" t="str">
-            <v>2018</v>
-          </cell>
-          <cell r="J11" t="str">
-            <v>2023</v>
-          </cell>
-          <cell r="L11" t="str">
-            <v>2018</v>
-          </cell>
-          <cell r="M11" t="str">
-            <v>2023</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="B12"/>
-          <cell r="C12"/>
-          <cell r="D12"/>
-          <cell r="E12"/>
-          <cell r="I12"/>
-          <cell r="J12"/>
-          <cell r="L12"/>
-          <cell r="M12"/>
-        </row>
-        <row r="13">
-          <cell r="B13" t="str">
-            <v>Demand satisfied with modern methods (married women or in-union) 1</v>
-          </cell>
-          <cell r="C13">
-            <v>57.99</v>
-          </cell>
-          <cell r="D13" t="str">
-            <v/>
-          </cell>
-          <cell r="E13">
-            <v>2020</v>
-          </cell>
-          <cell r="I13">
-            <v>56.35</v>
-          </cell>
-          <cell r="J13">
-            <v>60.55</v>
-          </cell>
-          <cell r="L13"/>
-          <cell r="M13"/>
-        </row>
-        <row r="14">
-          <cell r="B14" t="str">
-            <v>Antenatal care coverage (+4 visits) 2</v>
-          </cell>
-          <cell r="C14"/>
-          <cell r="D14" t="str">
-            <v/>
-          </cell>
-          <cell r="E14"/>
-          <cell r="I14">
-            <v>98.58</v>
-          </cell>
-          <cell r="J14">
-            <v>98.46</v>
-          </cell>
-          <cell r="L14"/>
-          <cell r="M14"/>
-        </row>
-        <row r="15">
-          <cell r="B15" t="str">
-            <v>DPT3 Immunization coverage</v>
-          </cell>
-          <cell r="C15">
-            <v>98</v>
-          </cell>
-          <cell r="D15" t="str">
-            <v/>
-          </cell>
-          <cell r="E15">
-            <v>2019</v>
-          </cell>
-          <cell r="I15">
-            <v>98</v>
-          </cell>
-          <cell r="J15">
-            <v>98.54</v>
-          </cell>
-          <cell r="L15"/>
-          <cell r="M15"/>
-        </row>
-        <row r="16">
-          <cell r="B16" t="str">
-            <v>Care seeking for suspected pneumonia</v>
-          </cell>
-          <cell r="C16"/>
-          <cell r="D16" t="str">
-            <v/>
-          </cell>
-          <cell r="E16"/>
-          <cell r="I16">
-            <v>89.91</v>
-          </cell>
-          <cell r="J16">
-            <v>90.82</v>
-          </cell>
-          <cell r="L16"/>
-          <cell r="M16"/>
-        </row>
-        <row r="17">
-          <cell r="B17" t="str">
-            <v>Average RMNCH</v>
-          </cell>
-          <cell r="C17"/>
-          <cell r="D17"/>
-          <cell r="E17"/>
-          <cell r="I17"/>
-          <cell r="J17"/>
-          <cell r="L17"/>
-          <cell r="M17"/>
-        </row>
-        <row r="18">
-          <cell r="B18"/>
-          <cell r="C18"/>
-          <cell r="D18"/>
-          <cell r="E18"/>
-          <cell r="I18"/>
-          <cell r="J18"/>
-          <cell r="L18"/>
-          <cell r="M18"/>
-        </row>
-        <row r="19">
-          <cell r="B19" t="str">
-            <v>TB treatment coverage</v>
-          </cell>
-          <cell r="C19">
-            <v>86.96</v>
-          </cell>
-          <cell r="D19" t="str">
-            <v/>
-          </cell>
-          <cell r="E19">
-            <v>2019</v>
-          </cell>
-          <cell r="I19">
-            <v>86.96</v>
-          </cell>
-          <cell r="J19">
-            <v>86.96</v>
-          </cell>
-          <cell r="L19"/>
-          <cell r="M19"/>
-        </row>
-        <row r="20">
-          <cell r="B20" t="str">
-            <v>HIV ART coverage</v>
-          </cell>
-          <cell r="C20">
-            <v>84.01</v>
-          </cell>
-          <cell r="D20" t="str">
-            <v/>
-          </cell>
-          <cell r="E20">
-            <v>2019</v>
-          </cell>
-          <cell r="I20">
-            <v>83.01</v>
-          </cell>
-          <cell r="J20">
-            <v>90.99</v>
-          </cell>
-          <cell r="L20"/>
-          <cell r="M20"/>
-        </row>
-        <row r="21">
-          <cell r="B21" t="str">
-            <v>ITN use 4</v>
-          </cell>
-          <cell r="C21"/>
-          <cell r="D21" t="str">
-            <v/>
-          </cell>
-          <cell r="E21"/>
-          <cell r="I21"/>
-          <cell r="J21"/>
-          <cell r="L21"/>
-          <cell r="M21"/>
-        </row>
-        <row r="22">
-          <cell r="B22" t="str">
-            <v>Use of basic sanitation</v>
-          </cell>
-          <cell r="C22">
-            <v>99.89</v>
-          </cell>
-          <cell r="D22" t="str">
-            <v/>
-          </cell>
-          <cell r="E22">
-            <v>2017</v>
-          </cell>
-          <cell r="I22">
-            <v>99.9</v>
-          </cell>
-          <cell r="J22">
-            <v>99.9</v>
-          </cell>
-          <cell r="L22"/>
-          <cell r="M22"/>
-        </row>
-        <row r="23">
-          <cell r="B23" t="str">
-            <v>Average Infectious diseases</v>
-          </cell>
-          <cell r="C23"/>
-          <cell r="D23"/>
-          <cell r="E23"/>
-          <cell r="I23"/>
-          <cell r="J23"/>
-          <cell r="L23"/>
-          <cell r="M23"/>
-        </row>
-        <row r="24">
-          <cell r="B24"/>
-          <cell r="C24"/>
-          <cell r="D24"/>
-          <cell r="E24"/>
-          <cell r="I24"/>
-          <cell r="J24"/>
-          <cell r="L24"/>
-          <cell r="M24"/>
-        </row>
-        <row r="25">
-          <cell r="B25" t="str">
-            <v>Prevalence of raised blood pressure*</v>
-          </cell>
-          <cell r="C25">
-            <v>17.55</v>
-          </cell>
-          <cell r="D25"/>
-          <cell r="E25">
-            <v>2015</v>
-          </cell>
-          <cell r="I25">
-            <v>16.68</v>
-          </cell>
-          <cell r="J25">
-            <v>15.29</v>
-          </cell>
-          <cell r="L25"/>
-          <cell r="M25"/>
-        </row>
-        <row r="26">
-          <cell r="B26" t="str">
-            <v>Mean fasting blood glucose (mmol/l)*</v>
-          </cell>
-          <cell r="C26">
-            <v>5.2</v>
-          </cell>
-          <cell r="D26"/>
-          <cell r="E26">
-            <v>2014</v>
-          </cell>
-          <cell r="I26">
-            <v>5.12</v>
-          </cell>
-          <cell r="J26">
-            <v>5.03</v>
-          </cell>
-          <cell r="L26"/>
-          <cell r="M26"/>
-        </row>
-        <row r="27">
-          <cell r="B27" t="str">
-            <v>Tobacco use prevalence* 3</v>
-          </cell>
-          <cell r="C27">
-            <v>21.9</v>
-          </cell>
-          <cell r="D27"/>
-          <cell r="E27">
-            <v>2018</v>
-          </cell>
-          <cell r="I27">
-            <v>21.9</v>
-          </cell>
-          <cell r="J27">
-            <v>19.5</v>
-          </cell>
-          <cell r="L27"/>
-          <cell r="M27"/>
-        </row>
-        <row r="28">
-          <cell r="B28" t="str">
-            <v>Average NCDs</v>
-          </cell>
-          <cell r="C28"/>
-          <cell r="D28"/>
-          <cell r="E28"/>
-          <cell r="I28"/>
-          <cell r="J28"/>
-          <cell r="L28"/>
-          <cell r="M28"/>
-        </row>
-        <row r="29">
-          <cell r="B29"/>
-          <cell r="C29"/>
-          <cell r="D29"/>
-          <cell r="E29"/>
-          <cell r="I29"/>
-          <cell r="J29"/>
-          <cell r="L29"/>
-          <cell r="M29"/>
-        </row>
-        <row r="30">
-          <cell r="B30" t="str">
-            <v>Hospital beds density*</v>
-          </cell>
-          <cell r="C30">
-            <v>129.04</v>
-          </cell>
-          <cell r="D30"/>
-          <cell r="E30">
-            <v>2018</v>
-          </cell>
-          <cell r="I30">
-            <v>129.04</v>
-          </cell>
-          <cell r="J30">
-            <v>130.5</v>
-          </cell>
-          <cell r="L30"/>
-          <cell r="M30"/>
-        </row>
-        <row r="31">
-          <cell r="B31" t="str">
-            <v>Health worker density*</v>
-          </cell>
-          <cell r="C31">
-            <v>151.77000000000001</v>
-          </cell>
-          <cell r="D31"/>
-          <cell r="E31">
-            <v>2018</v>
-          </cell>
-          <cell r="I31">
-            <v>151.77000000000001</v>
-          </cell>
-          <cell r="J31">
-            <v>172.69</v>
-          </cell>
-          <cell r="L31"/>
-          <cell r="M31"/>
-        </row>
-        <row r="32">
-          <cell r="B32" t="str">
-            <v>Density of doctors</v>
-          </cell>
-          <cell r="C32">
-            <v>24.8</v>
-          </cell>
-          <cell r="D32"/>
-          <cell r="E32">
-            <v>2018</v>
-          </cell>
-          <cell r="I32">
-            <v>24.8</v>
-          </cell>
-          <cell r="J32">
-            <v>27.38</v>
-          </cell>
-          <cell r="L32"/>
-          <cell r="M32"/>
-        </row>
-        <row r="33">
-          <cell r="B33" t="str">
-            <v>Density of nurses/midwives</v>
-          </cell>
-          <cell r="C33">
-            <v>126.98</v>
-          </cell>
-          <cell r="D33"/>
-          <cell r="E33">
-            <v>2018</v>
-          </cell>
-          <cell r="I33">
-            <v>126.98</v>
-          </cell>
-          <cell r="J33">
-            <v>145.31</v>
-          </cell>
-          <cell r="L33"/>
-          <cell r="M33"/>
-        </row>
-        <row r="34">
-          <cell r="B34" t="str">
-            <v>IHR core capacity index*</v>
-          </cell>
-          <cell r="C34">
-            <v>95</v>
-          </cell>
-          <cell r="D34"/>
-          <cell r="E34">
-            <v>2020</v>
-          </cell>
-          <cell r="I34">
-            <v>95</v>
-          </cell>
-          <cell r="J34">
-            <v>94.99</v>
-          </cell>
-          <cell r="L34"/>
-          <cell r="M34"/>
-        </row>
-        <row r="35">
-          <cell r="B35" t="str">
-            <v>Average Service capacity and access</v>
-          </cell>
-          <cell r="C35"/>
-          <cell r="D35"/>
-          <cell r="E35"/>
-          <cell r="I35"/>
-          <cell r="J35"/>
-          <cell r="L35"/>
-          <cell r="M35"/>
-        </row>
-        <row r="36">
-          <cell r="B36"/>
-          <cell r="C36"/>
-          <cell r="D36"/>
-          <cell r="E36"/>
-          <cell r="I36"/>
-          <cell r="J36"/>
-          <cell r="L36"/>
-          <cell r="M36"/>
-        </row>
-        <row r="37">
-          <cell r="B37" t="str">
-            <v>SDG 3.8.2 Proportion of population with household expenditures on health &gt;10% of total household expenditure or income **</v>
-          </cell>
-          <cell r="C37">
-            <v>4.3600000000000003</v>
-          </cell>
-          <cell r="D37" t="str">
-            <v/>
-          </cell>
-          <cell r="E37">
-            <v>2015</v>
-          </cell>
-          <cell r="I37">
-            <v>4.2300000000000004</v>
-          </cell>
-          <cell r="J37">
-            <v>4.0599999999999996</v>
-          </cell>
-          <cell r="L37"/>
-          <cell r="M37"/>
-        </row>
-        <row r="38">
-          <cell r="B38" t="str">
-            <v>UHC single measure</v>
-          </cell>
-          <cell r="C38"/>
-          <cell r="D38"/>
-          <cell r="E38"/>
-          <cell r="I38"/>
-          <cell r="J38"/>
-          <cell r="L38">
-            <v>61.09664039777099</v>
-          </cell>
-          <cell r="M38">
-            <v>63.310803650646406</v>
-          </cell>
-        </row>
-        <row r="39">
-          <cell r="B39" t="str">
-            <v>Change in UHC single measure over 2018-2023</v>
-          </cell>
-          <cell r="C39"/>
-          <cell r="D39"/>
-          <cell r="E39"/>
-          <cell r="I39"/>
-          <cell r="J39"/>
-          <cell r="L39"/>
-          <cell r="M39"/>
-        </row>
-        <row r="40">
-          <cell r="B40" t="str">
-            <v>UN Population 2023 (thousand)</v>
-          </cell>
-          <cell r="C40"/>
-          <cell r="D40"/>
-          <cell r="E40"/>
-          <cell r="I40"/>
-          <cell r="J40"/>
-          <cell r="L40"/>
-          <cell r="M40"/>
-        </row>
-        <row r="41">
-          <cell r="B41" t="str">
-            <v>Country contribution to UHC billion target (population - thousand)</v>
-          </cell>
-          <cell r="C41"/>
-          <cell r="D41"/>
-          <cell r="E41"/>
-          <cell r="I41"/>
-          <cell r="J41"/>
-          <cell r="L41"/>
-          <cell r="M41"/>
-        </row>
-        <row r="42">
-          <cell r="B42" t="str">
-            <v>% of country population newly covered by universal healthcare</v>
-          </cell>
-          <cell r="C42"/>
-          <cell r="D42"/>
-          <cell r="E42"/>
-          <cell r="I42"/>
-          <cell r="J42"/>
-          <cell r="L42"/>
-          <cell r="M42"/>
-        </row>
-        <row r="43">
-          <cell r="B43"/>
-          <cell r="C43"/>
-          <cell r="D43"/>
-          <cell r="E43"/>
-          <cell r="I43"/>
-          <cell r="J43"/>
-          <cell r="L43"/>
-          <cell r="M43"/>
-        </row>
-        <row r="44">
-          <cell r="B44"/>
-          <cell r="C44"/>
-          <cell r="D44"/>
-          <cell r="E44"/>
-          <cell r="I44"/>
-          <cell r="J44"/>
-          <cell r="L44"/>
-          <cell r="M44"/>
-        </row>
-        <row r="45">
-          <cell r="B45"/>
-          <cell r="C45"/>
-          <cell r="D45"/>
-          <cell r="E45"/>
-          <cell r="I45"/>
-          <cell r="J45"/>
-          <cell r="L45"/>
-          <cell r="M45"/>
-        </row>
-        <row r="46">
-          <cell r="B46"/>
-          <cell r="C46"/>
-          <cell r="D46"/>
-          <cell r="E46"/>
-          <cell r="I46"/>
-          <cell r="J46"/>
-          <cell r="L46"/>
-          <cell r="M46"/>
-        </row>
-        <row r="47">
-          <cell r="B47"/>
-          <cell r="C47"/>
-          <cell r="D47"/>
-          <cell r="E47"/>
-          <cell r="I47"/>
-          <cell r="J47"/>
-          <cell r="L47"/>
-          <cell r="M47"/>
-        </row>
-        <row r="48">
-          <cell r="B48"/>
-          <cell r="C48"/>
-          <cell r="D48"/>
-          <cell r="E48"/>
-          <cell r="I48"/>
-          <cell r="J48"/>
-          <cell r="L48"/>
-          <cell r="M48"/>
-        </row>
-        <row r="49">
-          <cell r="B49"/>
-          <cell r="C49"/>
-          <cell r="D49"/>
-          <cell r="E49"/>
-          <cell r="I49"/>
-          <cell r="J49"/>
-          <cell r="L49"/>
-          <cell r="M49"/>
-        </row>
-        <row r="50">
-          <cell r="B50"/>
-          <cell r="C50"/>
-          <cell r="D50"/>
-          <cell r="E50"/>
-          <cell r="I50"/>
-          <cell r="J50"/>
-          <cell r="L50"/>
-          <cell r="M50"/>
-        </row>
-        <row r="51">
-          <cell r="B51"/>
-          <cell r="C51"/>
-          <cell r="D51"/>
-          <cell r="E51"/>
-          <cell r="I51"/>
-          <cell r="J51"/>
-          <cell r="L51"/>
-          <cell r="M51"/>
-        </row>
-        <row r="52">
-          <cell r="B52"/>
-          <cell r="C52"/>
-          <cell r="D52"/>
-          <cell r="E52"/>
-          <cell r="I52"/>
-          <cell r="J52"/>
-          <cell r="L52"/>
-          <cell r="M52"/>
-        </row>
-        <row r="53">
-          <cell r="B53"/>
-          <cell r="C53"/>
-          <cell r="D53"/>
-          <cell r="E53"/>
-          <cell r="I53"/>
-          <cell r="J53"/>
-          <cell r="L53"/>
-          <cell r="M53"/>
-        </row>
-        <row r="54">
-          <cell r="B54"/>
-          <cell r="C54"/>
-          <cell r="D54"/>
-          <cell r="E54"/>
-          <cell r="I54"/>
-          <cell r="J54"/>
-          <cell r="L54"/>
-          <cell r="M54"/>
-        </row>
-        <row r="55">
-          <cell r="B55"/>
-          <cell r="C55"/>
-          <cell r="D55"/>
-          <cell r="E55"/>
-          <cell r="I55"/>
-          <cell r="J55"/>
-          <cell r="L55"/>
-          <cell r="M55"/>
-        </row>
-        <row r="56">
-          <cell r="B56"/>
-          <cell r="C56"/>
-          <cell r="D56"/>
-          <cell r="E56"/>
-          <cell r="I56"/>
-          <cell r="J56"/>
-          <cell r="L56"/>
-          <cell r="M56"/>
-        </row>
-        <row r="57">
-          <cell r="B57"/>
-          <cell r="C57"/>
-          <cell r="D57"/>
-          <cell r="E57"/>
-          <cell r="I57"/>
-          <cell r="J57"/>
-          <cell r="L57"/>
-          <cell r="M57"/>
-        </row>
-        <row r="58">
-          <cell r="B58"/>
-          <cell r="C58"/>
-          <cell r="D58"/>
-          <cell r="E58"/>
-          <cell r="I58"/>
-          <cell r="J58"/>
-          <cell r="L58"/>
-          <cell r="M58"/>
-        </row>
-        <row r="59">
-          <cell r="B59"/>
-          <cell r="C59"/>
-          <cell r="D59"/>
-          <cell r="E59"/>
-          <cell r="I59"/>
-          <cell r="J59"/>
-          <cell r="L59"/>
-          <cell r="M59"/>
-        </row>
-        <row r="60">
-          <cell r="B60"/>
-          <cell r="C60"/>
-          <cell r="D60"/>
-          <cell r="E60"/>
-          <cell r="I60"/>
-          <cell r="J60"/>
-          <cell r="L60"/>
-          <cell r="M60"/>
-        </row>
-        <row r="61">
-          <cell r="B61"/>
-          <cell r="C61"/>
-          <cell r="D61"/>
-          <cell r="E61"/>
-          <cell r="I61"/>
-          <cell r="J61"/>
-          <cell r="L61"/>
-          <cell r="M61"/>
-        </row>
-        <row r="62">
-          <cell r="B62"/>
-          <cell r="C62"/>
-          <cell r="D62"/>
-          <cell r="E62"/>
-          <cell r="I62"/>
-          <cell r="J62"/>
-          <cell r="L62"/>
-          <cell r="M62"/>
-        </row>
-        <row r="63">
-          <cell r="B63"/>
-          <cell r="C63"/>
-          <cell r="D63"/>
-          <cell r="E63"/>
-          <cell r="I63"/>
-          <cell r="J63"/>
-          <cell r="L63"/>
-          <cell r="M63"/>
-        </row>
-        <row r="64">
-          <cell r="B64"/>
-          <cell r="C64"/>
-          <cell r="D64"/>
-          <cell r="E64"/>
-          <cell r="I64"/>
-          <cell r="J64"/>
-          <cell r="L64"/>
-          <cell r="M64"/>
-        </row>
-        <row r="65">
-          <cell r="B65"/>
-          <cell r="C65"/>
-          <cell r="D65"/>
-          <cell r="E65"/>
-          <cell r="I65"/>
-          <cell r="J65"/>
-          <cell r="L65"/>
-          <cell r="M65"/>
-        </row>
-        <row r="66">
-          <cell r="B66"/>
-          <cell r="C66"/>
-          <cell r="D66"/>
-          <cell r="E66"/>
-          <cell r="I66"/>
-          <cell r="J66"/>
-          <cell r="L66"/>
-          <cell r="M66"/>
-        </row>
-        <row r="67">
-          <cell r="B67"/>
-          <cell r="C67"/>
-          <cell r="D67"/>
-          <cell r="E67"/>
-          <cell r="I67"/>
-          <cell r="J67"/>
-          <cell r="L67"/>
-          <cell r="M67"/>
-        </row>
-        <row r="68">
-          <cell r="B68"/>
-          <cell r="C68"/>
-          <cell r="D68"/>
-          <cell r="E68"/>
-          <cell r="I68"/>
-          <cell r="J68"/>
-          <cell r="L68"/>
-          <cell r="M68"/>
-        </row>
-        <row r="69">
-          <cell r="B69"/>
-          <cell r="C69"/>
-          <cell r="D69"/>
-          <cell r="E69"/>
-          <cell r="I69"/>
-          <cell r="J69"/>
-          <cell r="L69"/>
-          <cell r="M69"/>
-        </row>
-      </sheetData>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5">
-        <row r="3">
-          <cell r="A3" t="str">
-            <v>Demand satisfied with modern methods (married women or in-union) 1</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="A4" t="str">
-            <v>Antenatal care coverage (+4 visits) 2</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="A5" t="str">
-            <v>DPT3 Immunization coverage</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="A6" t="str">
-            <v>Care seeking for suspected pneumonia</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="A7" t="str">
-            <v>TB treatment coverage</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="A8" t="str">
-            <v>HIV ART coverage 4</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="A9" t="str">
-            <v>Use of basic sanitation</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="A10" t="str">
-            <v>Prevalence of raised blood pressure*</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="A11" t="str">
-            <v>Mean fasting blood glucose (mmol/l)*</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="A12" t="str">
-            <v>Tobacco use prevalence* 3</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="A13" t="str">
-            <v>Hospital beds density*</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="A14" t="str">
-            <v>Health worker density*</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="A15" t="str">
-            <v>IHR core capacity index*</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="A16"/>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -8923,664 +7915,664 @@
   <sheetData>
     <row r="1" spans="2:15" ht="10.5" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:15" ht="36" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="326" t="s">
+      <c r="B2" s="323" t="s">
         <v>337</v>
       </c>
-      <c r="C2" s="326"/>
-      <c r="D2" s="326"/>
-      <c r="E2" s="326"/>
-      <c r="F2" s="326"/>
-      <c r="G2" s="326"/>
-      <c r="H2" s="326"/>
-      <c r="I2" s="326"/>
-      <c r="J2" s="326"/>
-      <c r="K2" s="326"/>
-      <c r="L2" s="326"/>
-      <c r="M2" s="326"/>
+      <c r="C2" s="323"/>
+      <c r="D2" s="323"/>
+      <c r="E2" s="323"/>
+      <c r="F2" s="323"/>
+      <c r="G2" s="323"/>
+      <c r="H2" s="323"/>
+      <c r="I2" s="323"/>
+      <c r="J2" s="323"/>
+      <c r="K2" s="323"/>
+      <c r="L2" s="323"/>
+      <c r="M2" s="323"/>
       <c r="N2" s="61"/>
       <c r="O2" s="61"/>
     </row>
     <row r="3" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="327" t="s">
+      <c r="B3" s="324" t="s">
         <v>435</v>
       </c>
-      <c r="C3" s="327"/>
-      <c r="D3" s="327"/>
-      <c r="E3" s="327"/>
-      <c r="F3" s="327"/>
-      <c r="G3" s="327"/>
-      <c r="H3" s="327"/>
-      <c r="I3" s="327"/>
-      <c r="J3" s="327"/>
-      <c r="K3" s="327"/>
-      <c r="L3" s="327"/>
-      <c r="M3" s="327"/>
+      <c r="C3" s="324"/>
+      <c r="D3" s="324"/>
+      <c r="E3" s="324"/>
+      <c r="F3" s="324"/>
+      <c r="G3" s="324"/>
+      <c r="H3" s="324"/>
+      <c r="I3" s="324"/>
+      <c r="J3" s="324"/>
+      <c r="K3" s="324"/>
+      <c r="L3" s="324"/>
+      <c r="M3" s="324"/>
       <c r="N3" s="200"/>
       <c r="O3" s="200"/>
     </row>
     <row r="4" spans="2:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="323" t="s">
+      <c r="B4" s="320" t="s">
         <v>338</v>
       </c>
-      <c r="C4" s="323"/>
-      <c r="D4" s="323"/>
-      <c r="E4" s="323"/>
-      <c r="F4" s="323"/>
-      <c r="G4" s="323"/>
-      <c r="H4" s="323"/>
-      <c r="I4" s="323"/>
-      <c r="J4" s="323"/>
-      <c r="K4" s="323"/>
-      <c r="L4" s="323"/>
-      <c r="M4" s="323"/>
+      <c r="C4" s="320"/>
+      <c r="D4" s="320"/>
+      <c r="E4" s="320"/>
+      <c r="F4" s="320"/>
+      <c r="G4" s="320"/>
+      <c r="H4" s="320"/>
+      <c r="I4" s="320"/>
+      <c r="J4" s="320"/>
+      <c r="K4" s="320"/>
+      <c r="L4" s="320"/>
+      <c r="M4" s="320"/>
       <c r="N4" s="201"/>
       <c r="O4" s="201"/>
     </row>
     <row r="5" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="320" t="s">
+      <c r="B5" s="321" t="s">
         <v>358</v>
       </c>
-      <c r="C5" s="320"/>
-      <c r="D5" s="320"/>
-      <c r="E5" s="320"/>
-      <c r="F5" s="320"/>
-      <c r="G5" s="320"/>
-      <c r="H5" s="320"/>
-      <c r="I5" s="320"/>
-      <c r="J5" s="320"/>
-      <c r="K5" s="320"/>
-      <c r="L5" s="320"/>
-      <c r="M5" s="320"/>
+      <c r="C5" s="321"/>
+      <c r="D5" s="321"/>
+      <c r="E5" s="321"/>
+      <c r="F5" s="321"/>
+      <c r="G5" s="321"/>
+      <c r="H5" s="321"/>
+      <c r="I5" s="321"/>
+      <c r="J5" s="321"/>
+      <c r="K5" s="321"/>
+      <c r="L5" s="321"/>
+      <c r="M5" s="321"/>
       <c r="N5" s="200"/>
       <c r="O5" s="200"/>
     </row>
     <row r="6" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="325" t="s">
+      <c r="B6" s="319" t="s">
         <v>359</v>
       </c>
-      <c r="C6" s="325"/>
-      <c r="D6" s="325"/>
-      <c r="E6" s="325"/>
-      <c r="F6" s="325"/>
-      <c r="G6" s="325"/>
-      <c r="H6" s="325"/>
-      <c r="I6" s="325"/>
-      <c r="J6" s="325"/>
-      <c r="K6" s="325"/>
-      <c r="L6" s="325"/>
-      <c r="M6" s="325"/>
+      <c r="C6" s="319"/>
+      <c r="D6" s="319"/>
+      <c r="E6" s="319"/>
+      <c r="F6" s="319"/>
+      <c r="G6" s="319"/>
+      <c r="H6" s="319"/>
+      <c r="I6" s="319"/>
+      <c r="J6" s="319"/>
+      <c r="K6" s="319"/>
+      <c r="L6" s="319"/>
+      <c r="M6" s="319"/>
       <c r="N6" s="202"/>
       <c r="O6" s="202"/>
     </row>
     <row r="7" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="325" t="s">
+      <c r="B7" s="319" t="s">
         <v>360</v>
       </c>
-      <c r="C7" s="325"/>
-      <c r="D7" s="325"/>
-      <c r="E7" s="325"/>
-      <c r="F7" s="325"/>
-      <c r="G7" s="325"/>
-      <c r="H7" s="325"/>
-      <c r="I7" s="325"/>
-      <c r="J7" s="325"/>
-      <c r="K7" s="325"/>
-      <c r="L7" s="325"/>
-      <c r="M7" s="325"/>
+      <c r="C7" s="319"/>
+      <c r="D7" s="319"/>
+      <c r="E7" s="319"/>
+      <c r="F7" s="319"/>
+      <c r="G7" s="319"/>
+      <c r="H7" s="319"/>
+      <c r="I7" s="319"/>
+      <c r="J7" s="319"/>
+      <c r="K7" s="319"/>
+      <c r="L7" s="319"/>
+      <c r="M7" s="319"/>
       <c r="N7" s="202"/>
       <c r="O7" s="202"/>
     </row>
     <row r="8" spans="2:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="325" t="s">
+      <c r="B8" s="319" t="s">
         <v>361</v>
       </c>
-      <c r="C8" s="325"/>
-      <c r="D8" s="325"/>
-      <c r="E8" s="325"/>
-      <c r="F8" s="325"/>
-      <c r="G8" s="325"/>
-      <c r="H8" s="325"/>
-      <c r="I8" s="325"/>
-      <c r="J8" s="325"/>
-      <c r="K8" s="325"/>
-      <c r="L8" s="325"/>
-      <c r="M8" s="325"/>
+      <c r="C8" s="319"/>
+      <c r="D8" s="319"/>
+      <c r="E8" s="319"/>
+      <c r="F8" s="319"/>
+      <c r="G8" s="319"/>
+      <c r="H8" s="319"/>
+      <c r="I8" s="319"/>
+      <c r="J8" s="319"/>
+      <c r="K8" s="319"/>
+      <c r="L8" s="319"/>
+      <c r="M8" s="319"/>
       <c r="N8" s="202"/>
       <c r="O8" s="202"/>
     </row>
     <row r="9" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="320" t="s">
+      <c r="B9" s="321" t="s">
         <v>339</v>
       </c>
-      <c r="C9" s="320"/>
-      <c r="D9" s="320"/>
-      <c r="E9" s="320"/>
-      <c r="F9" s="320"/>
-      <c r="G9" s="320"/>
-      <c r="H9" s="320"/>
-      <c r="I9" s="320"/>
-      <c r="J9" s="320"/>
-      <c r="K9" s="320"/>
-      <c r="L9" s="320"/>
+      <c r="C9" s="321"/>
+      <c r="D9" s="321"/>
+      <c r="E9" s="321"/>
+      <c r="F9" s="321"/>
+      <c r="G9" s="321"/>
+      <c r="H9" s="321"/>
+      <c r="I9" s="321"/>
+      <c r="J9" s="321"/>
+      <c r="K9" s="321"/>
+      <c r="L9" s="321"/>
     </row>
     <row r="10" spans="2:15" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="320" t="s">
+      <c r="B10" s="321" t="s">
         <v>340</v>
       </c>
-      <c r="C10" s="320"/>
-      <c r="D10" s="320"/>
-      <c r="E10" s="320"/>
-      <c r="F10" s="320"/>
-      <c r="G10" s="320"/>
-      <c r="H10" s="320"/>
-      <c r="I10" s="320"/>
-      <c r="J10" s="320"/>
-      <c r="K10" s="320"/>
-      <c r="L10" s="320"/>
+      <c r="C10" s="321"/>
+      <c r="D10" s="321"/>
+      <c r="E10" s="321"/>
+      <c r="F10" s="321"/>
+      <c r="G10" s="321"/>
+      <c r="H10" s="321"/>
+      <c r="I10" s="321"/>
+      <c r="J10" s="321"/>
+      <c r="K10" s="321"/>
+      <c r="L10" s="321"/>
     </row>
     <row r="11" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="323" t="s">
+      <c r="B11" s="320" t="s">
         <v>341</v>
       </c>
-      <c r="C11" s="323"/>
-      <c r="D11" s="323"/>
-      <c r="E11" s="323"/>
-      <c r="F11" s="323"/>
-      <c r="G11" s="323"/>
-      <c r="H11" s="323"/>
-      <c r="I11" s="323"/>
-      <c r="J11" s="323"/>
-      <c r="K11" s="323"/>
-      <c r="L11" s="323"/>
-      <c r="M11" s="323"/>
+      <c r="C11" s="320"/>
+      <c r="D11" s="320"/>
+      <c r="E11" s="320"/>
+      <c r="F11" s="320"/>
+      <c r="G11" s="320"/>
+      <c r="H11" s="320"/>
+      <c r="I11" s="320"/>
+      <c r="J11" s="320"/>
+      <c r="K11" s="320"/>
+      <c r="L11" s="320"/>
+      <c r="M11" s="320"/>
       <c r="N11" s="62"/>
       <c r="O11" s="62"/>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B12" s="320" t="s">
+      <c r="B12" s="321" t="s">
         <v>342</v>
       </c>
-      <c r="C12" s="320"/>
-      <c r="D12" s="320"/>
-      <c r="E12" s="320"/>
-      <c r="F12" s="320"/>
-      <c r="G12" s="320"/>
-      <c r="H12" s="320"/>
-      <c r="I12" s="320"/>
-      <c r="J12" s="320"/>
-      <c r="K12" s="320"/>
-      <c r="L12" s="320"/>
-      <c r="M12" s="320"/>
+      <c r="C12" s="321"/>
+      <c r="D12" s="321"/>
+      <c r="E12" s="321"/>
+      <c r="F12" s="321"/>
+      <c r="G12" s="321"/>
+      <c r="H12" s="321"/>
+      <c r="I12" s="321"/>
+      <c r="J12" s="321"/>
+      <c r="K12" s="321"/>
+      <c r="L12" s="321"/>
+      <c r="M12" s="321"/>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B13" s="324" t="s">
+      <c r="B13" s="322" t="s">
         <v>367</v>
       </c>
-      <c r="C13" s="325"/>
-      <c r="D13" s="325"/>
-      <c r="E13" s="325"/>
-      <c r="F13" s="325"/>
-      <c r="G13" s="325"/>
-      <c r="H13" s="325"/>
-      <c r="I13" s="325"/>
-      <c r="J13" s="325"/>
-      <c r="K13" s="325"/>
-      <c r="L13" s="325"/>
-      <c r="M13" s="325"/>
+      <c r="C13" s="319"/>
+      <c r="D13" s="319"/>
+      <c r="E13" s="319"/>
+      <c r="F13" s="319"/>
+      <c r="G13" s="319"/>
+      <c r="H13" s="319"/>
+      <c r="I13" s="319"/>
+      <c r="J13" s="319"/>
+      <c r="K13" s="319"/>
+      <c r="L13" s="319"/>
+      <c r="M13" s="319"/>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B14" s="324" t="s">
+      <c r="B14" s="322" t="s">
         <v>368</v>
       </c>
-      <c r="C14" s="325"/>
-      <c r="D14" s="325"/>
-      <c r="E14" s="325"/>
-      <c r="F14" s="325"/>
-      <c r="G14" s="325"/>
-      <c r="H14" s="325"/>
-      <c r="I14" s="325"/>
-      <c r="J14" s="325"/>
-      <c r="K14" s="325"/>
-      <c r="L14" s="325"/>
-      <c r="M14" s="325"/>
+      <c r="C14" s="319"/>
+      <c r="D14" s="319"/>
+      <c r="E14" s="319"/>
+      <c r="F14" s="319"/>
+      <c r="G14" s="319"/>
+      <c r="H14" s="319"/>
+      <c r="I14" s="319"/>
+      <c r="J14" s="319"/>
+      <c r="K14" s="319"/>
+      <c r="L14" s="319"/>
+      <c r="M14" s="319"/>
     </row>
     <row r="15" spans="2:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="324" t="s">
+      <c r="B15" s="322" t="s">
         <v>369</v>
       </c>
-      <c r="C15" s="325"/>
-      <c r="D15" s="325"/>
-      <c r="E15" s="325"/>
-      <c r="F15" s="325"/>
-      <c r="G15" s="325"/>
-      <c r="H15" s="325"/>
-      <c r="I15" s="325"/>
-      <c r="J15" s="325"/>
-      <c r="K15" s="325"/>
-      <c r="L15" s="325"/>
-      <c r="M15" s="325"/>
+      <c r="C15" s="319"/>
+      <c r="D15" s="319"/>
+      <c r="E15" s="319"/>
+      <c r="F15" s="319"/>
+      <c r="G15" s="319"/>
+      <c r="H15" s="319"/>
+      <c r="I15" s="319"/>
+      <c r="J15" s="319"/>
+      <c r="K15" s="319"/>
+      <c r="L15" s="319"/>
+      <c r="M15" s="319"/>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B16" s="320" t="s">
+      <c r="B16" s="321" t="s">
         <v>366</v>
       </c>
-      <c r="C16" s="320"/>
-      <c r="D16" s="320"/>
-      <c r="E16" s="320"/>
-      <c r="F16" s="320"/>
-      <c r="G16" s="320"/>
-      <c r="H16" s="320"/>
-      <c r="I16" s="320"/>
-      <c r="J16" s="320"/>
-      <c r="K16" s="320"/>
-      <c r="L16" s="320"/>
-      <c r="M16" s="320"/>
+      <c r="C16" s="321"/>
+      <c r="D16" s="321"/>
+      <c r="E16" s="321"/>
+      <c r="F16" s="321"/>
+      <c r="G16" s="321"/>
+      <c r="H16" s="321"/>
+      <c r="I16" s="321"/>
+      <c r="J16" s="321"/>
+      <c r="K16" s="321"/>
+      <c r="L16" s="321"/>
+      <c r="M16" s="321"/>
     </row>
     <row r="17" spans="2:13" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="B17" s="323" t="s">
+      <c r="B17" s="320" t="s">
         <v>343</v>
       </c>
-      <c r="C17" s="323"/>
-      <c r="D17" s="323"/>
-      <c r="E17" s="323"/>
-      <c r="F17" s="323"/>
-      <c r="G17" s="323"/>
-      <c r="H17" s="323"/>
-      <c r="I17" s="323"/>
-      <c r="J17" s="323"/>
-      <c r="K17" s="323"/>
-      <c r="L17" s="323"/>
-      <c r="M17" s="323"/>
+      <c r="C17" s="320"/>
+      <c r="D17" s="320"/>
+      <c r="E17" s="320"/>
+      <c r="F17" s="320"/>
+      <c r="G17" s="320"/>
+      <c r="H17" s="320"/>
+      <c r="I17" s="320"/>
+      <c r="J17" s="320"/>
+      <c r="K17" s="320"/>
+      <c r="L17" s="320"/>
+      <c r="M17" s="320"/>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B18" s="320" t="s">
+      <c r="B18" s="321" t="s">
         <v>344</v>
       </c>
-      <c r="C18" s="320"/>
-      <c r="D18" s="320"/>
-      <c r="E18" s="320"/>
-      <c r="F18" s="320"/>
-      <c r="G18" s="320"/>
-      <c r="H18" s="320"/>
-      <c r="I18" s="320"/>
-      <c r="J18" s="320"/>
-      <c r="K18" s="320"/>
-      <c r="L18" s="320"/>
-      <c r="M18" s="320"/>
+      <c r="C18" s="321"/>
+      <c r="D18" s="321"/>
+      <c r="E18" s="321"/>
+      <c r="F18" s="321"/>
+      <c r="G18" s="321"/>
+      <c r="H18" s="321"/>
+      <c r="I18" s="321"/>
+      <c r="J18" s="321"/>
+      <c r="K18" s="321"/>
+      <c r="L18" s="321"/>
+      <c r="M18" s="321"/>
     </row>
     <row r="19" spans="2:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" s="258"/>
-      <c r="C19" s="319" t="s">
+      <c r="C19" s="325" t="s">
         <v>362</v>
       </c>
-      <c r="D19" s="319"/>
-      <c r="E19" s="319"/>
-      <c r="F19" s="319"/>
-      <c r="G19" s="319"/>
-      <c r="H19" s="319"/>
-      <c r="I19" s="319"/>
-      <c r="J19" s="319"/>
-      <c r="K19" s="319"/>
-      <c r="L19" s="319"/>
-      <c r="M19" s="319"/>
+      <c r="D19" s="325"/>
+      <c r="E19" s="325"/>
+      <c r="F19" s="325"/>
+      <c r="G19" s="325"/>
+      <c r="H19" s="325"/>
+      <c r="I19" s="325"/>
+      <c r="J19" s="325"/>
+      <c r="K19" s="325"/>
+      <c r="L19" s="325"/>
+      <c r="M19" s="325"/>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B20" s="258"/>
-      <c r="C20" s="319" t="s">
+      <c r="C20" s="325" t="s">
         <v>363</v>
       </c>
-      <c r="D20" s="319"/>
-      <c r="E20" s="319"/>
-      <c r="F20" s="319"/>
-      <c r="G20" s="319"/>
-      <c r="H20" s="319"/>
-      <c r="I20" s="319"/>
-      <c r="J20" s="319"/>
-      <c r="K20" s="319"/>
-      <c r="L20" s="319"/>
-      <c r="M20" s="319"/>
+      <c r="D20" s="325"/>
+      <c r="E20" s="325"/>
+      <c r="F20" s="325"/>
+      <c r="G20" s="325"/>
+      <c r="H20" s="325"/>
+      <c r="I20" s="325"/>
+      <c r="J20" s="325"/>
+      <c r="K20" s="325"/>
+      <c r="L20" s="325"/>
+      <c r="M20" s="325"/>
     </row>
     <row r="21" spans="2:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B21" s="258"/>
-      <c r="C21" s="319" t="s">
+      <c r="C21" s="325" t="s">
         <v>462</v>
       </c>
-      <c r="D21" s="319"/>
-      <c r="E21" s="319"/>
-      <c r="F21" s="319"/>
-      <c r="G21" s="319"/>
-      <c r="H21" s="319"/>
-      <c r="I21" s="319"/>
-      <c r="J21" s="319"/>
-      <c r="K21" s="319"/>
-      <c r="L21" s="319"/>
-      <c r="M21" s="319"/>
+      <c r="D21" s="325"/>
+      <c r="E21" s="325"/>
+      <c r="F21" s="325"/>
+      <c r="G21" s="325"/>
+      <c r="H21" s="325"/>
+      <c r="I21" s="325"/>
+      <c r="J21" s="325"/>
+      <c r="K21" s="325"/>
+      <c r="L21" s="325"/>
+      <c r="M21" s="325"/>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B22" s="258"/>
-      <c r="C22" s="319" t="s">
+      <c r="C22" s="325" t="s">
         <v>458</v>
       </c>
-      <c r="D22" s="319"/>
-      <c r="E22" s="319"/>
-      <c r="F22" s="319"/>
-      <c r="G22" s="319"/>
-      <c r="H22" s="319"/>
-      <c r="I22" s="319"/>
-      <c r="J22" s="319"/>
-      <c r="K22" s="319"/>
-      <c r="L22" s="319"/>
-      <c r="M22" s="319"/>
+      <c r="D22" s="325"/>
+      <c r="E22" s="325"/>
+      <c r="F22" s="325"/>
+      <c r="G22" s="325"/>
+      <c r="H22" s="325"/>
+      <c r="I22" s="325"/>
+      <c r="J22" s="325"/>
+      <c r="K22" s="325"/>
+      <c r="L22" s="325"/>
+      <c r="M22" s="325"/>
     </row>
     <row r="23" spans="2:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B23" s="258"/>
       <c r="C23" s="258"/>
-      <c r="D23" s="319" t="s">
+      <c r="D23" s="325" t="s">
         <v>454</v>
       </c>
-      <c r="E23" s="319"/>
-      <c r="F23" s="319"/>
-      <c r="G23" s="319"/>
-      <c r="H23" s="319"/>
-      <c r="I23" s="319"/>
-      <c r="J23" s="319"/>
-      <c r="K23" s="319"/>
-      <c r="L23" s="319"/>
-      <c r="M23" s="319"/>
+      <c r="E23" s="325"/>
+      <c r="F23" s="325"/>
+      <c r="G23" s="325"/>
+      <c r="H23" s="325"/>
+      <c r="I23" s="325"/>
+      <c r="J23" s="325"/>
+      <c r="K23" s="325"/>
+      <c r="L23" s="325"/>
+      <c r="M23" s="325"/>
     </row>
     <row r="24" spans="2:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B24" s="258"/>
       <c r="C24" s="258"/>
-      <c r="D24" s="319" t="s">
+      <c r="D24" s="325" t="s">
         <v>455</v>
       </c>
-      <c r="E24" s="319"/>
-      <c r="F24" s="319"/>
-      <c r="G24" s="319"/>
-      <c r="H24" s="319"/>
-      <c r="I24" s="319"/>
-      <c r="J24" s="319"/>
-      <c r="K24" s="319"/>
-      <c r="L24" s="319"/>
-      <c r="M24" s="319"/>
+      <c r="E24" s="325"/>
+      <c r="F24" s="325"/>
+      <c r="G24" s="325"/>
+      <c r="H24" s="325"/>
+      <c r="I24" s="325"/>
+      <c r="J24" s="325"/>
+      <c r="K24" s="325"/>
+      <c r="L24" s="325"/>
+      <c r="M24" s="325"/>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B25" s="255"/>
       <c r="C25" s="256"/>
-      <c r="D25" s="320" t="s">
+      <c r="D25" s="321" t="s">
         <v>456</v>
       </c>
-      <c r="E25" s="320"/>
-      <c r="F25" s="320"/>
-      <c r="G25" s="320"/>
-      <c r="H25" s="320"/>
-      <c r="I25" s="320"/>
-      <c r="J25" s="320"/>
-      <c r="K25" s="320"/>
-      <c r="L25" s="320"/>
-      <c r="M25" s="320"/>
+      <c r="E25" s="321"/>
+      <c r="F25" s="321"/>
+      <c r="G25" s="321"/>
+      <c r="H25" s="321"/>
+      <c r="I25" s="321"/>
+      <c r="J25" s="321"/>
+      <c r="K25" s="321"/>
+      <c r="L25" s="321"/>
+      <c r="M25" s="321"/>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B26" s="255"/>
       <c r="C26" s="256"/>
-      <c r="D26" s="319" t="s">
+      <c r="D26" s="325" t="s">
         <v>457</v>
       </c>
-      <c r="E26" s="319"/>
-      <c r="F26" s="319"/>
-      <c r="G26" s="319"/>
-      <c r="H26" s="319"/>
-      <c r="I26" s="319"/>
-      <c r="J26" s="319"/>
-      <c r="K26" s="319"/>
-      <c r="L26" s="319"/>
-      <c r="M26" s="319"/>
+      <c r="E26" s="325"/>
+      <c r="F26" s="325"/>
+      <c r="G26" s="325"/>
+      <c r="H26" s="325"/>
+      <c r="I26" s="325"/>
+      <c r="J26" s="325"/>
+      <c r="K26" s="325"/>
+      <c r="L26" s="325"/>
+      <c r="M26" s="325"/>
     </row>
     <row r="27" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="324" t="s">
+      <c r="B27" s="322" t="s">
         <v>364</v>
       </c>
-      <c r="C27" s="325"/>
-      <c r="D27" s="325"/>
-      <c r="E27" s="325"/>
-      <c r="F27" s="325"/>
-      <c r="G27" s="325"/>
-      <c r="H27" s="325"/>
-      <c r="I27" s="325"/>
-      <c r="J27" s="325"/>
-      <c r="K27" s="325"/>
-      <c r="L27" s="325"/>
-      <c r="M27" s="325"/>
+      <c r="C27" s="319"/>
+      <c r="D27" s="319"/>
+      <c r="E27" s="319"/>
+      <c r="F27" s="319"/>
+      <c r="G27" s="319"/>
+      <c r="H27" s="319"/>
+      <c r="I27" s="319"/>
+      <c r="J27" s="319"/>
+      <c r="K27" s="319"/>
+      <c r="L27" s="319"/>
+      <c r="M27" s="319"/>
     </row>
     <row r="28" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="324" t="s">
+      <c r="B28" s="322" t="s">
         <v>365</v>
       </c>
-      <c r="C28" s="325"/>
-      <c r="D28" s="325"/>
-      <c r="E28" s="325"/>
-      <c r="F28" s="325"/>
-      <c r="G28" s="325"/>
-      <c r="H28" s="325"/>
-      <c r="I28" s="325"/>
-      <c r="J28" s="325"/>
-      <c r="K28" s="325"/>
-      <c r="L28" s="325"/>
-      <c r="M28" s="325"/>
+      <c r="C28" s="319"/>
+      <c r="D28" s="319"/>
+      <c r="E28" s="319"/>
+      <c r="F28" s="319"/>
+      <c r="G28" s="319"/>
+      <c r="H28" s="319"/>
+      <c r="I28" s="319"/>
+      <c r="J28" s="319"/>
+      <c r="K28" s="319"/>
+      <c r="L28" s="319"/>
+      <c r="M28" s="319"/>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B29" s="199"/>
     </row>
     <row r="30" spans="2:13" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="B30" s="323" t="s">
+      <c r="B30" s="320" t="s">
         <v>345</v>
       </c>
-      <c r="C30" s="323"/>
-      <c r="D30" s="323"/>
-      <c r="E30" s="323"/>
-      <c r="F30" s="323"/>
-      <c r="G30" s="323"/>
-      <c r="H30" s="323"/>
-      <c r="I30" s="323"/>
-      <c r="J30" s="323"/>
-      <c r="K30" s="323"/>
-      <c r="L30" s="323"/>
-      <c r="M30" s="323"/>
+      <c r="C30" s="320"/>
+      <c r="D30" s="320"/>
+      <c r="E30" s="320"/>
+      <c r="F30" s="320"/>
+      <c r="G30" s="320"/>
+      <c r="H30" s="320"/>
+      <c r="I30" s="320"/>
+      <c r="J30" s="320"/>
+      <c r="K30" s="320"/>
+      <c r="L30" s="320"/>
+      <c r="M30" s="320"/>
     </row>
     <row r="31" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="320" t="s">
+      <c r="B31" s="321" t="s">
         <v>370</v>
       </c>
-      <c r="C31" s="320"/>
-      <c r="D31" s="320"/>
-      <c r="E31" s="320"/>
-      <c r="F31" s="320"/>
-      <c r="G31" s="320"/>
-      <c r="H31" s="320"/>
-      <c r="I31" s="320"/>
-      <c r="J31" s="320"/>
-      <c r="K31" s="320"/>
-      <c r="L31" s="320"/>
-      <c r="M31" s="320"/>
+      <c r="C31" s="321"/>
+      <c r="D31" s="321"/>
+      <c r="E31" s="321"/>
+      <c r="F31" s="321"/>
+      <c r="G31" s="321"/>
+      <c r="H31" s="321"/>
+      <c r="I31" s="321"/>
+      <c r="J31" s="321"/>
+      <c r="K31" s="321"/>
+      <c r="L31" s="321"/>
+      <c r="M31" s="321"/>
     </row>
     <row r="32" spans="2:13" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="320" t="s">
+      <c r="B32" s="321" t="s">
         <v>346</v>
       </c>
-      <c r="C32" s="320"/>
-      <c r="D32" s="320"/>
-      <c r="E32" s="320"/>
-      <c r="F32" s="320"/>
-      <c r="G32" s="320"/>
-      <c r="H32" s="320"/>
-      <c r="I32" s="320"/>
-      <c r="J32" s="320"/>
-      <c r="K32" s="320"/>
-      <c r="L32" s="320"/>
-      <c r="M32" s="320"/>
+      <c r="C32" s="321"/>
+      <c r="D32" s="321"/>
+      <c r="E32" s="321"/>
+      <c r="F32" s="321"/>
+      <c r="G32" s="321"/>
+      <c r="H32" s="321"/>
+      <c r="I32" s="321"/>
+      <c r="J32" s="321"/>
+      <c r="K32" s="321"/>
+      <c r="L32" s="321"/>
+      <c r="M32" s="321"/>
     </row>
     <row r="33" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B33" s="320" t="s">
+      <c r="B33" s="321" t="s">
         <v>347</v>
       </c>
-      <c r="C33" s="320"/>
-      <c r="D33" s="320"/>
-      <c r="E33" s="320"/>
-      <c r="F33" s="320"/>
-      <c r="G33" s="320"/>
-      <c r="H33" s="320"/>
-      <c r="I33" s="320"/>
-      <c r="J33" s="320"/>
-      <c r="K33" s="320"/>
-      <c r="L33" s="320"/>
-      <c r="M33" s="320"/>
+      <c r="C33" s="321"/>
+      <c r="D33" s="321"/>
+      <c r="E33" s="321"/>
+      <c r="F33" s="321"/>
+      <c r="G33" s="321"/>
+      <c r="H33" s="321"/>
+      <c r="I33" s="321"/>
+      <c r="J33" s="321"/>
+      <c r="K33" s="321"/>
+      <c r="L33" s="321"/>
+      <c r="M33" s="321"/>
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B34" s="320" t="s">
+      <c r="B34" s="321" t="s">
         <v>348</v>
       </c>
-      <c r="C34" s="320"/>
-      <c r="D34" s="320"/>
-      <c r="E34" s="320"/>
-      <c r="F34" s="320"/>
-      <c r="G34" s="320"/>
-      <c r="H34" s="320"/>
-      <c r="I34" s="320"/>
-      <c r="J34" s="320"/>
-      <c r="K34" s="320"/>
-      <c r="L34" s="320"/>
-      <c r="M34" s="320"/>
+      <c r="C34" s="321"/>
+      <c r="D34" s="321"/>
+      <c r="E34" s="321"/>
+      <c r="F34" s="321"/>
+      <c r="G34" s="321"/>
+      <c r="H34" s="321"/>
+      <c r="I34" s="321"/>
+      <c r="J34" s="321"/>
+      <c r="K34" s="321"/>
+      <c r="L34" s="321"/>
+      <c r="M34" s="321"/>
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B35" s="320" t="s">
+      <c r="B35" s="321" t="s">
         <v>349</v>
       </c>
-      <c r="C35" s="320"/>
-      <c r="D35" s="320"/>
-      <c r="E35" s="320"/>
-      <c r="F35" s="320"/>
-      <c r="G35" s="320"/>
-      <c r="H35" s="320"/>
-      <c r="I35" s="320"/>
-      <c r="J35" s="320"/>
-      <c r="K35" s="320"/>
-      <c r="L35" s="320"/>
-      <c r="M35" s="320"/>
+      <c r="C35" s="321"/>
+      <c r="D35" s="321"/>
+      <c r="E35" s="321"/>
+      <c r="F35" s="321"/>
+      <c r="G35" s="321"/>
+      <c r="H35" s="321"/>
+      <c r="I35" s="321"/>
+      <c r="J35" s="321"/>
+      <c r="K35" s="321"/>
+      <c r="L35" s="321"/>
+      <c r="M35" s="321"/>
     </row>
     <row r="36" spans="2:13" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="B36" s="323" t="s">
+      <c r="B36" s="320" t="s">
         <v>350</v>
       </c>
-      <c r="C36" s="323"/>
-      <c r="D36" s="323"/>
-      <c r="E36" s="323"/>
-      <c r="F36" s="323"/>
-      <c r="G36" s="323"/>
-      <c r="H36" s="323"/>
-      <c r="I36" s="323"/>
-      <c r="J36" s="323"/>
-      <c r="K36" s="323"/>
-      <c r="L36" s="323"/>
-      <c r="M36" s="323"/>
+      <c r="C36" s="320"/>
+      <c r="D36" s="320"/>
+      <c r="E36" s="320"/>
+      <c r="F36" s="320"/>
+      <c r="G36" s="320"/>
+      <c r="H36" s="320"/>
+      <c r="I36" s="320"/>
+      <c r="J36" s="320"/>
+      <c r="K36" s="320"/>
+      <c r="L36" s="320"/>
+      <c r="M36" s="320"/>
     </row>
     <row r="37" spans="2:13" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B37" s="320" t="s">
+      <c r="B37" s="321" t="s">
         <v>351</v>
       </c>
-      <c r="C37" s="320"/>
-      <c r="D37" s="320"/>
-      <c r="E37" s="320"/>
-      <c r="F37" s="320"/>
-      <c r="G37" s="320"/>
-      <c r="H37" s="320"/>
-      <c r="I37" s="320"/>
-      <c r="J37" s="320"/>
-      <c r="K37" s="320"/>
-      <c r="L37" s="320"/>
-      <c r="M37" s="320"/>
+      <c r="C37" s="321"/>
+      <c r="D37" s="321"/>
+      <c r="E37" s="321"/>
+      <c r="F37" s="321"/>
+      <c r="G37" s="321"/>
+      <c r="H37" s="321"/>
+      <c r="I37" s="321"/>
+      <c r="J37" s="321"/>
+      <c r="K37" s="321"/>
+      <c r="L37" s="321"/>
+      <c r="M37" s="321"/>
     </row>
     <row r="38" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B38" s="320" t="s">
+      <c r="B38" s="321" t="s">
         <v>352</v>
       </c>
-      <c r="C38" s="320"/>
-      <c r="D38" s="320"/>
-      <c r="E38" s="320"/>
-      <c r="F38" s="320"/>
-      <c r="G38" s="320"/>
-      <c r="H38" s="320"/>
-      <c r="I38" s="320"/>
-      <c r="J38" s="320"/>
-      <c r="K38" s="320"/>
-      <c r="L38" s="320"/>
-      <c r="M38" s="320"/>
+      <c r="C38" s="321"/>
+      <c r="D38" s="321"/>
+      <c r="E38" s="321"/>
+      <c r="F38" s="321"/>
+      <c r="G38" s="321"/>
+      <c r="H38" s="321"/>
+      <c r="I38" s="321"/>
+      <c r="J38" s="321"/>
+      <c r="K38" s="321"/>
+      <c r="L38" s="321"/>
+      <c r="M38" s="321"/>
     </row>
     <row r="39" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B39" s="199"/>
     </row>
     <row r="40" spans="2:13" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="B40" s="323" t="s">
+      <c r="B40" s="320" t="s">
         <v>353</v>
       </c>
-      <c r="C40" s="323"/>
-      <c r="D40" s="323"/>
-      <c r="E40" s="323"/>
-      <c r="F40" s="323"/>
-      <c r="G40" s="323"/>
-      <c r="H40" s="323"/>
-      <c r="I40" s="323"/>
-      <c r="J40" s="323"/>
-      <c r="K40" s="323"/>
-      <c r="L40" s="323"/>
-      <c r="M40" s="323"/>
+      <c r="C40" s="320"/>
+      <c r="D40" s="320"/>
+      <c r="E40" s="320"/>
+      <c r="F40" s="320"/>
+      <c r="G40" s="320"/>
+      <c r="H40" s="320"/>
+      <c r="I40" s="320"/>
+      <c r="J40" s="320"/>
+      <c r="K40" s="320"/>
+      <c r="L40" s="320"/>
+      <c r="M40" s="320"/>
     </row>
     <row r="41" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B41" s="322" t="s">
+      <c r="B41" s="327" t="s">
         <v>354</v>
       </c>
-      <c r="C41" s="322"/>
-      <c r="D41" s="322"/>
-      <c r="E41" s="322"/>
-      <c r="F41" s="322"/>
-      <c r="G41" s="322"/>
-      <c r="H41" s="322"/>
-      <c r="I41" s="322"/>
-      <c r="J41" s="322"/>
-      <c r="K41" s="322"/>
-      <c r="L41" s="322"/>
-      <c r="M41" s="322"/>
+      <c r="C41" s="327"/>
+      <c r="D41" s="327"/>
+      <c r="E41" s="327"/>
+      <c r="F41" s="327"/>
+      <c r="G41" s="327"/>
+      <c r="H41" s="327"/>
+      <c r="I41" s="327"/>
+      <c r="J41" s="327"/>
+      <c r="K41" s="327"/>
+      <c r="L41" s="327"/>
+      <c r="M41" s="327"/>
     </row>
     <row r="42" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B42" s="322" t="s">
+      <c r="B42" s="327" t="s">
         <v>355</v>
       </c>
-      <c r="C42" s="322"/>
-      <c r="D42" s="322"/>
-      <c r="E42" s="322"/>
-      <c r="F42" s="322"/>
-      <c r="G42" s="322"/>
-      <c r="H42" s="322"/>
-      <c r="I42" s="322"/>
-      <c r="J42" s="322"/>
-      <c r="K42" s="322"/>
-      <c r="L42" s="322"/>
-      <c r="M42" s="322"/>
+      <c r="C42" s="327"/>
+      <c r="D42" s="327"/>
+      <c r="E42" s="327"/>
+      <c r="F42" s="327"/>
+      <c r="G42" s="327"/>
+      <c r="H42" s="327"/>
+      <c r="I42" s="327"/>
+      <c r="J42" s="327"/>
+      <c r="K42" s="327"/>
+      <c r="L42" s="327"/>
+      <c r="M42" s="327"/>
     </row>
     <row r="43" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B43" s="322" t="s">
+      <c r="B43" s="327" t="s">
         <v>356</v>
       </c>
-      <c r="C43" s="322"/>
-      <c r="D43" s="322"/>
-      <c r="E43" s="322"/>
-      <c r="F43" s="322"/>
-      <c r="G43" s="322"/>
-      <c r="H43" s="322"/>
-      <c r="I43" s="322"/>
-      <c r="J43" s="322"/>
-      <c r="K43" s="322"/>
-      <c r="L43" s="322"/>
-      <c r="M43" s="322"/>
+      <c r="C43" s="327"/>
+      <c r="D43" s="327"/>
+      <c r="E43" s="327"/>
+      <c r="F43" s="327"/>
+      <c r="G43" s="327"/>
+      <c r="H43" s="327"/>
+      <c r="I43" s="327"/>
+      <c r="J43" s="327"/>
+      <c r="K43" s="327"/>
+      <c r="L43" s="327"/>
+      <c r="M43" s="327"/>
     </row>
     <row r="44" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B44" s="249" t="s">
@@ -9599,82 +8591,55 @@
       <c r="M44" s="247"/>
     </row>
     <row r="45" spans="2:13" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="B45" s="323" t="s">
+      <c r="B45" s="320" t="s">
         <v>357</v>
       </c>
-      <c r="C45" s="323"/>
-      <c r="D45" s="323"/>
-      <c r="E45" s="323"/>
-      <c r="F45" s="323"/>
-      <c r="G45" s="323"/>
-      <c r="H45" s="323"/>
-      <c r="I45" s="323"/>
-      <c r="J45" s="323"/>
-      <c r="K45" s="323"/>
-      <c r="L45" s="323"/>
-      <c r="M45" s="323"/>
+      <c r="C45" s="320"/>
+      <c r="D45" s="320"/>
+      <c r="E45" s="320"/>
+      <c r="F45" s="320"/>
+      <c r="G45" s="320"/>
+      <c r="H45" s="320"/>
+      <c r="I45" s="320"/>
+      <c r="J45" s="320"/>
+      <c r="K45" s="320"/>
+      <c r="L45" s="320"/>
+      <c r="M45" s="320"/>
     </row>
     <row r="46" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B46" s="320" t="s">
+      <c r="B46" s="321" t="s">
         <v>461</v>
       </c>
-      <c r="C46" s="320"/>
-      <c r="D46" s="320"/>
-      <c r="E46" s="320"/>
-      <c r="F46" s="320"/>
-      <c r="G46" s="320"/>
-      <c r="H46" s="320"/>
-      <c r="I46" s="320"/>
-      <c r="J46" s="320"/>
-      <c r="K46" s="320"/>
-      <c r="L46" s="320"/>
-      <c r="M46" s="320"/>
+      <c r="C46" s="321"/>
+      <c r="D46" s="321"/>
+      <c r="E46" s="321"/>
+      <c r="F46" s="321"/>
+      <c r="G46" s="321"/>
+      <c r="H46" s="321"/>
+      <c r="I46" s="321"/>
+      <c r="J46" s="321"/>
+      <c r="K46" s="321"/>
+      <c r="L46" s="321"/>
+      <c r="M46" s="321"/>
     </row>
     <row r="47" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B47" s="321" t="s">
+      <c r="B47" s="326" t="s">
         <v>447</v>
       </c>
-      <c r="C47" s="321"/>
-      <c r="D47" s="321"/>
-      <c r="E47" s="321"/>
-      <c r="F47" s="321"/>
-      <c r="G47" s="321"/>
-      <c r="H47" s="321"/>
-      <c r="I47" s="321"/>
-      <c r="J47" s="321"/>
-      <c r="K47" s="321"/>
-      <c r="L47" s="321"/>
-      <c r="M47" s="321"/>
+      <c r="C47" s="326"/>
+      <c r="D47" s="326"/>
+      <c r="E47" s="326"/>
+      <c r="F47" s="326"/>
+      <c r="G47" s="326"/>
+      <c r="H47" s="326"/>
+      <c r="I47" s="326"/>
+      <c r="J47" s="326"/>
+      <c r="K47" s="326"/>
+      <c r="L47" s="326"/>
+      <c r="M47" s="326"/>
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="B7:M7"/>
-    <mergeCell ref="B8:M8"/>
-    <mergeCell ref="B11:M11"/>
-    <mergeCell ref="B12:M12"/>
-    <mergeCell ref="B13:M13"/>
-    <mergeCell ref="B2:M2"/>
-    <mergeCell ref="B3:M3"/>
-    <mergeCell ref="B4:M4"/>
-    <mergeCell ref="B5:M5"/>
-    <mergeCell ref="B6:M6"/>
-    <mergeCell ref="C21:M21"/>
-    <mergeCell ref="C22:M22"/>
-    <mergeCell ref="B15:M15"/>
-    <mergeCell ref="B9:L9"/>
-    <mergeCell ref="B10:L10"/>
-    <mergeCell ref="B14:M14"/>
-    <mergeCell ref="B16:M16"/>
-    <mergeCell ref="B17:M17"/>
-    <mergeCell ref="B18:M18"/>
-    <mergeCell ref="C19:M19"/>
-    <mergeCell ref="C20:M20"/>
-    <mergeCell ref="B33:M33"/>
-    <mergeCell ref="B34:M34"/>
-    <mergeCell ref="B35:M35"/>
-    <mergeCell ref="B27:M27"/>
-    <mergeCell ref="B28:M28"/>
-    <mergeCell ref="B30:M30"/>
     <mergeCell ref="D23:M23"/>
     <mergeCell ref="D24:M24"/>
     <mergeCell ref="D25:M25"/>
@@ -9691,6 +8656,33 @@
     <mergeCell ref="B41:M41"/>
     <mergeCell ref="B31:M31"/>
     <mergeCell ref="B32:M32"/>
+    <mergeCell ref="B33:M33"/>
+    <mergeCell ref="B34:M34"/>
+    <mergeCell ref="B35:M35"/>
+    <mergeCell ref="B27:M27"/>
+    <mergeCell ref="B28:M28"/>
+    <mergeCell ref="B30:M30"/>
+    <mergeCell ref="C21:M21"/>
+    <mergeCell ref="C22:M22"/>
+    <mergeCell ref="B15:M15"/>
+    <mergeCell ref="B9:L9"/>
+    <mergeCell ref="B10:L10"/>
+    <mergeCell ref="B14:M14"/>
+    <mergeCell ref="B16:M16"/>
+    <mergeCell ref="B17:M17"/>
+    <mergeCell ref="B18:M18"/>
+    <mergeCell ref="C19:M19"/>
+    <mergeCell ref="C20:M20"/>
+    <mergeCell ref="B2:M2"/>
+    <mergeCell ref="B3:M3"/>
+    <mergeCell ref="B4:M4"/>
+    <mergeCell ref="B5:M5"/>
+    <mergeCell ref="B6:M6"/>
+    <mergeCell ref="B7:M7"/>
+    <mergeCell ref="B8:M8"/>
+    <mergeCell ref="B11:M11"/>
+    <mergeCell ref="B12:M12"/>
+    <mergeCell ref="B13:M13"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B41" r:id="rId1" display="https://cdn.who.int/media/docs/default-source/documents/about-us/thirteenth-general-programme/gpw13_methodology_nov9_online-version1b3170f8-98ea-4fcc-aa3a-059ede7e51ad.pdf?sfvrsn=12dfeb0d_1&amp;download=true" xr:uid="{5B1AD3AB-AC30-4E70-9D4E-7E9B49DF39DD}"/>
@@ -13829,40 +12821,40 @@
       <c r="Z8" s="13"/>
     </row>
     <row r="9" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="354" t="s">
+      <c r="A9" s="357" t="s">
         <v>77</v>
       </c>
-      <c r="B9" s="354"/>
-      <c r="C9" s="361" t="s">
+      <c r="B9" s="357"/>
+      <c r="C9" s="362" t="s">
         <v>80</v>
       </c>
-      <c r="D9" s="361"/>
-      <c r="E9" s="361"/>
-      <c r="F9" s="361"/>
-      <c r="G9" s="361"/>
-      <c r="H9" s="361"/>
-      <c r="I9" s="361"/>
+      <c r="D9" s="362"/>
+      <c r="E9" s="362"/>
+      <c r="F9" s="362"/>
+      <c r="G9" s="362"/>
+      <c r="H9" s="362"/>
+      <c r="I9" s="362"/>
       <c r="J9" s="29"/>
-      <c r="K9" s="362" t="s">
+      <c r="K9" s="363" t="s">
         <v>78</v>
       </c>
-      <c r="L9" s="362"/>
-      <c r="M9" s="362"/>
-      <c r="N9" s="362"/>
-      <c r="O9" s="362"/>
-      <c r="P9" s="362"/>
-      <c r="Q9" s="362"/>
-      <c r="R9" s="362"/>
-      <c r="S9" s="362"/>
-      <c r="T9" s="362"/>
-      <c r="U9" s="362"/>
+      <c r="L9" s="363"/>
+      <c r="M9" s="363"/>
+      <c r="N9" s="363"/>
+      <c r="O9" s="363"/>
+      <c r="P9" s="363"/>
+      <c r="Q9" s="363"/>
+      <c r="R9" s="363"/>
+      <c r="S9" s="363"/>
+      <c r="T9" s="363"/>
+      <c r="U9" s="363"/>
       <c r="V9" s="29"/>
-      <c r="W9" s="358" t="s">
+      <c r="W9" s="359" t="s">
         <v>79</v>
       </c>
-      <c r="X9" s="359"/>
-      <c r="Y9" s="359"/>
-      <c r="Z9" s="360"/>
+      <c r="X9" s="360"/>
+      <c r="Y9" s="360"/>
+      <c r="Z9" s="361"/>
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A10" s="355" t="s">
@@ -13886,48 +12878,48 @@
       <c r="G10" s="355" t="s">
         <v>85</v>
       </c>
-      <c r="H10" s="363" t="s">
+      <c r="H10" s="364" t="s">
         <v>113</v>
       </c>
-      <c r="I10" s="363" t="s">
+      <c r="I10" s="364" t="s">
         <v>114</v>
       </c>
       <c r="J10" s="30"/>
-      <c r="K10" s="364" t="s">
+      <c r="K10" s="354" t="s">
         <v>81</v>
       </c>
-      <c r="L10" s="364" t="s">
+      <c r="L10" s="354" t="s">
         <v>82</v>
       </c>
       <c r="M10" s="78"/>
-      <c r="N10" s="364" t="s">
+      <c r="N10" s="354" t="s">
         <v>83</v>
       </c>
-      <c r="O10" s="364" t="s">
+      <c r="O10" s="354" t="s">
         <v>82</v>
       </c>
       <c r="P10" s="78"/>
-      <c r="Q10" s="364" t="s">
+      <c r="Q10" s="354" t="s">
         <v>84</v>
       </c>
-      <c r="R10" s="364" t="s">
+      <c r="R10" s="354" t="s">
         <v>82</v>
       </c>
       <c r="S10" s="78"/>
-      <c r="T10" s="364" t="s">
+      <c r="T10" s="354" t="s">
         <v>85</v>
       </c>
-      <c r="U10" s="364" t="s">
+      <c r="U10" s="354" t="s">
         <v>82</v>
       </c>
       <c r="V10" s="30"/>
-      <c r="W10" s="357" t="s">
+      <c r="W10" s="358" t="s">
         <v>118</v>
       </c>
-      <c r="X10" s="357" t="s">
+      <c r="X10" s="358" t="s">
         <v>115</v>
       </c>
-      <c r="Y10" s="357" t="s">
+      <c r="Y10" s="358" t="s">
         <v>116</v>
       </c>
       <c r="Z10" s="355" t="s">
@@ -15741,11 +14733,6 @@
     <row r="76" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="T10:U10"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="G10:G11"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="Y10:Y11"/>
@@ -15762,6 +14749,11 @@
     <mergeCell ref="K10:L10"/>
     <mergeCell ref="N10:O10"/>
     <mergeCell ref="Q10:R10"/>
+    <mergeCell ref="T10:U10"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="G10:G11"/>
   </mergeCells>
   <conditionalFormatting sqref="E12:E28">
     <cfRule type="expression" dxfId="1" priority="2">
@@ -17106,7 +16098,7 @@
   <dimension ref="A1:V75"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" outlineLevelRow="1" x14ac:dyDescent="0.35"/>
@@ -28052,11 +27044,9 @@
         <v>1</v>
       </c>
       <c r="C3" s="50">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!L$1:L$101,MATCH([1]UHC_Inter!$A3,[1]UHC_summary!$B$1:$B$101,0))=0,INDEX([1]UHC_summary!I$1:I$101,MATCH([1]UHC_Inter!$A3,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!L$1:L$101,MATCH([1]UHC_Inter!$A3,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>56.35</v>
       </c>
       <c r="D3" s="50">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!M$1:M$101,MATCH([1]UHC_Inter!$A3,[1]UHC_summary!$B$1:$B$101,0))=0,INDEX([1]UHC_summary!J$1:J$101,MATCH([1]UHC_Inter!$A3,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!M$1:M$101,MATCH([1]UHC_Inter!$A3,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>60.55</v>
       </c>
       <c r="E3" s="50">
@@ -28076,16 +27066,13 @@
         <v>#N/A</v>
       </c>
       <c r="I3" s="50">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!D$1:D$101,MATCH([1]UHC_Inter!$A3,[1]UHC_summary!$B$1:$B$101,0))="",INDEX([1]UHC_summary!C$1:C$101,MATCH([1]UHC_Inter!$A3,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!D$1:D$101,MATCH([1]UHC_Inter!$A3,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>57.99</v>
       </c>
       <c r="J3" s="198">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!E$1:E$101,MATCH([1]UHC_Inter!$A3,[1]UHC_summary!$B$1:$B$101,0))=0,"",INDEX([1]UHC_summary!E$1:E$101,MATCH([1]UHC_Inter!$A3,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>2020</v>
       </c>
-      <c r="K3" t="str">
-        <f>INDEX([1]UHC_summary!D$1:D$101,MATCH([1]UHC_Inter!$A3,[1]UHC_summary!$B$1:$B$101,0))</f>
-        <v/>
+      <c r="K3" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
@@ -28096,11 +27083,9 @@
         <v>2</v>
       </c>
       <c r="C4" s="50">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!L$1:L$101,MATCH([1]UHC_Inter!$A4,[1]UHC_summary!$B$1:$B$101,0))=0,INDEX([1]UHC_summary!I$1:I$101,MATCH([1]UHC_Inter!$A4,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!L$1:L$101,MATCH([1]UHC_Inter!$A4,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>98.58</v>
       </c>
       <c r="D4" s="50">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!M$1:M$101,MATCH([1]UHC_Inter!$A4,[1]UHC_summary!$B$1:$B$101,0))=0,INDEX([1]UHC_summary!J$1:J$101,MATCH([1]UHC_Inter!$A4,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!M$1:M$101,MATCH([1]UHC_Inter!$A4,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>98.46</v>
       </c>
       <c r="E4" s="50" t="e">
@@ -28120,12 +27105,10 @@
         <v>0.12000000000000455</v>
       </c>
       <c r="I4" s="50">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!D$1:D$101,MATCH([1]UHC_Inter!$A4,[1]UHC_summary!$B$1:$B$101,0))="",INDEX([1]UHC_summary!C$1:C$101,MATCH([1]UHC_Inter!$A4,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!D$1:D$101,MATCH([1]UHC_Inter!$A4,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>0</v>
       </c>
-      <c r="J4" s="198" t="str">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!E$1:E$101,MATCH([1]UHC_Inter!$A4,[1]UHC_summary!$B$1:$B$101,0))=0,"",INDEX([1]UHC_summary!E$1:E$101,MATCH([1]UHC_Inter!$A4,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
-        <v/>
+      <c r="J4" s="198" t="s">
+        <v>82</v>
       </c>
       <c r="L4" s="21"/>
     </row>
@@ -28137,11 +27120,9 @@
         <v>3</v>
       </c>
       <c r="C5" s="50">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!L$1:L$101,MATCH([1]UHC_Inter!$A5,[1]UHC_summary!$B$1:$B$101,0))=0,INDEX([1]UHC_summary!I$1:I$101,MATCH([1]UHC_Inter!$A5,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!L$1:L$101,MATCH([1]UHC_Inter!$A5,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>98</v>
       </c>
       <c r="D5" s="50">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!M$1:M$101,MATCH([1]UHC_Inter!$A5,[1]UHC_summary!$B$1:$B$101,0))=0,INDEX([1]UHC_summary!J$1:J$101,MATCH([1]UHC_Inter!$A5,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!M$1:M$101,MATCH([1]UHC_Inter!$A5,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>98.54</v>
       </c>
       <c r="E5" s="50">
@@ -28161,11 +27142,9 @@
         <v>#N/A</v>
       </c>
       <c r="I5" s="50">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!D$1:D$101,MATCH([1]UHC_Inter!$A5,[1]UHC_summary!$B$1:$B$101,0))="",INDEX([1]UHC_summary!C$1:C$101,MATCH([1]UHC_Inter!$A5,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!D$1:D$101,MATCH([1]UHC_Inter!$A5,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>98</v>
       </c>
       <c r="J5" s="198">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!E$1:E$101,MATCH([1]UHC_Inter!$A5,[1]UHC_summary!$B$1:$B$101,0))=0,"",INDEX([1]UHC_summary!E$1:E$101,MATCH([1]UHC_Inter!$A5,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>2019</v>
       </c>
     </row>
@@ -28177,11 +27156,9 @@
         <v>4</v>
       </c>
       <c r="C6" s="50">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!L$1:L$101,MATCH([1]UHC_Inter!$A6,[1]UHC_summary!$B$1:$B$101,0))=0,INDEX([1]UHC_summary!I$1:I$101,MATCH([1]UHC_Inter!$A6,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!L$1:L$101,MATCH([1]UHC_Inter!$A6,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>89.91</v>
       </c>
       <c r="D6" s="50">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!M$1:M$101,MATCH([1]UHC_Inter!$A6,[1]UHC_summary!$B$1:$B$101,0))=0,INDEX([1]UHC_summary!J$1:J$101,MATCH([1]UHC_Inter!$A6,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!M$1:M$101,MATCH([1]UHC_Inter!$A6,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>90.82</v>
       </c>
       <c r="E6" s="50">
@@ -28201,12 +27178,10 @@
         <v>#N/A</v>
       </c>
       <c r="I6" s="50">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!D$1:D$101,MATCH([1]UHC_Inter!$A6,[1]UHC_summary!$B$1:$B$101,0))="",INDEX([1]UHC_summary!C$1:C$101,MATCH([1]UHC_Inter!$A6,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!D$1:D$101,MATCH([1]UHC_Inter!$A6,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>0</v>
       </c>
-      <c r="J6" s="198" t="str">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!E$1:E$101,MATCH([1]UHC_Inter!$A6,[1]UHC_summary!$B$1:$B$101,0))=0,"",INDEX([1]UHC_summary!E$1:E$101,MATCH([1]UHC_Inter!$A6,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
-        <v/>
+      <c r="J6" s="198" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.35">
@@ -28217,11 +27192,9 @@
         <v>5</v>
       </c>
       <c r="C7" s="50">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!L$1:L$101,MATCH([1]UHC_Inter!$A7,[1]UHC_summary!$B$1:$B$101,0))=0,INDEX([1]UHC_summary!I$1:I$101,MATCH([1]UHC_Inter!$A7,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!L$1:L$101,MATCH([1]UHC_Inter!$A7,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>86.96</v>
       </c>
       <c r="D7" s="50">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!M$1:M$101,MATCH([1]UHC_Inter!$A7,[1]UHC_summary!$B$1:$B$101,0))=0,INDEX([1]UHC_summary!J$1:J$101,MATCH([1]UHC_Inter!$A7,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!M$1:M$101,MATCH([1]UHC_Inter!$A7,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>86.96</v>
       </c>
       <c r="E7" s="50" t="e">
@@ -28241,11 +27214,9 @@
         <v>#N/A</v>
       </c>
       <c r="I7" s="50">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!D$1:D$101,MATCH([1]UHC_Inter!$A7,[1]UHC_summary!$B$1:$B$101,0))="",INDEX([1]UHC_summary!C$1:C$101,MATCH([1]UHC_Inter!$A7,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!D$1:D$101,MATCH([1]UHC_Inter!$A7,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>86.96</v>
       </c>
       <c r="J7" s="198">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!E$1:E$101,MATCH([1]UHC_Inter!$A7,[1]UHC_summary!$B$1:$B$101,0))=0,"",INDEX([1]UHC_summary!E$1:E$101,MATCH([1]UHC_Inter!$A7,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>2019</v>
       </c>
     </row>
@@ -28256,13 +27227,11 @@
       <c r="B8" s="49">
         <v>6</v>
       </c>
-      <c r="C8" s="50" t="str">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!L$1:L$101,MATCH([1]UHC_Inter!$A8,[1]UHC_summary!$B$1:$B$101,0))=0,INDEX([1]UHC_summary!I$1:I$101,MATCH([1]UHC_Inter!$A8,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!L$1:L$101,MATCH([1]UHC_Inter!$A8,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
-        <v/>
-      </c>
-      <c r="D8" s="50" t="str">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!M$1:M$101,MATCH([1]UHC_Inter!$A8,[1]UHC_summary!$B$1:$B$101,0))=0,INDEX([1]UHC_summary!J$1:J$101,MATCH([1]UHC_Inter!$A8,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!M$1:M$101,MATCH([1]UHC_Inter!$A8,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
-        <v/>
+      <c r="C8" s="50" t="s">
+        <v>82</v>
+      </c>
+      <c r="D8" s="50" t="s">
+        <v>82</v>
       </c>
       <c r="E8" s="50" t="e">
         <f t="shared" si="0"/>
@@ -28280,13 +27249,11 @@
         <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
-      <c r="I8" s="50" t="str">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!D$1:D$101,MATCH([1]UHC_Inter!$A8,[1]UHC_summary!$B$1:$B$101,0))="",INDEX([1]UHC_summary!C$1:C$101,MATCH([1]UHC_Inter!$A8,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!D$1:D$101,MATCH([1]UHC_Inter!$A8,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
-        <v/>
-      </c>
-      <c r="J8" s="198" t="str">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!E$1:E$101,MATCH([1]UHC_Inter!$A8,[1]UHC_summary!$B$1:$B$101,0))=0,"",INDEX([1]UHC_summary!E$1:E$101,MATCH([1]UHC_Inter!$A8,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
-        <v/>
+      <c r="I8" s="50" t="s">
+        <v>82</v>
+      </c>
+      <c r="J8" s="198" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
@@ -28297,11 +27264,9 @@
         <v>7</v>
       </c>
       <c r="C9" s="50">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!L$1:L$101,MATCH([1]UHC_Inter!$A9,[1]UHC_summary!$B$1:$B$101,0))=0,INDEX([1]UHC_summary!I$1:I$101,MATCH([1]UHC_Inter!$A9,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!L$1:L$101,MATCH([1]UHC_Inter!$A9,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>99.9</v>
       </c>
       <c r="D9" s="50">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!M$1:M$101,MATCH([1]UHC_Inter!$A9,[1]UHC_summary!$B$1:$B$101,0))=0,INDEX([1]UHC_summary!J$1:J$101,MATCH([1]UHC_Inter!$A9,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!M$1:M$101,MATCH([1]UHC_Inter!$A9,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>99.9</v>
       </c>
       <c r="E9" s="50" t="e">
@@ -28321,11 +27286,9 @@
         <v>#N/A</v>
       </c>
       <c r="I9" s="50">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!D$1:D$101,MATCH([1]UHC_Inter!$A9,[1]UHC_summary!$B$1:$B$101,0))="",INDEX([1]UHC_summary!C$1:C$101,MATCH([1]UHC_Inter!$A9,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!D$1:D$101,MATCH([1]UHC_Inter!$A9,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>99.89</v>
       </c>
       <c r="J9" s="198">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!E$1:E$101,MATCH([1]UHC_Inter!$A9,[1]UHC_summary!$B$1:$B$101,0))=0,"",INDEX([1]UHC_summary!E$1:E$101,MATCH([1]UHC_Inter!$A9,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>2017</v>
       </c>
     </row>
@@ -28337,11 +27300,9 @@
         <v>8</v>
       </c>
       <c r="C10" s="50">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!L$1:L$101,MATCH([1]UHC_Inter!$A10,[1]UHC_summary!$B$1:$B$101,0))=0,INDEX([1]UHC_summary!I$1:I$101,MATCH([1]UHC_Inter!$A10,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!L$1:L$101,MATCH([1]UHC_Inter!$A10,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>16.68</v>
       </c>
       <c r="D10" s="50">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!M$1:M$101,MATCH([1]UHC_Inter!$A10,[1]UHC_summary!$B$1:$B$101,0))=0,INDEX([1]UHC_summary!J$1:J$101,MATCH([1]UHC_Inter!$A10,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!M$1:M$101,MATCH([1]UHC_Inter!$A10,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>15.29</v>
       </c>
       <c r="E10" s="50" t="e">
@@ -28361,11 +27322,9 @@
         <v>1.3900000000000006</v>
       </c>
       <c r="I10" s="50">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!D$1:D$101,MATCH([1]UHC_Inter!$A10,[1]UHC_summary!$B$1:$B$101,0))="",INDEX([1]UHC_summary!C$1:C$101,MATCH([1]UHC_Inter!$A10,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!D$1:D$101,MATCH([1]UHC_Inter!$A10,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>17.55</v>
       </c>
       <c r="J10" s="198">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!E$1:E$101,MATCH([1]UHC_Inter!$A10,[1]UHC_summary!$B$1:$B$101,0))=0,"",INDEX([1]UHC_summary!E$1:E$101,MATCH([1]UHC_Inter!$A10,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>2015</v>
       </c>
     </row>
@@ -28377,11 +27336,9 @@
         <v>9</v>
       </c>
       <c r="C11" s="50">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!L$1:L$101,MATCH([1]UHC_Inter!$A11,[1]UHC_summary!$B$1:$B$101,0))=0,INDEX([1]UHC_summary!I$1:I$101,MATCH([1]UHC_Inter!$A11,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!L$1:L$101,MATCH([1]UHC_Inter!$A11,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>5.12</v>
       </c>
       <c r="D11" s="50">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!M$1:M$101,MATCH([1]UHC_Inter!$A11,[1]UHC_summary!$B$1:$B$101,0))=0,INDEX([1]UHC_summary!J$1:J$101,MATCH([1]UHC_Inter!$A11,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!M$1:M$101,MATCH([1]UHC_Inter!$A11,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>5.03</v>
       </c>
       <c r="E11" s="50" t="e">
@@ -28401,11 +27358,9 @@
         <v>8.9999999999999858E-2</v>
       </c>
       <c r="I11" s="50">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!D$1:D$101,MATCH([1]UHC_Inter!$A11,[1]UHC_summary!$B$1:$B$101,0))="",INDEX([1]UHC_summary!C$1:C$101,MATCH([1]UHC_Inter!$A11,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!D$1:D$101,MATCH([1]UHC_Inter!$A11,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>5.2</v>
       </c>
       <c r="J11" s="198">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!E$1:E$101,MATCH([1]UHC_Inter!$A11,[1]UHC_summary!$B$1:$B$101,0))=0,"",INDEX([1]UHC_summary!E$1:E$101,MATCH([1]UHC_Inter!$A11,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>2014</v>
       </c>
     </row>
@@ -28417,11 +27372,9 @@
         <v>10</v>
       </c>
       <c r="C12" s="50">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!L$1:L$101,MATCH([1]UHC_Inter!$A12,[1]UHC_summary!$B$1:$B$101,0))=0,INDEX([1]UHC_summary!I$1:I$101,MATCH([1]UHC_Inter!$A12,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!L$1:L$101,MATCH([1]UHC_Inter!$A12,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>21.9</v>
       </c>
       <c r="D12" s="50">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!M$1:M$101,MATCH([1]UHC_Inter!$A12,[1]UHC_summary!$B$1:$B$101,0))=0,INDEX([1]UHC_summary!J$1:J$101,MATCH([1]UHC_Inter!$A12,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!M$1:M$101,MATCH([1]UHC_Inter!$A12,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>19.5</v>
       </c>
       <c r="E12" s="50" t="e">
@@ -28441,11 +27394,9 @@
         <v>2.3999999999999986</v>
       </c>
       <c r="I12" s="50">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!D$1:D$101,MATCH([1]UHC_Inter!$A12,[1]UHC_summary!$B$1:$B$101,0))="",INDEX([1]UHC_summary!C$1:C$101,MATCH([1]UHC_Inter!$A12,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!D$1:D$101,MATCH([1]UHC_Inter!$A12,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>21.9</v>
       </c>
       <c r="J12" s="198">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!E$1:E$101,MATCH([1]UHC_Inter!$A12,[1]UHC_summary!$B$1:$B$101,0))=0,"",INDEX([1]UHC_summary!E$1:E$101,MATCH([1]UHC_Inter!$A12,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>2018</v>
       </c>
     </row>
@@ -28457,11 +27408,9 @@
         <v>11</v>
       </c>
       <c r="C13" s="50">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!L$1:L$101,MATCH([1]UHC_Inter!$A13,[1]UHC_summary!$B$1:$B$101,0))=0,INDEX([1]UHC_summary!I$1:I$101,MATCH([1]UHC_Inter!$A13,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!L$1:L$101,MATCH([1]UHC_Inter!$A13,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>129.04</v>
       </c>
       <c r="D13" s="50">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!M$1:M$101,MATCH([1]UHC_Inter!$A13,[1]UHC_summary!$B$1:$B$101,0))=0,INDEX([1]UHC_summary!J$1:J$101,MATCH([1]UHC_Inter!$A13,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!M$1:M$101,MATCH([1]UHC_Inter!$A13,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>130.5</v>
       </c>
       <c r="E13" s="50">
@@ -28481,11 +27430,9 @@
         <v>#N/A</v>
       </c>
       <c r="I13" s="50">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!D$1:D$101,MATCH([1]UHC_Inter!$A13,[1]UHC_summary!$B$1:$B$101,0))="",INDEX([1]UHC_summary!C$1:C$101,MATCH([1]UHC_Inter!$A13,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!D$1:D$101,MATCH([1]UHC_Inter!$A13,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>129.04</v>
       </c>
       <c r="J13" s="198">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!E$1:E$101,MATCH([1]UHC_Inter!$A13,[1]UHC_summary!$B$1:$B$101,0))=0,"",INDEX([1]UHC_summary!E$1:E$101,MATCH([1]UHC_Inter!$A13,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>2018</v>
       </c>
     </row>
@@ -28497,11 +27444,9 @@
         <v>12</v>
       </c>
       <c r="C14" s="50">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!L$1:L$101,MATCH([1]UHC_Inter!$A14,[1]UHC_summary!$B$1:$B$101,0))=0,INDEX([1]UHC_summary!I$1:I$101,MATCH([1]UHC_Inter!$A14,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!L$1:L$101,MATCH([1]UHC_Inter!$A14,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>151.77000000000001</v>
       </c>
       <c r="D14" s="50">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!M$1:M$101,MATCH([1]UHC_Inter!$A14,[1]UHC_summary!$B$1:$B$101,0))=0,INDEX([1]UHC_summary!J$1:J$101,MATCH([1]UHC_Inter!$A14,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!M$1:M$101,MATCH([1]UHC_Inter!$A14,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>172.69</v>
       </c>
       <c r="E14" s="50">
@@ -28521,11 +27466,9 @@
         <v>#N/A</v>
       </c>
       <c r="I14" s="50">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!D$1:D$101,MATCH([1]UHC_Inter!$A14,[1]UHC_summary!$B$1:$B$101,0))="",INDEX([1]UHC_summary!C$1:C$101,MATCH([1]UHC_Inter!$A14,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!D$1:D$101,MATCH([1]UHC_Inter!$A14,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>151.77000000000001</v>
       </c>
       <c r="J14" s="198">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!E$1:E$101,MATCH([1]UHC_Inter!$A14,[1]UHC_summary!$B$1:$B$101,0))=0,"",INDEX([1]UHC_summary!E$1:E$101,MATCH([1]UHC_Inter!$A14,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>2018</v>
       </c>
     </row>
@@ -28537,11 +27480,9 @@
         <v>13</v>
       </c>
       <c r="C15" s="50">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!L$1:L$101,MATCH([1]UHC_Inter!$A15,[1]UHC_summary!$B$1:$B$101,0))=0,INDEX([1]UHC_summary!I$1:I$101,MATCH([1]UHC_Inter!$A15,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!L$1:L$101,MATCH([1]UHC_Inter!$A15,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>95</v>
       </c>
       <c r="D15" s="50">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!M$1:M$101,MATCH([1]UHC_Inter!$A15,[1]UHC_summary!$B$1:$B$101,0))=0,INDEX([1]UHC_summary!J$1:J$101,MATCH([1]UHC_Inter!$A15,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!M$1:M$101,MATCH([1]UHC_Inter!$A15,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>94.99</v>
       </c>
       <c r="E15" s="50" t="e">
@@ -28561,11 +27502,9 @@
         <v>1.0000000000005116E-2</v>
       </c>
       <c r="I15" s="50">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!D$1:D$101,MATCH([1]UHC_Inter!$A15,[1]UHC_summary!$B$1:$B$101,0))="",INDEX([1]UHC_summary!C$1:C$101,MATCH([1]UHC_Inter!$A15,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!D$1:D$101,MATCH([1]UHC_Inter!$A15,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>95</v>
       </c>
       <c r="J15" s="198">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!E$1:E$101,MATCH([1]UHC_Inter!$A15,[1]UHC_summary!$B$1:$B$101,0))=0,"",INDEX([1]UHC_summary!E$1:E$101,MATCH([1]UHC_Inter!$A15,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
         <v>2020</v>
       </c>
     </row>
@@ -28574,13 +27513,11 @@
       <c r="B16" s="49">
         <v>14</v>
       </c>
-      <c r="C16" s="50" t="str">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!L$1:L$101,MATCH([1]UHC_Inter!$A16,[1]UHC_summary!$B$1:$B$101,0))=0,INDEX([1]UHC_summary!I$1:I$101,MATCH([1]UHC_Inter!$A16,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!L$1:L$101,MATCH([1]UHC_Inter!$A16,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
-        <v/>
-      </c>
-      <c r="D16" s="50" t="str">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!M$1:M$101,MATCH([1]UHC_Inter!$A16,[1]UHC_summary!$B$1:$B$101,0))=0,INDEX([1]UHC_summary!J$1:J$101,MATCH([1]UHC_Inter!$A16,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!M$1:M$101,MATCH([1]UHC_Inter!$A16,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
-        <v/>
+      <c r="C16" s="50" t="s">
+        <v>82</v>
+      </c>
+      <c r="D16" s="50" t="s">
+        <v>82</v>
       </c>
       <c r="E16" s="50" t="e">
         <f t="shared" si="0"/>
@@ -28598,13 +27535,11 @@
         <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
-      <c r="I16" s="50" t="str">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!D$1:D$101,MATCH([1]UHC_Inter!$A16,[1]UHC_summary!$B$1:$B$101,0))="",INDEX([1]UHC_summary!C$1:C$101,MATCH([1]UHC_Inter!$A16,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!D$1:D$101,MATCH([1]UHC_Inter!$A16,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
-        <v/>
-      </c>
-      <c r="J16" s="198" t="str">
-        <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!E$1:E$101,MATCH([1]UHC_Inter!$A16,[1]UHC_summary!$B$1:$B$101,0))=0,"",INDEX([1]UHC_summary!E$1:E$101,MATCH([1]UHC_Inter!$A16,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
-        <v/>
+      <c r="I16" s="50" t="s">
+        <v>82</v>
+      </c>
+      <c r="J16" s="198" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.35">
@@ -28879,11 +27814,11 @@
         <f>F47/1000</f>
         <v>0</v>
       </c>
-      <c r="H5" s="347" t="s">
+      <c r="H5" s="343" t="s">
         <v>152</v>
       </c>
-      <c r="I5" s="348"/>
-      <c r="J5" s="348"/>
+      <c r="I5" s="344"/>
+      <c r="J5" s="344"/>
       <c r="K5" s="13"/>
       <c r="L5" s="13"/>
       <c r="M5" s="13"/>
@@ -28919,11 +27854,11 @@
         <f>F48</f>
         <v>0</v>
       </c>
-      <c r="H6" s="347" t="s">
+      <c r="H6" s="343" t="s">
         <v>46</v>
       </c>
-      <c r="I6" s="348"/>
-      <c r="J6" s="348"/>
+      <c r="I6" s="344"/>
+      <c r="J6" s="344"/>
       <c r="K6" s="13"/>
       <c r="L6" s="13"/>
       <c r="M6" s="13"/>
@@ -28959,11 +27894,11 @@
         <f>F49/1000</f>
         <v>0</v>
       </c>
-      <c r="H7" s="347" t="s">
+      <c r="H7" s="343" t="s">
         <v>152</v>
       </c>
-      <c r="I7" s="348"/>
-      <c r="J7" s="348"/>
+      <c r="I7" s="344"/>
+      <c r="J7" s="344"/>
       <c r="K7" s="66"/>
       <c r="L7" s="66"/>
       <c r="M7" s="66"/>
@@ -29020,31 +27955,31 @@
       <c r="AE8" s="13"/>
     </row>
     <row r="9" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="350" t="s">
+      <c r="A9" s="346" t="s">
         <v>77</v>
       </c>
-      <c r="B9" s="350"/>
-      <c r="C9" s="346" t="s">
+      <c r="B9" s="346"/>
+      <c r="C9" s="348" t="s">
         <v>80</v>
       </c>
-      <c r="D9" s="346"/>
-      <c r="E9" s="346"/>
-      <c r="F9" s="346"/>
-      <c r="G9" s="346"/>
+      <c r="D9" s="348"/>
+      <c r="E9" s="348"/>
+      <c r="F9" s="348"/>
+      <c r="G9" s="348"/>
       <c r="H9" s="156"/>
-      <c r="I9" s="349" t="s">
+      <c r="I9" s="345" t="s">
         <v>153</v>
       </c>
-      <c r="J9" s="349"/>
-      <c r="K9" s="349"/>
-      <c r="L9" s="349"/>
-      <c r="M9" s="349"/>
-      <c r="N9" s="349"/>
-      <c r="O9" s="349"/>
-      <c r="P9" s="349"/>
-      <c r="Q9" s="349"/>
-      <c r="R9" s="349"/>
-      <c r="S9" s="349"/>
+      <c r="J9" s="345"/>
+      <c r="K9" s="345"/>
+      <c r="L9" s="345"/>
+      <c r="M9" s="345"/>
+      <c r="N9" s="345"/>
+      <c r="O9" s="345"/>
+      <c r="P9" s="345"/>
+      <c r="Q9" s="345"/>
+      <c r="R9" s="345"/>
+      <c r="S9" s="345"/>
       <c r="T9" s="115"/>
       <c r="U9" s="115"/>
       <c r="V9" s="115"/>
@@ -29059,47 +27994,47 @@
       <c r="AE9" s="13"/>
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A10" s="344" t="s">
+      <c r="A10" s="347" t="s">
         <v>121</v>
       </c>
-      <c r="B10" s="344" t="s">
+      <c r="B10" s="347" t="s">
         <v>270</v>
       </c>
-      <c r="C10" s="345" t="s">
+      <c r="C10" s="350" t="s">
         <v>268</v>
       </c>
-      <c r="D10" s="344" t="s">
+      <c r="D10" s="347" t="s">
         <v>269</v>
       </c>
-      <c r="E10" s="345" t="s">
+      <c r="E10" s="350" t="s">
         <v>87</v>
       </c>
-      <c r="F10" s="345" t="s">
+      <c r="F10" s="350" t="s">
         <v>84</v>
       </c>
-      <c r="G10" s="344" t="s">
+      <c r="G10" s="347" t="s">
         <v>154</v>
       </c>
       <c r="H10" s="127"/>
-      <c r="I10" s="343" t="s">
+      <c r="I10" s="349" t="s">
         <v>268</v>
       </c>
-      <c r="J10" s="343"/>
+      <c r="J10" s="349"/>
       <c r="K10" s="132"/>
-      <c r="L10" s="343" t="s">
+      <c r="L10" s="349" t="s">
         <v>269</v>
       </c>
-      <c r="M10" s="343"/>
+      <c r="M10" s="349"/>
       <c r="N10" s="132"/>
-      <c r="O10" s="343" t="s">
+      <c r="O10" s="349" t="s">
         <v>84</v>
       </c>
-      <c r="P10" s="343"/>
+      <c r="P10" s="349"/>
       <c r="Q10" s="132"/>
-      <c r="R10" s="343" t="s">
+      <c r="R10" s="349" t="s">
         <v>85</v>
       </c>
-      <c r="S10" s="343"/>
+      <c r="S10" s="349"/>
       <c r="Y10" s="13"/>
       <c r="Z10" s="13"/>
       <c r="AA10" s="13"/>
@@ -29109,13 +28044,13 @@
       <c r="AE10" s="13"/>
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A11" s="344"/>
-      <c r="B11" s="344"/>
-      <c r="C11" s="345"/>
-      <c r="D11" s="344"/>
-      <c r="E11" s="345"/>
-      <c r="F11" s="345"/>
-      <c r="G11" s="344"/>
+      <c r="A11" s="347"/>
+      <c r="B11" s="347"/>
+      <c r="C11" s="350"/>
+      <c r="D11" s="347"/>
+      <c r="E11" s="350"/>
+      <c r="F11" s="350"/>
+      <c r="G11" s="347"/>
       <c r="H11" s="127"/>
       <c r="I11" s="131">
         <v>2018</v>
@@ -31272,16 +30207,6 @@
     <row r="83" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="H7:J7"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="I9:S9"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="O10:P10"/>
     <mergeCell ref="R10:S10"/>
     <mergeCell ref="G10:G11"/>
     <mergeCell ref="B10:B11"/>
@@ -31289,6 +30214,16 @@
     <mergeCell ref="D10:D11"/>
     <mergeCell ref="E10:E11"/>
     <mergeCell ref="F10:F11"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="I9:S9"/>
+    <mergeCell ref="A9:B9"/>
   </mergeCells>
   <conditionalFormatting sqref="D13:D25 L13:M25">
     <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
@@ -31331,21 +30266,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FB6FBD5E95BAB542B810C32545CA4E3B" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c88f4da8c98e9c6f14dc759bd92b3b9d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="f244dd4c-ee25-4b14-a7cd-a89d47e877b9" xmlns:ns4="7d5efbb1-7b5c-4600-961f-d0c91f173691" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e11dd0c1a7b4f1799f1daf73497fb7c0" ns3:_="" ns4:_="">
     <xsd:import namespace="f244dd4c-ee25-4b14-a7cd-a89d47e877b9"/>
@@ -31556,32 +30476,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B8C5798F-31D9-455C-A266-3CF2A88C6872}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="7d5efbb1-7b5c-4600-961f-d0c91f173691"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="f244dd4c-ee25-4b14-a7cd-a89d47e877b9"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5668EAE9-BE2F-449B-83FE-5638B2ED2DF4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B491DB35-4E91-4B2D-816E-03001B21F1D3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -31598,4 +30508,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5668EAE9-BE2F-449B-83FE-5638B2ED2DF4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B8C5798F-31D9-455C-A266-3CF2A88C6872}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="7d5efbb1-7b5c-4600-961f-d0c91f173691"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="f244dd4c-ee25-4b14-a7cd-a89d47e877b9"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>